<commit_message>
Updates for gas cooler model
</commit_message>
<xml_diff>
--- a/ComponentTests/supercritical/Table.xlsx
+++ b/ComponentTests/supercritical/Table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28315"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="1080" windowWidth="30120" windowHeight="19640" tabRatio="500"/>
+    <workbookView xWindow="1960" yWindow="440" windowWidth="30120" windowHeight="20560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="173">
   <si>
     <t>Test Conditions</t>
   </si>
@@ -83,13 +83,469 @@
     <t>Q_siml</t>
   </si>
   <si>
-    <t>Ref out temp (new)</t>
-  </si>
-  <si>
-    <t>Q (new)</t>
-  </si>
-  <si>
     <t>Q_exp</t>
+  </si>
+  <si>
+    <t>Q_new_FV</t>
+  </si>
+  <si>
+    <t>T_r_FV</t>
+  </si>
+  <si>
+    <t>10 seg</t>
+  </si>
+  <si>
+    <t>7.55330519695 39.4513890453</t>
+  </si>
+  <si>
+    <t>8.58867006795 35.0041888069</t>
+  </si>
+  <si>
+    <t>9.26059570094 32.5749759237</t>
+  </si>
+  <si>
+    <t>8.58820867009 39.8149298066</t>
+  </si>
+  <si>
+    <t>9.42837269968 32.9991854139</t>
+  </si>
+  <si>
+    <t>9.6278748701 31.1513471125</t>
+  </si>
+  <si>
+    <t>9.23317173388 38.269444473</t>
+  </si>
+  <si>
+    <t>9.77892664801 31.8789380628</t>
+  </si>
+  <si>
+    <t>9.90968153542 30.5645407111</t>
+  </si>
+  <si>
+    <t>6.60448420642 41.8385627577</t>
+  </si>
+  <si>
+    <t>7.51006585342 39.6771323781</t>
+  </si>
+  <si>
+    <t>7.98489928789 38.5923948553</t>
+  </si>
+  <si>
+    <t>7.73051394642 43.8664616353</t>
+  </si>
+  <si>
+    <t>8.61078768324 39.3677891844</t>
+  </si>
+  <si>
+    <t>8.94810502382 37.4926415656</t>
+  </si>
+  <si>
+    <t>8.55368332317 43.8266757061</t>
+  </si>
+  <si>
+    <t>9.25707203453 38.1417852491</t>
+  </si>
+  <si>
+    <t>9.44483552636 36.605576936</t>
+  </si>
+  <si>
+    <t>9.28564239471 43.2114571241</t>
+  </si>
+  <si>
+    <t>11.5057620809 39.9011752294</t>
+  </si>
+  <si>
+    <t>12.7163403219 38.1971710942</t>
+  </si>
+  <si>
+    <t>10.9315129215 46.7821908229</t>
+  </si>
+  <si>
+    <t>13.3009930245 41.1405558993</t>
+  </si>
+  <si>
+    <t>14.4313644177 37.2340240737</t>
+  </si>
+  <si>
+    <t>12.3155898273 49.0916991431</t>
+  </si>
+  <si>
+    <t>14.6700101146 40.2857106535</t>
+  </si>
+  <si>
+    <t>15.5491515253 35.6812260181</t>
+  </si>
+  <si>
+    <t>7.90700989062 45.5814237842</t>
+  </si>
+  <si>
+    <t>9.46693188 42.0948213195</t>
+  </si>
+  <si>
+    <t>10.3150664294 40.8381703404</t>
+  </si>
+  <si>
+    <t>9.76125019301 49.1849315458</t>
+  </si>
+  <si>
+    <t>11.7153222225 44.6196496908</t>
+  </si>
+  <si>
+    <t>12.59690798 42.2827024896</t>
+  </si>
+  <si>
+    <t>10.9756476888 51.7276890947</t>
+  </si>
+  <si>
+    <t>13.0733374289 45.1127022152</t>
+  </si>
+  <si>
+    <t>13.9636307615 41.5704080551</t>
+  </si>
+  <si>
+    <t>ACM_FV1</t>
+  </si>
+  <si>
+    <t>ACM_FV2</t>
+  </si>
+  <si>
+    <t>7.55635651214 39.4611530923</t>
+  </si>
+  <si>
+    <t>8.59153325979 35.0000257344</t>
+  </si>
+  <si>
+    <t>9.2627015986 32.5699000303</t>
+  </si>
+  <si>
+    <t>8.5900926733 39.8149071486</t>
+  </si>
+  <si>
+    <t>9.42948267852 32.9961728137</t>
+  </si>
+  <si>
+    <t>9.62866191374 31.1496453304</t>
+  </si>
+  <si>
+    <t>9.23426244031 38.2670959326</t>
+  </si>
+  <si>
+    <t>9.77949931701 31.8774992336</t>
+  </si>
+  <si>
+    <t>9.91012780718 30.5638031587</t>
+  </si>
+  <si>
+    <t>6.6074393127 41.8499644259</t>
+  </si>
+  <si>
+    <t>7.51458809235 39.6844915186</t>
+  </si>
+  <si>
+    <t>7.98982092031 38.5952912562</t>
+  </si>
+  <si>
+    <t>7.73272013031 43.8717356144</t>
+  </si>
+  <si>
+    <t>8.61289079423 39.3659372857</t>
+  </si>
+  <si>
+    <t>8.9497934137 37.4903023976</t>
+  </si>
+  <si>
+    <t>8.55510812687 43.8268412836</t>
+  </si>
+  <si>
+    <t>9.25807056342 38.1399991727</t>
+  </si>
+  <si>
+    <t>9.44562788438 36.60440774</t>
+  </si>
+  <si>
+    <t>9.29438792668 43.2552390953</t>
+  </si>
+  <si>
+    <t>11.5221894912 39.9390733099</t>
+  </si>
+  <si>
+    <t>12.7357049771 38.2174798319</t>
+  </si>
+  <si>
+    <t>10.9389811996 46.8163660391</t>
+  </si>
+  <si>
+    <t>13.3116295339 41.1502023659</t>
+  </si>
+  <si>
+    <t>14.4408004019 37.2289837481</t>
+  </si>
+  <si>
+    <t>12.3216048282 49.1137242115</t>
+  </si>
+  <si>
+    <t>14.6765753043 40.2838859595</t>
+  </si>
+  <si>
+    <t>15.5541904451 35.6757145024</t>
+  </si>
+  <si>
+    <t>7.91423416354 45.6176599869</t>
+  </si>
+  <si>
+    <t>9.48133092104 42.1309519</t>
+  </si>
+  <si>
+    <t>10.3345980618 40.8718934992</t>
+  </si>
+  <si>
+    <t>9.76818360727 49.2178676009</t>
+  </si>
+  <si>
+    <t>11.727182173 44.6422802651</t>
+  </si>
+  <si>
+    <t>12.6099956951 42.292765709</t>
+  </si>
+  <si>
+    <t>10.9813850458 51.7518735698</t>
+  </si>
+  <si>
+    <t>13.0812110844 45.1193046127</t>
+  </si>
+  <si>
+    <t>13.9709129605 41.5688063413</t>
+  </si>
+  <si>
+    <t>7.78747815569 38.9578331072</t>
+  </si>
+  <si>
+    <t>8.83681317127 33.7896155659</t>
+  </si>
+  <si>
+    <t>9.44850852389 31.4303941672</t>
+  </si>
+  <si>
+    <t>8.82381933824 38.6579820726</t>
+  </si>
+  <si>
+    <t>9.58861513486 31.8143091955</t>
+  </si>
+  <si>
+    <t>9.72751394489 30.3691196449</t>
+  </si>
+  <si>
+    <t>9.44498940783 36.7569990006</t>
+  </si>
+  <si>
+    <t>9.88981644109 30.9255266183</t>
+  </si>
+  <si>
+    <t>9.97500115397 29.988362888</t>
+  </si>
+  <si>
+    <t>6.79297899493 41.3799071479</t>
+  </si>
+  <si>
+    <t>7.75729016267 39.1688135839</t>
+  </si>
+  <si>
+    <t>8.24372919401 37.9350829674</t>
+  </si>
+  <si>
+    <t>7.94680947703 43.1373361517</t>
+  </si>
+  <si>
+    <t>8.81706593834 38.3213671162</t>
+  </si>
+  <si>
+    <t>9.10266464767 36.5961961029</t>
+  </si>
+  <si>
+    <t>8.76640074196 42.6631164502</t>
+  </si>
+  <si>
+    <t>9.40205335604 37.1111043238</t>
+  </si>
+  <si>
+    <t>9.53949787669 35.8979582595</t>
+  </si>
+  <si>
+    <t>9.54671490111 42.7727034639</t>
+  </si>
+  <si>
+    <t>11.9077081452 39.5167577279</t>
+  </si>
+  <si>
+    <t>13.190602817 37.5898778037</t>
+  </si>
+  <si>
+    <t>11.2292491728 46.283794939</t>
+  </si>
+  <si>
+    <t>13.7143825605 40.2741241615</t>
+  </si>
+  <si>
+    <t>14.8434128288 36.022541774</t>
+  </si>
+  <si>
+    <t>12.6387370599 48.4049451247</t>
+  </si>
+  <si>
+    <t>15.0668554362 39.0027347549</t>
+  </si>
+  <si>
+    <t>15.8922514656 34.3526064138</t>
+  </si>
+  <si>
+    <t>8.12009665869 45.0714056395</t>
+  </si>
+  <si>
+    <t>ACM_FV3</t>
+  </si>
+  <si>
+    <t>9.77725347912 41.6821574544</t>
+  </si>
+  <si>
+    <t>10.6896465564 40.4544710172</t>
+  </si>
+  <si>
+    <t>10.0252572149 48.6372492007</t>
+  </si>
+  <si>
+    <t>12.0901517295 44.0290892248</t>
+  </si>
+  <si>
+    <t>13.0067978161 41.5187420892</t>
+  </si>
+  <si>
+    <t>11.2635608203 51.0986254063</t>
+  </si>
+  <si>
+    <t>13.450224049 44.1713748701</t>
+  </si>
+  <si>
+    <t>14.3277066059 40.4687393039</t>
+  </si>
+  <si>
+    <t>7.79067825519 38.9659763116</t>
+  </si>
+  <si>
+    <t>8.83951329857 33.783333015</t>
+  </si>
+  <si>
+    <t>9.4502730958 31.4257402629</t>
+  </si>
+  <si>
+    <t>no accel</t>
+  </si>
+  <si>
+    <t>8.82573586139 38.6560806762</t>
+  </si>
+  <si>
+    <t>ACM_FV4</t>
+  </si>
+  <si>
+    <t>accel</t>
+  </si>
+  <si>
+    <t>40 seg</t>
+  </si>
+  <si>
+    <t>9.58959466043 31.8115166982</t>
+  </si>
+  <si>
+    <t>9.72820175176 30.3678296238</t>
+  </si>
+  <si>
+    <t>9.44605644161 36.7539007174</t>
+  </si>
+  <si>
+    <t>9.8903277739 30.9243293108</t>
+  </si>
+  <si>
+    <t>9.97540420094 29.9878582329</t>
+  </si>
+  <si>
+    <t>6.79615789367 41.3912128077</t>
+  </si>
+  <si>
+    <t>7.76205584118 39.1743423493</t>
+  </si>
+  <si>
+    <t>8.24864478538 37.9349418972</t>
+  </si>
+  <si>
+    <t>7.94911052613 43.141277277</t>
+  </si>
+  <si>
+    <t>8.81906568822 38.318458812</t>
+  </si>
+  <si>
+    <t>9.10417439162 36.5938433965</t>
+  </si>
+  <si>
+    <t>8.76784372562 42.6621346599</t>
+  </si>
+  <si>
+    <t>9.40296591638 37.1093341759</t>
+  </si>
+  <si>
+    <t>9.54021361577 35.8970256924</t>
+  </si>
+  <si>
+    <t>9.55596360417 42.817243198</t>
+  </si>
+  <si>
+    <t>11.9251250026 39.5522133699</t>
+  </si>
+  <si>
+    <t>13.2106790713 37.6022884066</t>
+  </si>
+  <si>
+    <t>11.2370976351 46.3172659632</t>
+  </si>
+  <si>
+    <t>13.7254084326 40.2788775535</t>
+  </si>
+  <si>
+    <t>14.8527512786 36.0136327979</t>
+  </si>
+  <si>
+    <t>12.6450345547 48.4253008836</t>
+  </si>
+  <si>
+    <t>15.0735162746 38.9978556111</t>
+  </si>
+  <si>
+    <t>15.897095665 34.3460170067</t>
+  </si>
+  <si>
+    <t>8.12783631188 45.1083609204</t>
+  </si>
+  <si>
+    <t>9.79284624391 41.7185658128</t>
+  </si>
+  <si>
+    <t>10.7107742966 40.4870380761</t>
+  </si>
+  <si>
+    <t>10.0325920831 48.6702937492</t>
+  </si>
+  <si>
+    <t>12.1026786384 44.0491271619</t>
+  </si>
+  <si>
+    <t>13.0203086341 41.5241222157</t>
+  </si>
+  <si>
+    <t>11.2695906641 51.1219968414</t>
+  </si>
+  <si>
+    <t>13.4583702648 44.1748251417</t>
+  </si>
+  <si>
+    <t>14.3349546861 40.464673009</t>
   </si>
 </sst>
 </file>
@@ -131,6 +587,7 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -222,7 +679,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -258,8 +715,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -270,16 +755,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -297,6 +790,20 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -314,6 +821,20 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -648,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:AH76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I38"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,9 +1184,12 @@
     <col min="6" max="6" width="19.33203125" customWidth="1"/>
     <col min="7" max="7" width="28.5" customWidth="1"/>
     <col min="8" max="8" width="32.83203125" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -691,25 +1215,26 @@
         <v>11</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="T1" s="8"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -735,25 +1260,64 @@
         <v>2</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="M2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="P2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -778,26 +1342,38 @@
       <c r="H3" s="1">
         <v>38</v>
       </c>
-      <c r="I3" s="9">
-        <v>7.9192091124299999</v>
-      </c>
-      <c r="J3" s="9">
-        <v>38.7446464326</v>
+      <c r="I3" s="7">
+        <v>8</v>
+      </c>
+      <c r="J3" s="7">
+        <v>7.1413843960000003</v>
       </c>
       <c r="K3" s="8">
-        <v>8</v>
+        <v>8.3480151618700003</v>
       </c>
       <c r="L3" s="8">
-        <v>34.06534121</v>
-      </c>
-      <c r="M3" s="8">
-        <v>9.2273926429999999</v>
-      </c>
-      <c r="N3" s="8">
-        <v>7.1413843960000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+        <v>37.598140358199998</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="P3" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB3" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="AD3" s="8"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="12"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <f>A3+1</f>
         <v>2</v>
@@ -823,26 +1399,34 @@
       <c r="H4" s="3">
         <v>33.5</v>
       </c>
-      <c r="I4" s="9">
-        <v>8.7658026757999998</v>
-      </c>
-      <c r="J4" s="9">
-        <v>34.194287103400001</v>
+      <c r="I4" s="7">
+        <v>9</v>
+      </c>
+      <c r="J4" s="7">
+        <v>8.8980085080000002</v>
       </c>
       <c r="K4" s="8">
-        <v>9</v>
+        <v>9.0046645190600003</v>
       </c>
       <c r="L4" s="8">
-        <v>30.022436989999999</v>
-      </c>
-      <c r="M4" s="8">
-        <v>9.4557607860000008</v>
-      </c>
-      <c r="N4" s="8">
-        <v>8.8980085080000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+        <v>32.904882553500002</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="P4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB4" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF4" s="7"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A38" si="0">A4+1</f>
         <v>3</v>
@@ -868,26 +1452,34 @@
       <c r="H5" s="1">
         <v>31.5</v>
       </c>
-      <c r="I5" s="9">
-        <v>9.2561465402599996</v>
-      </c>
-      <c r="J5" s="9">
-        <v>32.634348317600001</v>
+      <c r="I5" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="J5" s="7">
+        <v>9.4732699789999995</v>
       </c>
       <c r="K5" s="8">
-        <v>9.5</v>
+        <v>9.4461843300799995</v>
       </c>
       <c r="L5" s="8">
-        <v>29.536602160000001</v>
-      </c>
-      <c r="M5" s="8">
-        <v>9.7305265030000001</v>
-      </c>
-      <c r="N5" s="8">
-        <v>9.4732699789999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+        <v>31.4733065936</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="P5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="X5" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB5" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="AF5" s="7"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -913,26 +1505,34 @@
       <c r="H6" s="4">
         <v>36.9</v>
       </c>
-      <c r="I6" s="9">
-        <v>8.6262401476699999</v>
-      </c>
-      <c r="J6" s="9">
-        <v>39.684482002700001</v>
+      <c r="I6" s="7">
+        <v>9.25</v>
+      </c>
+      <c r="J6" s="7">
+        <v>8.2142050090000005</v>
       </c>
       <c r="K6" s="8">
-        <v>9.25</v>
+        <v>8.9216813518000002</v>
       </c>
       <c r="L6" s="8">
-        <v>33.966128640000001</v>
-      </c>
-      <c r="M6" s="8">
-        <v>9.6059367649999992</v>
-      </c>
-      <c r="N6" s="8">
-        <v>8.2142050090000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+        <v>38.183843151200001</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="P6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB6" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="AF6" s="7"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -958,26 +1558,34 @@
       <c r="H7" s="1">
         <v>31.2</v>
       </c>
-      <c r="I7" s="9">
-        <v>9.24516348555</v>
-      </c>
-      <c r="J7" s="9">
-        <v>34.312111672500002</v>
+      <c r="I7" s="7">
+        <v>9.75</v>
+      </c>
+      <c r="J7" s="7">
+        <v>9.5267881840000008</v>
       </c>
       <c r="K7" s="8">
-        <v>9.75</v>
+        <v>9.4468013662200008</v>
       </c>
       <c r="L7" s="8">
-        <v>29.878186700000001</v>
-      </c>
-      <c r="M7" s="8">
-        <v>9.8360378239999999</v>
-      </c>
-      <c r="N7" s="8">
-        <v>9.5267881840000008</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+        <v>32.889245552399998</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="P7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="X7" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB7" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="AF7" s="7"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1003,26 +1611,34 @@
       <c r="H8" s="4">
         <v>30.3</v>
       </c>
-      <c r="I8" s="9">
-        <v>9.4244434269900008</v>
-      </c>
-      <c r="J8" s="9">
-        <v>32.707419180300001</v>
+      <c r="I8" s="7">
+        <v>9.9</v>
+      </c>
+      <c r="J8" s="7">
+        <v>9.6370043079999999</v>
       </c>
       <c r="K8" s="8">
-        <v>9.9</v>
+        <v>9.5920280747500009</v>
       </c>
       <c r="L8" s="8">
-        <v>29.49021123</v>
-      </c>
-      <c r="M8" s="8">
-        <v>9.8368274539999998</v>
-      </c>
-      <c r="N8" s="8">
-        <v>9.6370043079999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+        <v>31.448114325999999</v>
+      </c>
+      <c r="M8" s="8"/>
+      <c r="P8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="X8" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB8" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF8" s="7"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1048,26 +1664,34 @@
       <c r="H9" s="1">
         <v>34.299999999999997</v>
       </c>
-      <c r="I9" s="9">
-        <v>8.9776195048599998</v>
-      </c>
-      <c r="J9" s="9">
-        <v>40.010687577399999</v>
+      <c r="I9" s="7">
+        <v>9.9</v>
+      </c>
+      <c r="J9" s="7">
+        <v>8.9167739380000004</v>
       </c>
       <c r="K9" s="8">
-        <v>9.9</v>
+        <v>9.2330228139399999</v>
       </c>
       <c r="L9" s="8">
-        <v>33.768299710000001</v>
-      </c>
-      <c r="M9" s="8">
-        <v>9.8343836939999996</v>
-      </c>
-      <c r="N9" s="8">
-        <v>8.9167739380000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+        <v>38.298985446800003</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="P9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="X9" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB9" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF9" s="7"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1093,26 +1717,34 @@
       <c r="H10" s="4">
         <v>30.4</v>
       </c>
-      <c r="I10" s="9">
-        <v>9.4888731965099993</v>
-      </c>
-      <c r="J10" s="9">
-        <v>34.288693768900004</v>
+      <c r="I10" s="7">
+        <v>10</v>
+      </c>
+      <c r="J10" s="7">
+        <v>9.8017882400000005</v>
       </c>
       <c r="K10" s="8">
-        <v>10</v>
+        <v>9.6931736170900002</v>
       </c>
       <c r="L10" s="8">
-        <v>29.788514450000001</v>
-      </c>
-      <c r="M10" s="8">
-        <v>10.0191246</v>
-      </c>
-      <c r="N10" s="8">
-        <v>9.8017882400000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+        <v>32.618685882900003</v>
+      </c>
+      <c r="M10" s="8"/>
+      <c r="P10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="T10" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="X10" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB10" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF10" s="7"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <f>A10+1</f>
         <v>9</v>
@@ -1138,26 +1770,34 @@
       <c r="H11" s="1">
         <v>29.9</v>
       </c>
-      <c r="I11" s="9">
-        <v>9.6692811424799991</v>
-      </c>
-      <c r="J11" s="9">
-        <v>32.639071408299998</v>
+      <c r="I11" s="7">
+        <v>10</v>
+      </c>
+      <c r="J11" s="7">
+        <v>9.8729621600000002</v>
       </c>
       <c r="K11" s="8">
-        <v>10</v>
+        <v>9.8386747769599996</v>
       </c>
       <c r="L11" s="8">
-        <v>29.463365209999999</v>
-      </c>
-      <c r="M11" s="8">
-        <v>10.03420859</v>
-      </c>
-      <c r="N11" s="8">
-        <v>9.8729621600000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+        <v>31.197889342300002</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="P11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="X11" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB11" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="AF11" s="7"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1183,26 +1823,34 @@
       <c r="H12" s="4">
         <v>40.6</v>
       </c>
-      <c r="I12" s="9">
-        <v>6.6126740253999996</v>
-      </c>
-      <c r="J12" s="9">
-        <v>41.953696299699999</v>
+      <c r="I12" s="7">
+        <v>7</v>
+      </c>
+      <c r="J12" s="7">
+        <v>6.2168311879999996</v>
       </c>
       <c r="K12" s="8">
-        <v>7</v>
+        <v>7.0496039637000001</v>
       </c>
       <c r="L12" s="8">
-        <v>38.457074400000003</v>
-      </c>
-      <c r="M12" s="8">
-        <v>8.1959767810000006</v>
-      </c>
-      <c r="N12" s="8">
-        <v>6.2168311879999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>40.9285437407</v>
+      </c>
+      <c r="M12" s="8"/>
+      <c r="P12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="X12" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB12" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="AF12" s="7"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1228,26 +1876,34 @@
       <c r="H13" s="1">
         <v>38.799999999999997</v>
       </c>
-      <c r="I13" s="9">
-        <v>7.9181819971399996</v>
-      </c>
-      <c r="J13" s="9">
-        <v>38.897920638499997</v>
+      <c r="I13" s="7">
+        <v>7.9</v>
+      </c>
+      <c r="J13" s="7">
+        <v>7.4978749960000002</v>
       </c>
       <c r="K13" s="8">
-        <v>7.9</v>
+        <v>8.3564408941699995</v>
       </c>
       <c r="L13" s="8">
-        <v>35.3012984</v>
-      </c>
-      <c r="M13" s="8">
-        <v>9.0340666069999997</v>
-      </c>
-      <c r="N13" s="8">
-        <v>7.4978749960000002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+        <v>37.765944230499997</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="P13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="X13" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB13" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="AF13" s="7"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1273,26 +1929,34 @@
       <c r="H14" s="4">
         <v>37.9</v>
       </c>
-      <c r="I14" s="9">
-        <v>8.3386718548999994</v>
-      </c>
-      <c r="J14" s="9">
-        <v>37.730435579000002</v>
+      <c r="I14" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="J14" s="7">
+        <v>8.171220924</v>
       </c>
       <c r="K14" s="8">
-        <v>8.1</v>
+        <v>8.6641307019799996</v>
       </c>
       <c r="L14" s="8">
-        <v>35.029306419999998</v>
-      </c>
-      <c r="M14" s="8">
-        <v>9.0643478290000008</v>
-      </c>
-      <c r="N14" s="8">
-        <v>8.171220924</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+        <v>36.667063314099998</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="P14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="T14" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="X14" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB14" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF14" s="7"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1318,26 +1982,34 @@
       <c r="H15" s="1">
         <v>41.9</v>
       </c>
-      <c r="I15" s="9">
-        <v>7.7771759233899997</v>
-      </c>
-      <c r="J15" s="9">
-        <v>43.789521868000001</v>
+      <c r="I15" s="7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J15" s="7">
+        <v>7.25616532</v>
       </c>
       <c r="K15" s="8">
-        <v>8.1999999999999993</v>
+        <v>8.1476187211800006</v>
       </c>
       <c r="L15" s="8">
-        <v>38.962523609999998</v>
-      </c>
-      <c r="M15" s="8">
-        <v>8.9608700429999999</v>
-      </c>
-      <c r="N15" s="8">
-        <v>7.25616532</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+        <v>42.487170725600002</v>
+      </c>
+      <c r="M15" s="8"/>
+      <c r="P15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="T15" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="X15" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB15" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="AF15" s="7"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1363,26 +2035,34 @@
       <c r="H16" s="4">
         <v>37.9</v>
       </c>
-      <c r="I16" s="9">
-        <v>8.6235361314900008</v>
-      </c>
-      <c r="J16" s="9">
-        <v>39.349501308400001</v>
+      <c r="I16" s="7">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J16" s="7">
+        <v>8.7522152630000001</v>
       </c>
       <c r="K16" s="8">
-        <v>8.8000000000000007</v>
+        <v>8.8779532591700008</v>
       </c>
       <c r="L16" s="8">
-        <v>35.304396609999998</v>
-      </c>
-      <c r="M16" s="8">
-        <v>9.3349326730000008</v>
-      </c>
-      <c r="N16" s="8">
-        <v>8.7522152630000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+        <v>38.031601374300003</v>
+      </c>
+      <c r="M16" s="8"/>
+      <c r="P16" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="T16" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="X16" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB16" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="AF16" s="7"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1408,26 +2088,34 @@
       <c r="H17" s="1">
         <v>36.6</v>
       </c>
-      <c r="I17" s="9">
-        <v>8.8775350834500006</v>
-      </c>
-      <c r="J17" s="9">
-        <v>37.921190752900003</v>
+      <c r="I17" s="7">
+        <v>9</v>
+      </c>
+      <c r="J17" s="7">
+        <v>9.0054255229999995</v>
       </c>
       <c r="K17" s="8">
-        <v>9</v>
+        <v>9.0770235013599994</v>
       </c>
       <c r="L17" s="8">
-        <v>35.028511340000001</v>
-      </c>
-      <c r="M17" s="8">
-        <v>9.3565337900000003</v>
-      </c>
-      <c r="N17" s="8">
-        <v>9.0054255229999995</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+        <v>36.780133411900003</v>
+      </c>
+      <c r="M17" s="8"/>
+      <c r="P17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="T17" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="X17" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB17" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="AF17" s="7"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1453,26 +2141,34 @@
       <c r="H18" s="4">
         <v>40.9</v>
       </c>
-      <c r="I18" s="9">
-        <v>8.4101045303199999</v>
-      </c>
-      <c r="J18" s="9">
-        <v>44.623339962099998</v>
+      <c r="I18" s="7">
+        <v>9</v>
+      </c>
+      <c r="J18" s="7">
+        <v>8.1321077689999992</v>
       </c>
       <c r="K18" s="8">
-        <v>9</v>
+        <v>8.7033832451999995</v>
       </c>
       <c r="L18" s="8">
-        <v>38.98535322</v>
-      </c>
-      <c r="M18" s="8">
-        <v>9.3667524370000006</v>
-      </c>
-      <c r="N18" s="8">
-        <v>8.1321077689999992</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+        <v>43.057176394599999</v>
+      </c>
+      <c r="M18" s="8"/>
+      <c r="P18" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="T18" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="X18" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB18" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="AF18" s="7"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1498,26 +2194,34 @@
       <c r="H19" s="1">
         <v>36.6</v>
       </c>
-      <c r="I19" s="9">
-        <v>9.0610772544699998</v>
-      </c>
-      <c r="J19" s="9">
-        <v>39.499881566500001</v>
+      <c r="I19" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="J19" s="7">
+        <v>9.2810226670000002</v>
       </c>
       <c r="K19" s="8">
-        <v>9.5</v>
+        <v>9.2743858831299999</v>
       </c>
       <c r="L19" s="8">
-        <v>35.26413745</v>
-      </c>
-      <c r="M19" s="8">
-        <v>9.6509882339999997</v>
-      </c>
-      <c r="N19" s="8">
-        <v>9.2810226670000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+        <v>38.046641301599998</v>
+      </c>
+      <c r="M19" s="8"/>
+      <c r="P19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="T19" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="X19" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB19" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="AF19" s="7"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1543,26 +2247,34 @@
       <c r="H20" s="4">
         <v>35.6</v>
       </c>
-      <c r="I20" s="9">
-        <v>9.2553960572099996</v>
-      </c>
-      <c r="J20" s="9">
-        <v>37.995796544900003</v>
+      <c r="I20" s="7">
+        <v>9.65</v>
+      </c>
+      <c r="J20" s="7">
+        <v>9.4350865689999992</v>
       </c>
       <c r="K20" s="8">
-        <v>9.65</v>
+        <v>9.4285119794799996</v>
       </c>
       <c r="L20" s="8">
-        <v>35.02257041</v>
-      </c>
-      <c r="M20" s="8">
-        <v>9.6558080369999999</v>
-      </c>
-      <c r="N20" s="8">
-        <v>9.4350865689999992</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+        <v>36.748522556099999</v>
+      </c>
+      <c r="M20" s="8"/>
+      <c r="P20" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T20" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="X20" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB20" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF20" s="7"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1588,26 +2300,34 @@
       <c r="H21" s="1">
         <v>41.1</v>
       </c>
-      <c r="I21" s="9">
-        <v>8.9528353419600002</v>
-      </c>
-      <c r="J21" s="9">
-        <v>44.394619956500001</v>
+      <c r="I21" s="7">
+        <v>10</v>
+      </c>
+      <c r="J21" s="7">
+        <v>11.177502260000001</v>
       </c>
       <c r="K21" s="8">
-        <v>10</v>
+        <v>9.3406659813200008</v>
       </c>
       <c r="L21" s="8">
-        <v>42.034089289999997</v>
-      </c>
-      <c r="M21" s="8">
-        <v>10.39887839</v>
-      </c>
-      <c r="N21" s="8">
-        <v>11.177502260000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+        <v>43.658894520600001</v>
+      </c>
+      <c r="M21" s="8"/>
+      <c r="P21" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="T21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="X21" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB21" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF21" s="7"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1633,26 +2353,34 @@
       <c r="H22" s="4">
         <v>38.799999999999997</v>
       </c>
-      <c r="I22" s="9">
-        <v>12.196955339400001</v>
-      </c>
-      <c r="J22" s="9">
-        <v>39.561222616400002</v>
+      <c r="I22" s="7">
+        <v>11.7</v>
+      </c>
+      <c r="J22" s="7">
+        <v>13.219360229999999</v>
       </c>
       <c r="K22" s="8">
-        <v>11.7</v>
+        <v>12.9437558676</v>
       </c>
       <c r="L22" s="8">
-        <v>35.611136219999999</v>
-      </c>
-      <c r="M22" s="8">
-        <v>14.89636114</v>
-      </c>
-      <c r="N22" s="8">
-        <v>13.219360229999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+        <v>38.7385219214</v>
+      </c>
+      <c r="M22" s="8"/>
+      <c r="P22" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="T22" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="X22" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB22" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="AF22" s="7"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1678,26 +2406,34 @@
       <c r="H23" s="1">
         <v>37.799999999999997</v>
       </c>
-      <c r="I23" s="9">
-        <v>13.6198328674</v>
-      </c>
-      <c r="J23" s="9">
-        <v>37.157775445200002</v>
+      <c r="I23" s="7">
+        <v>12.5</v>
+      </c>
+      <c r="J23" s="7">
+        <v>13.59416671</v>
       </c>
       <c r="K23" s="8">
-        <v>12.5</v>
+        <v>14.2350662448</v>
       </c>
       <c r="L23" s="8">
-        <v>32.084828780000002</v>
-      </c>
-      <c r="M23" s="8">
-        <v>15.80480888</v>
-      </c>
-      <c r="N23" s="8">
-        <v>13.59416671</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+        <v>36.037707650800002</v>
+      </c>
+      <c r="M23" s="8"/>
+      <c r="P23" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="T23" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="X23" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB23" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF23" s="7"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1723,26 +2459,34 @@
       <c r="H24" s="4">
         <v>44.9</v>
       </c>
-      <c r="I24" s="9">
-        <v>10.607289916199999</v>
-      </c>
-      <c r="J24" s="9">
-        <v>47.748556644399997</v>
+      <c r="I24" s="7">
+        <v>11.5</v>
+      </c>
+      <c r="J24" s="7">
+        <v>11.735591189999999</v>
       </c>
       <c r="K24" s="8">
-        <v>11.5</v>
+        <v>11.0366847651</v>
       </c>
       <c r="L24" s="8">
-        <v>45.088016719999999</v>
-      </c>
-      <c r="M24" s="8">
-        <v>12.17090411</v>
-      </c>
-      <c r="N24" s="8">
-        <v>11.735591189999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+        <v>46.979798993700001</v>
+      </c>
+      <c r="M24" s="8"/>
+      <c r="P24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="T24" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="X24" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB24" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AF24" s="7"/>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1768,26 +2512,34 @@
       <c r="H25" s="1">
         <v>40.4</v>
       </c>
-      <c r="I25" s="9">
-        <v>13.508423135699999</v>
-      </c>
-      <c r="J25" s="9">
-        <v>40.897857679399998</v>
+      <c r="I25" s="7">
+        <v>13.5</v>
+      </c>
+      <c r="J25" s="7">
+        <v>14.282737859999999</v>
       </c>
       <c r="K25" s="8">
-        <v>13.5</v>
+        <v>14.0376455414</v>
       </c>
       <c r="L25" s="8">
-        <v>35.577398610000003</v>
-      </c>
-      <c r="M25" s="8">
-        <v>15.520311400000001</v>
-      </c>
-      <c r="N25" s="8">
-        <v>14.282737859999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+        <v>39.6997978598</v>
+      </c>
+      <c r="M25" s="8"/>
+      <c r="P25" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="T25" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="X25" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB25" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="AF25" s="7"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1813,26 +2565,34 @@
       <c r="H26" s="4">
         <v>37.5</v>
       </c>
-      <c r="I26" s="9">
-        <v>14.361990887899999</v>
-      </c>
-      <c r="J26" s="9">
-        <v>37.551711292100002</v>
+      <c r="I26" s="7">
+        <v>14.2</v>
+      </c>
+      <c r="J26" s="7">
+        <v>15.104304369999999</v>
       </c>
       <c r="K26" s="8">
-        <v>14.2</v>
+        <v>14.8250921988</v>
       </c>
       <c r="L26" s="8">
-        <v>31.81963734</v>
-      </c>
-      <c r="M26" s="8">
-        <v>16.091846749999998</v>
-      </c>
-      <c r="N26" s="8">
-        <v>15.104304369999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+        <v>36.184008874900002</v>
+      </c>
+      <c r="M26" s="8"/>
+      <c r="P26" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="T26" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="X26" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB26" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="AF26" s="7"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1858,26 +2618,34 @@
       <c r="H27" s="1">
         <v>47</v>
       </c>
-      <c r="I27" s="9">
-        <v>11.901174947499999</v>
-      </c>
-      <c r="J27" s="9">
-        <v>50.252434781399998</v>
+      <c r="I27" s="7">
+        <v>13</v>
+      </c>
+      <c r="J27" s="7">
+        <v>12.34060298</v>
       </c>
       <c r="K27" s="8">
-        <v>13</v>
+        <v>12.329546318</v>
       </c>
       <c r="L27" s="8">
-        <v>46.863682220000001</v>
-      </c>
-      <c r="M27" s="8">
-        <v>13.43887924</v>
-      </c>
-      <c r="N27" s="8">
-        <v>12.34060298</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+        <v>49.323975191000002</v>
+      </c>
+      <c r="M27" s="8"/>
+      <c r="P27" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="T27" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="X27" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB27" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="AF27" s="7"/>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1903,26 +2671,34 @@
       <c r="H28" s="4">
         <v>39.5</v>
       </c>
-      <c r="I28" s="9">
-        <v>14.351913245</v>
-      </c>
-      <c r="J28" s="9">
-        <v>41.382540007199999</v>
+      <c r="I28" s="7">
+        <v>14.8</v>
+      </c>
+      <c r="J28" s="7">
+        <v>15.272513630000001</v>
       </c>
       <c r="K28" s="8">
-        <v>14.8</v>
+        <v>14.832398797</v>
       </c>
       <c r="L28" s="8">
-        <v>35.203163199999999</v>
-      </c>
-      <c r="M28" s="8">
-        <v>16.142805989999999</v>
-      </c>
-      <c r="N28" s="8">
-        <v>15.272513630000001</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+        <v>39.876106315400001</v>
+      </c>
+      <c r="M28" s="8"/>
+      <c r="P28" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="T28" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="X28" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB28" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="AF28" s="7"/>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1948,26 +2724,34 @@
       <c r="H29" s="1">
         <v>35.6</v>
       </c>
-      <c r="I29" s="9">
-        <v>15.0522278741</v>
-      </c>
-      <c r="J29" s="9">
-        <v>37.590715597200003</v>
+      <c r="I29" s="7">
+        <v>15.7</v>
+      </c>
+      <c r="J29" s="7">
+        <v>16.021434150000001</v>
       </c>
       <c r="K29" s="8">
-        <v>15.7</v>
+        <v>15.512902462</v>
       </c>
       <c r="L29" s="8">
-        <v>31.464731090000001</v>
-      </c>
-      <c r="M29" s="8">
-        <v>16.605308050000001</v>
-      </c>
-      <c r="N29" s="8">
-        <v>16.021434150000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+        <v>35.892675915399998</v>
+      </c>
+      <c r="M29" s="8"/>
+      <c r="P29" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="T29" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="X29" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB29" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF29" s="7"/>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1993,26 +2777,34 @@
       <c r="H30" s="4">
         <v>43.3</v>
       </c>
-      <c r="I30" s="9">
-        <v>7.4803040562199996</v>
-      </c>
-      <c r="J30" s="9">
-        <v>47.324734524299998</v>
+      <c r="I30" s="7">
+        <v>8</v>
+      </c>
+      <c r="J30" s="7">
+        <v>9.0038824539999993</v>
       </c>
       <c r="K30" s="8">
-        <v>8</v>
+        <v>7.7752160422700003</v>
       </c>
       <c r="L30" s="8">
-        <v>44.673194219999999</v>
-      </c>
-      <c r="M30" s="8">
-        <v>8.5582126269999996</v>
-      </c>
-      <c r="N30" s="8">
-        <v>9.0038824539999993</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+        <v>46.516168034400003</v>
+      </c>
+      <c r="M30" s="8"/>
+      <c r="P30" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="T30" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="X30" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB30" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="AF30" s="7"/>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2038,26 +2830,34 @@
       <c r="H31" s="1">
         <v>40.9</v>
       </c>
-      <c r="I31" s="9">
-        <v>9.5775817123600007</v>
-      </c>
-      <c r="J31" s="9">
-        <v>42.411655227899999</v>
+      <c r="I31" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="J31" s="7">
+        <v>11.48457443</v>
       </c>
       <c r="K31" s="8">
-        <v>9.5</v>
+        <v>10.2018576794</v>
       </c>
       <c r="L31" s="8">
-        <v>39.425971789999998</v>
-      </c>
-      <c r="M31" s="8">
-        <v>12.23357923</v>
-      </c>
-      <c r="N31" s="8">
-        <v>11.48457443</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+        <v>41.596327217000002</v>
+      </c>
+      <c r="M31" s="8"/>
+      <c r="P31" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="T31" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="X31" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB31" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF31" s="7"/>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2083,26 +2883,34 @@
       <c r="H32" s="4">
         <v>40</v>
       </c>
-      <c r="I32" s="9">
-        <v>10.8414157373</v>
-      </c>
-      <c r="J32" s="9">
-        <v>40.674915021899999</v>
+      <c r="I32" s="7">
+        <v>10</v>
+      </c>
+      <c r="J32" s="7">
+        <v>12.07212595</v>
       </c>
       <c r="K32" s="8">
-        <v>10</v>
+        <v>11.6451410943</v>
       </c>
       <c r="L32" s="8">
-        <v>37.104379649999998</v>
-      </c>
-      <c r="M32" s="8">
-        <v>13.828535779999999</v>
-      </c>
-      <c r="N32" s="8">
-        <v>12.07212595</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+        <v>39.844373985700003</v>
+      </c>
+      <c r="M32" s="8"/>
+      <c r="P32" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="T32" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="X32" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB32" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF32" s="7"/>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2128,26 +2936,34 @@
       <c r="H33" s="1">
         <v>47.2</v>
       </c>
-      <c r="I33" s="9">
-        <v>9.3029398998899993</v>
-      </c>
-      <c r="J33" s="9">
-        <v>50.6773205127</v>
+      <c r="I33" s="7">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J33" s="7">
+        <v>10.56273097</v>
       </c>
       <c r="K33" s="8">
-        <v>10.199999999999999</v>
+        <v>9.6744266823499991</v>
       </c>
       <c r="L33" s="8">
-        <v>47.822798249999998</v>
-      </c>
-      <c r="M33" s="8">
-        <v>10.65745716</v>
-      </c>
-      <c r="N33" s="8">
-        <v>10.56273097</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+        <v>49.816837546800002</v>
+      </c>
+      <c r="M33" s="8"/>
+      <c r="P33" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="T33" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="X33" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB33" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF33" s="7"/>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2173,26 +2989,34 @@
       <c r="H34" s="4">
         <v>43.6</v>
       </c>
-      <c r="I34" s="9">
-        <v>11.891615034399999</v>
-      </c>
-      <c r="J34" s="9">
-        <v>44.624816233399997</v>
+      <c r="I34" s="7">
+        <v>12</v>
+      </c>
+      <c r="J34" s="7">
+        <v>12.62581915</v>
       </c>
       <c r="K34" s="8">
-        <v>12</v>
+        <v>12.5151756476</v>
       </c>
       <c r="L34" s="8">
-        <v>40.25003641</v>
-      </c>
-      <c r="M34" s="8">
-        <v>14.22854369</v>
-      </c>
-      <c r="N34" s="8">
-        <v>12.62581915</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+        <v>43.589375310000001</v>
+      </c>
+      <c r="M34" s="8"/>
+      <c r="P34" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="T34" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="X34" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB34" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="AF34" s="7"/>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2218,26 +3042,34 @@
       <c r="H35" s="1">
         <v>42</v>
       </c>
-      <c r="I35" s="9">
-        <v>12.8590262949</v>
-      </c>
-      <c r="J35" s="9">
-        <v>42.000313897200002</v>
+      <c r="I35" s="7">
+        <v>12.5</v>
+      </c>
+      <c r="J35" s="7">
+        <v>13.304688799999999</v>
       </c>
       <c r="K35" s="8">
-        <v>12.5</v>
+        <v>13.431470279299999</v>
       </c>
       <c r="L35" s="8">
-        <v>37.12756813</v>
-      </c>
-      <c r="M35" s="8">
-        <v>14.90352135</v>
-      </c>
-      <c r="N35" s="8">
-        <v>13.304688799999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+        <v>40.829516938200001</v>
+      </c>
+      <c r="M35" s="8"/>
+      <c r="P35" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="T35" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="X35" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB35" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="AF35" s="7"/>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2263,26 +3095,34 @@
       <c r="H36" s="4">
         <v>49.7</v>
       </c>
-      <c r="I36" s="9">
-        <v>10.4794116972</v>
-      </c>
-      <c r="J36" s="9">
-        <v>53.183492150100001</v>
+      <c r="I36" s="7">
+        <v>11.5</v>
+      </c>
+      <c r="J36" s="7">
+        <v>11.21689995</v>
       </c>
       <c r="K36" s="8">
-        <v>11.5</v>
+        <v>10.8671689562</v>
       </c>
       <c r="L36" s="8">
-        <v>50.067027420000002</v>
-      </c>
-      <c r="M36" s="8">
-        <v>11.87155939</v>
-      </c>
-      <c r="N36" s="8">
-        <v>11.21689995</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+        <v>52.285627960399999</v>
+      </c>
+      <c r="M36" s="8"/>
+      <c r="P36" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="T36" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="X36" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB36" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF36" s="7"/>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2308,26 +3148,34 @@
       <c r="H37" s="1">
         <v>44.3</v>
       </c>
-      <c r="I37" s="9">
-        <v>12.929101706100001</v>
-      </c>
-      <c r="J37" s="9">
-        <v>45.6378383387</v>
+      <c r="I37" s="7">
+        <v>13.5</v>
+      </c>
+      <c r="J37" s="7">
+        <v>13.723713310000001</v>
       </c>
       <c r="K37" s="8">
-        <v>13.5</v>
+        <v>13.4397995098</v>
       </c>
       <c r="L37" s="8">
-        <v>40.332840750000003</v>
-      </c>
-      <c r="M37" s="8">
-        <v>14.83736959</v>
-      </c>
-      <c r="N37" s="8">
-        <v>13.723713310000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+        <v>44.352922091700002</v>
+      </c>
+      <c r="M37" s="8"/>
+      <c r="P37" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="T37" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="X37" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB37" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="AF37" s="7"/>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2353,27 +3201,155 @@
       <c r="H38" s="4">
         <v>41.6</v>
       </c>
-      <c r="I38" s="9">
-        <v>13.7192627448</v>
-      </c>
-      <c r="J38" s="9">
-        <v>42.404654787600002</v>
+      <c r="I38" s="7">
+        <v>14</v>
+      </c>
+      <c r="J38" s="7">
+        <v>14.35144721</v>
       </c>
       <c r="K38" s="8">
-        <v>14</v>
+        <v>14.1935320248</v>
       </c>
       <c r="L38" s="8">
-        <v>36.954649860000004</v>
-      </c>
-      <c r="M38" s="8">
-        <v>15.392389270000001</v>
-      </c>
-      <c r="N38" s="8">
-        <v>14.35144721</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="J39" s="9"/>
+        <v>40.9925610855</v>
+      </c>
+      <c r="M38" s="8"/>
+      <c r="P38" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="T38" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="X38" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB38" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF38" s="7"/>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="J39" s="8"/>
+      <c r="M39" s="8"/>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="M40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="M41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="T41" s="8"/>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="M42" s="8"/>
+      <c r="P42" s="7"/>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="M43" s="8"/>
+      <c r="P43" s="7"/>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="M44" s="8"/>
+      <c r="P44" s="7"/>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="P45" s="7"/>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="P46" s="7"/>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="P47" s="7"/>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="P48" s="7"/>
+    </row>
+    <row r="49" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P49" s="7"/>
+    </row>
+    <row r="50" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P50" s="7"/>
+    </row>
+    <row r="51" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P51" s="7"/>
+    </row>
+    <row r="52" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P52" s="7"/>
+    </row>
+    <row r="53" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P53" s="7"/>
+    </row>
+    <row r="54" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P54" s="7"/>
+    </row>
+    <row r="55" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P55" s="7"/>
+    </row>
+    <row r="56" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P56" s="7"/>
+    </row>
+    <row r="57" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P57" s="7"/>
+    </row>
+    <row r="58" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P58" s="7"/>
+    </row>
+    <row r="59" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P59" s="8"/>
+    </row>
+    <row r="60" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P60" s="8"/>
+    </row>
+    <row r="61" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P61" s="8"/>
+    </row>
+    <row r="62" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P62" s="8"/>
+    </row>
+    <row r="63" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P63" s="8"/>
+    </row>
+    <row r="64" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P64" s="8"/>
+    </row>
+    <row r="65" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P65" s="8"/>
+    </row>
+    <row r="66" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P66" s="8"/>
+    </row>
+    <row r="67" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P67" s="8"/>
+    </row>
+    <row r="68" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P68" s="8"/>
+    </row>
+    <row r="69" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P69" s="8"/>
+    </row>
+    <row r="70" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P70" s="8"/>
+    </row>
+    <row r="71" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P71" s="8"/>
+    </row>
+    <row r="72" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P72" s="8"/>
+    </row>
+    <row r="73" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P73" s="8"/>
+    </row>
+    <row r="74" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P74" s="8"/>
+    </row>
+    <row r="75" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P75" s="8"/>
+    </row>
+    <row r="76" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P76" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update gas cooler model and update paper's figure
</commit_message>
<xml_diff>
--- a/ComponentTests/supercritical/Table.xlsx
+++ b/ComponentTests/supercritical/Table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="440" windowWidth="30120" windowHeight="20560" tabRatio="500"/>
+    <workbookView xWindow="1840" yWindow="440" windowWidth="30120" windowHeight="20560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
   <si>
     <t>Test Conditions</t>
   </si>
@@ -438,13 +439,16 @@
   </si>
   <si>
     <t>FV2</t>
+  </si>
+  <si>
+    <t>Tout</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -500,6 +504,13 @@
       <color theme="1"/>
       <name val="SF Mono"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -527,7 +538,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -570,8 +581,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -635,8 +659,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -661,8 +689,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -694,6 +724,8 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -725,6 +757,8 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1061,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3201,4 +3235,1016 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AH76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.5" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="7" max="7" width="28.5" customWidth="1"/>
+    <col min="8" max="8" width="32.83203125" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="11"/>
+      <c r="U2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="9"/>
+      <c r="AA2" s="9"/>
+      <c r="AC2" s="9"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14">
+        <v>15</v>
+      </c>
+      <c r="C3" s="15">
+        <v>3</v>
+      </c>
+      <c r="D3" s="15">
+        <v>123.1</v>
+      </c>
+      <c r="E3" s="15">
+        <v>11</v>
+      </c>
+      <c r="F3" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="O3" s="11"/>
+      <c r="P3" s="8"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="8"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="AA3" s="8"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="10"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="11"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="14">
+        <v>15</v>
+      </c>
+      <c r="C4" s="15">
+        <v>3</v>
+      </c>
+      <c r="D4" s="15">
+        <v>123.1</v>
+      </c>
+      <c r="E4" s="15">
+        <v>11</v>
+      </c>
+      <c r="F4" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="8"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="8"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="AA4" s="8"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="7"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="8"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="8"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="11"/>
+      <c r="AA5" s="8"/>
+      <c r="AD5" s="11"/>
+      <c r="AE5" s="11"/>
+      <c r="AF5" s="7"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AF6" s="7"/>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AF7" s="7"/>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AF8" s="7"/>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AF9" s="7"/>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="T10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AF10" s="7"/>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AF11" s="7"/>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AF12" s="7"/>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AF13" s="7"/>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AF14" s="7"/>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AF15" s="7"/>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="AA16" s="8"/>
+      <c r="AF16" s="7"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="AA17" s="8"/>
+      <c r="AF17" s="7"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="AA18" s="8"/>
+      <c r="AF18" s="7"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="AA19" s="8"/>
+      <c r="AF19" s="7"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="AA20" s="8"/>
+      <c r="AF20" s="7"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="AA21" s="8"/>
+      <c r="AF21" s="7"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="AA22" s="8"/>
+      <c r="AF22" s="7"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="AA23" s="8"/>
+      <c r="AF23" s="7"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="AA24" s="8"/>
+      <c r="AF24" s="7"/>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="AA25" s="8"/>
+      <c r="AF25" s="7"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="AA26" s="8"/>
+      <c r="AF26" s="7"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="8"/>
+      <c r="P27" s="8"/>
+      <c r="T27" s="8"/>
+      <c r="W27" s="8"/>
+      <c r="AA27" s="8"/>
+      <c r="AF27" s="7"/>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8"/>
+      <c r="M28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="T28" s="8"/>
+      <c r="W28" s="8"/>
+      <c r="AA28" s="8"/>
+      <c r="AF28" s="7"/>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8"/>
+      <c r="M29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="T29" s="8"/>
+      <c r="W29" s="8"/>
+      <c r="AA29" s="8"/>
+      <c r="AF29" s="7"/>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8"/>
+      <c r="M30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="T30" s="8"/>
+      <c r="W30" s="8"/>
+      <c r="AA30" s="8"/>
+      <c r="AF30" s="7"/>
+    </row>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="T31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="AA31" s="8"/>
+      <c r="AF31" s="7"/>
+    </row>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+      <c r="M32" s="8"/>
+      <c r="P32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="AA32" s="8"/>
+      <c r="AF32" s="7"/>
+    </row>
+    <row r="33" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
+      <c r="P33" s="8"/>
+      <c r="T33" s="8"/>
+      <c r="W33" s="8"/>
+      <c r="AA33" s="8"/>
+      <c r="AF33" s="7"/>
+    </row>
+    <row r="34" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="8"/>
+      <c r="M34" s="8"/>
+      <c r="P34" s="8"/>
+      <c r="T34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="AA34" s="8"/>
+      <c r="AF34" s="7"/>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="8"/>
+      <c r="L35" s="8"/>
+      <c r="M35" s="8"/>
+      <c r="P35" s="8"/>
+      <c r="T35" s="8"/>
+      <c r="W35" s="8"/>
+      <c r="AA35" s="8"/>
+      <c r="AF35" s="7"/>
+    </row>
+    <row r="36" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="8"/>
+      <c r="L36" s="8"/>
+      <c r="M36" s="8"/>
+      <c r="P36" s="8"/>
+      <c r="T36" s="8"/>
+      <c r="W36" s="8"/>
+      <c r="AA36" s="8"/>
+      <c r="AF36" s="7"/>
+    </row>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="8"/>
+      <c r="L37" s="8"/>
+      <c r="M37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="T37" s="8"/>
+      <c r="W37" s="8"/>
+      <c r="AA37" s="8"/>
+      <c r="AF37" s="7"/>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="8"/>
+      <c r="L38" s="8"/>
+      <c r="M38" s="8"/>
+      <c r="P38" s="8"/>
+      <c r="T38" s="8"/>
+      <c r="W38" s="8"/>
+      <c r="AA38" s="8"/>
+      <c r="AF38" s="7"/>
+    </row>
+    <row r="39" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="M39" s="8"/>
+    </row>
+    <row r="40" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="M40" s="8"/>
+      <c r="O40" s="8"/>
+      <c r="P40" s="8"/>
+    </row>
+    <row r="41" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="M41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="T41" s="8"/>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="M42" s="8"/>
+      <c r="P42" s="7"/>
+    </row>
+    <row r="43" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="M43" s="8"/>
+      <c r="P43" s="7"/>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="M44" s="8"/>
+      <c r="P44" s="7"/>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="P45" s="7"/>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="P46" s="7"/>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="P47" s="7"/>
+    </row>
+    <row r="48" spans="1:32" x14ac:dyDescent="0.2">
+      <c r="P48" s="7"/>
+    </row>
+    <row r="49" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P49" s="7"/>
+    </row>
+    <row r="50" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P50" s="7"/>
+    </row>
+    <row r="51" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P51" s="7"/>
+    </row>
+    <row r="52" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P52" s="7"/>
+    </row>
+    <row r="53" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P53" s="7"/>
+    </row>
+    <row r="54" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P54" s="7"/>
+    </row>
+    <row r="55" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P55" s="7"/>
+    </row>
+    <row r="56" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P56" s="7"/>
+    </row>
+    <row r="57" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P57" s="7"/>
+    </row>
+    <row r="58" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P58" s="7"/>
+    </row>
+    <row r="59" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P59" s="8"/>
+    </row>
+    <row r="60" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P60" s="8"/>
+    </row>
+    <row r="61" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P61" s="8"/>
+    </row>
+    <row r="62" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P62" s="8"/>
+    </row>
+    <row r="63" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P63" s="8"/>
+    </row>
+    <row r="64" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P64" s="8"/>
+    </row>
+    <row r="65" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P65" s="8"/>
+    </row>
+    <row r="66" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P66" s="8"/>
+    </row>
+    <row r="67" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P67" s="8"/>
+    </row>
+    <row r="68" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P68" s="8"/>
+    </row>
+    <row r="69" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P69" s="8"/>
+    </row>
+    <row r="70" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P70" s="8"/>
+    </row>
+    <row r="71" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P71" s="8"/>
+    </row>
+    <row r="72" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P72" s="8"/>
+    </row>
+    <row r="73" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P73" s="8"/>
+    </row>
+    <row r="74" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P74" s="8"/>
+    </row>
+    <row r="75" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P75" s="8"/>
+    </row>
+    <row r="76" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P76" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add more parity plots for the gas cooler
</commit_message>
<xml_diff>
--- a/ComponentTests/supercritical/Table.xlsx
+++ b/ComponentTests/supercritical/Table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="29005"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="440" windowWidth="30120" windowHeight="20560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1320" yWindow="440" windowWidth="30120" windowHeight="20560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="149">
   <si>
     <t>Test Conditions</t>
   </si>
@@ -60,12 +60,6 @@
     <t>kg/s</t>
   </si>
   <si>
-    <t>Tested Refrigerant Outlet Temp</t>
-  </si>
-  <si>
-    <t>Simulated Refrigerant Outlet Temp</t>
-  </si>
-  <si>
     <t>MPa</t>
   </si>
   <si>
@@ -442,12 +436,54 @@
   </si>
   <si>
     <t>Tout</t>
+  </si>
+  <si>
+    <t>Approach Temp</t>
+  </si>
+  <si>
+    <t>Ref enthalpy difference</t>
+  </si>
+  <si>
+    <t>kJ/kg</t>
+  </si>
+  <si>
+    <t>Ref Inlet Temp</t>
+  </si>
+  <si>
+    <t>Ref Inlet Pressure</t>
+  </si>
+  <si>
+    <t>Ref Flow Rate</t>
+  </si>
+  <si>
+    <t>Tested Ref Outlet Temp</t>
+  </si>
+  <si>
+    <t>Simulated Ref Outlet Temp</t>
+  </si>
+  <si>
+    <t>kpa</t>
+  </si>
+  <si>
+    <t>predicted pressure drop</t>
+  </si>
+  <si>
+    <t>kPa</t>
+  </si>
+  <si>
+    <t>Tested pressure drop</t>
+  </si>
+  <si>
+    <t>pred T_approach</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -664,7 +700,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -691,6 +727,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1095,22 +1137,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="S3" sqref="S3:S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="28.5" customWidth="1"/>
-    <col min="8" max="8" width="32.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.83203125" customWidth="1"/>
     <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
@@ -1124,47 +1172,57 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>5</v>
+        <v>139</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>7</v>
+        <v>140</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>8</v>
+        <v>141</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>142</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="O1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="13"/>
+      <c r="S1" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="T1" s="11"/>
       <c r="U1" s="11"/>
       <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
+      <c r="W1" s="13"/>
       <c r="X1" s="11"/>
       <c r="Y1" s="11"/>
       <c r="Z1" s="11"/>
@@ -1173,6 +1231,7 @@
       <c r="AC1" s="11"/>
       <c r="AD1" s="11"/>
       <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -1188,7 +1247,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>
@@ -1199,56 +1258,65 @@
       <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>16</v>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>15</v>
+        <v>146</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="11"/>
-      <c r="P2" s="9" t="s">
+      <c r="Q2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="W2" s="9"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="Q2" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="R2" s="9"/>
-      <c r="S2" s="11"/>
-      <c r="T2" t="s">
-        <v>98</v>
-      </c>
-      <c r="U2" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA2" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC2" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD2" s="9"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
+      <c r="AF2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1275,39 +1343,45 @@
       <c r="H3" s="1">
         <v>38</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="1">
+        <v>10.7</v>
+      </c>
+      <c r="J3" s="1">
+        <v>186</v>
+      </c>
+      <c r="L3" s="7">
         <v>8</v>
       </c>
-      <c r="J3" s="7">
+      <c r="M3" s="7">
         <v>7.1413843960000003</v>
       </c>
-      <c r="K3" s="8">
+      <c r="N3" s="8">
         <v>8.3480151618700003</v>
       </c>
-      <c r="L3" s="8">
+      <c r="O3" s="8">
         <v>37.598140358199998</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="R3" s="11"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="W3" s="13"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="AA3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD3" s="13"/>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="11"/>
-      <c r="AH3" s="11"/>
+      <c r="P3" s="17">
+        <v>8.1967583050799995</v>
+      </c>
+      <c r="Q3" s="8"/>
+      <c r="S3" s="8">
+        <v>26.362735761300002</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="W3" s="11"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AF3" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
@@ -1335,37 +1409,45 @@
       <c r="H4" s="3">
         <v>33.5</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="J4" s="3">
+        <v>233.1</v>
+      </c>
+      <c r="L4" s="7">
         <v>9</v>
       </c>
-      <c r="J4" s="7">
+      <c r="M4" s="7">
         <v>8.8980085080000002</v>
       </c>
-      <c r="K4" s="8">
+      <c r="N4" s="8">
         <v>9.0046645190600003</v>
       </c>
-      <c r="L4" s="8">
+      <c r="O4" s="8">
         <v>32.904882553500002</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="W4" s="13"/>
+      <c r="P4" s="17">
+        <v>3.50355105552</v>
+      </c>
+      <c r="Q4" s="8"/>
+      <c r="S4" s="8">
+        <v>23.102332791599999</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="W4" s="11"/>
       <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="AA4" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="Y4" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="11"/>
       <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="7"/>
+      <c r="AF4" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1393,37 +1475,45 @@
       <c r="H5" s="1">
         <v>31.5</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J5" s="1">
+        <v>248.6</v>
+      </c>
+      <c r="L5" s="7">
         <v>9.5</v>
       </c>
-      <c r="J5" s="7">
+      <c r="M5" s="7">
         <v>9.4732699789999995</v>
       </c>
-      <c r="K5" s="8">
+      <c r="N5" s="8">
         <v>9.4461843300799995</v>
       </c>
-      <c r="L5" s="8">
+      <c r="O5" s="8">
         <v>31.4733065936</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="W5" s="13"/>
+      <c r="P5" s="17">
+        <v>2.0721776162099999</v>
+      </c>
+      <c r="Q5" s="8"/>
+      <c r="S5" s="8">
+        <v>22.896745982100001</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="W5" s="11"/>
       <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="AA5" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="Y5" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
-      <c r="AE5" s="11"/>
-      <c r="AF5" s="7"/>
+      <c r="AF5" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
@@ -1451,30 +1541,41 @@
       <c r="H6" s="4">
         <v>36.9</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="4">
+        <v>12.2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>214.8</v>
+      </c>
+      <c r="L6" s="7">
         <v>9.25</v>
       </c>
-      <c r="J6" s="7">
+      <c r="M6" s="7">
         <v>8.2142050090000005</v>
       </c>
-      <c r="K6" s="8">
+      <c r="N6" s="8">
         <v>8.9216813518000002</v>
       </c>
-      <c r="L6" s="8">
+      <c r="O6" s="8">
         <v>38.183843151200001</v>
       </c>
-      <c r="M6" s="8"/>
-      <c r="P6" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="T6" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="W6" s="8"/>
-      <c r="AA6" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF6" s="7"/>
+      <c r="P6" s="17">
+        <v>8.7822393613000003</v>
+      </c>
+      <c r="Q6" s="8"/>
+      <c r="S6" s="8">
+        <v>22.501191319699998</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y6" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB6" s="8"/>
+      <c r="AF6" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1502,30 +1603,41 @@
       <c r="H7" s="1">
         <v>31.2</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="J7" s="1">
+        <v>250.2</v>
+      </c>
+      <c r="L7" s="7">
         <v>9.75</v>
       </c>
-      <c r="J7" s="7">
+      <c r="M7" s="7">
         <v>9.5267881840000008</v>
       </c>
-      <c r="K7" s="8">
+      <c r="N7" s="8">
         <v>9.4468013662200008</v>
       </c>
-      <c r="L7" s="8">
+      <c r="O7" s="8">
         <v>32.889245552399998</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="P7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="W7" s="8"/>
-      <c r="AA7" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF7" s="7"/>
+      <c r="P7" s="17">
+        <v>3.4877818652000001</v>
+      </c>
+      <c r="Q7" s="8"/>
+      <c r="S7" s="8">
+        <v>20.177074323500001</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y7" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB7" s="8"/>
+      <c r="AF7" s="8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
@@ -1553,30 +1665,41 @@
       <c r="H8" s="4">
         <v>30.3</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="J8" s="4">
+        <v>253.1</v>
+      </c>
+      <c r="L8" s="7">
         <v>9.9</v>
       </c>
-      <c r="J8" s="7">
+      <c r="M8" s="7">
         <v>9.6370043079999999</v>
       </c>
-      <c r="K8" s="8">
+      <c r="N8" s="8">
         <v>9.5920280747500009</v>
       </c>
-      <c r="L8" s="8">
+      <c r="O8" s="8">
         <v>31.448114325999999</v>
       </c>
-      <c r="M8" s="8"/>
-      <c r="P8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="T8" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="W8" s="8"/>
-      <c r="AA8" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="AF8" s="7"/>
+      <c r="P8" s="17">
+        <v>2.04684293113</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="S8" s="8">
+        <v>19.663378294299999</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y8" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB8" s="8"/>
+      <c r="AF8" s="8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1604,30 +1727,41 @@
       <c r="H9" s="1">
         <v>34.299999999999997</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>234.3</v>
+      </c>
+      <c r="L9" s="7">
         <v>9.9</v>
       </c>
-      <c r="J9" s="7">
+      <c r="M9" s="7">
         <v>8.9167739380000004</v>
       </c>
-      <c r="K9" s="8">
+      <c r="N9" s="8">
         <v>9.2330228139399999</v>
       </c>
-      <c r="L9" s="8">
+      <c r="O9" s="8">
         <v>38.298985446800003</v>
       </c>
-      <c r="M9" s="8"/>
-      <c r="P9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="T9" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="W9" s="8"/>
-      <c r="AA9" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF9" s="7"/>
+      <c r="P9" s="17">
+        <v>8.89722508985</v>
+      </c>
+      <c r="Q9" s="8"/>
+      <c r="S9" s="8">
+        <v>19.855245389</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y9" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AB9" s="8"/>
+      <c r="AF9" s="8" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
@@ -1655,30 +1789,41 @@
       <c r="H10" s="4">
         <v>30.4</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="J10" s="4">
+        <v>257.8</v>
+      </c>
+      <c r="L10" s="7">
         <v>10</v>
       </c>
-      <c r="J10" s="7">
+      <c r="M10" s="7">
         <v>9.8017882400000005</v>
       </c>
-      <c r="K10" s="8">
+      <c r="N10" s="8">
         <v>9.6931736170900002</v>
       </c>
-      <c r="L10" s="8">
+      <c r="O10" s="8">
         <v>32.618685882900003</v>
       </c>
-      <c r="M10" s="8"/>
-      <c r="P10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="T10" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="W10" s="8"/>
-      <c r="AA10" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="AF10" s="7"/>
+      <c r="P10" s="17">
+        <v>3.2171215737200001</v>
+      </c>
+      <c r="Q10" s="8"/>
+      <c r="S10" s="8">
+        <v>18.0854586574</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y10" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB10" s="8"/>
+      <c r="AF10" s="8" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1706,30 +1851,41 @@
       <c r="H11" s="1">
         <v>29.9</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J11" s="1">
+        <v>259.39999999999998</v>
+      </c>
+      <c r="L11" s="7">
         <v>10</v>
       </c>
-      <c r="J11" s="7">
+      <c r="M11" s="7">
         <v>9.8729621600000002</v>
       </c>
-      <c r="K11" s="8">
+      <c r="N11" s="8">
         <v>9.8386747769599996</v>
       </c>
-      <c r="L11" s="8">
+      <c r="O11" s="8">
         <v>31.197889342300002</v>
       </c>
-      <c r="M11" s="8"/>
-      <c r="P11" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="T11" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="W11" s="8"/>
-      <c r="AA11" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="AF11" s="7"/>
+      <c r="P11" s="17">
+        <v>1.79666832575</v>
+      </c>
+      <c r="Q11" s="8"/>
+      <c r="S11" s="8">
+        <v>17.754273489799999</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y11" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB11" s="8"/>
+      <c r="AF11" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
@@ -1757,30 +1913,41 @@
       <c r="H12" s="4">
         <v>40.6</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="4">
+        <v>7.8</v>
+      </c>
+      <c r="J12" s="4">
+        <v>163.1</v>
+      </c>
+      <c r="L12" s="7">
         <v>7</v>
       </c>
-      <c r="J12" s="7">
+      <c r="M12" s="7">
         <v>6.2168311879999996</v>
       </c>
-      <c r="K12" s="8">
+      <c r="N12" s="8">
         <v>7.0496039637000001</v>
       </c>
-      <c r="L12" s="8">
+      <c r="O12" s="8">
         <v>40.9285437407</v>
       </c>
-      <c r="M12" s="8"/>
-      <c r="P12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="T12" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="W12" s="8"/>
-      <c r="AA12" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="AF12" s="7"/>
+      <c r="P12" s="17">
+        <v>5.9273643826600004</v>
+      </c>
+      <c r="Q12" s="8"/>
+      <c r="S12" s="8">
+        <v>28.177888376599999</v>
+      </c>
+      <c r="U12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y12" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AB12" s="8"/>
+      <c r="AF12" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1808,30 +1975,41 @@
       <c r="H13" s="1">
         <v>38.799999999999997</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="J13" s="1">
+        <v>198.2</v>
+      </c>
+      <c r="L13" s="7">
         <v>7.9</v>
       </c>
-      <c r="J13" s="7">
+      <c r="M13" s="7">
         <v>7.4978749960000002</v>
       </c>
-      <c r="K13" s="8">
+      <c r="N13" s="8">
         <v>8.3564408941699995</v>
       </c>
-      <c r="L13" s="8">
+      <c r="O13" s="8">
         <v>37.765944230499997</v>
       </c>
-      <c r="M13" s="8"/>
-      <c r="P13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="T13" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="W13" s="8"/>
-      <c r="AA13" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF13" s="7"/>
+      <c r="P13" s="17">
+        <v>2.7646593460500002</v>
+      </c>
+      <c r="Q13" s="8"/>
+      <c r="S13" s="8">
+        <v>26.583976598300001</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y13" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB13" s="8"/>
+      <c r="AF13" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
@@ -1859,30 +2037,41 @@
       <c r="H14" s="4">
         <v>37.9</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="J14" s="4">
+        <v>214.3</v>
+      </c>
+      <c r="L14" s="7">
         <v>8.1</v>
       </c>
-      <c r="J14" s="7">
+      <c r="M14" s="7">
         <v>8.171220924</v>
       </c>
-      <c r="K14" s="8">
+      <c r="N14" s="8">
         <v>8.6641307019799996</v>
       </c>
-      <c r="L14" s="8">
+      <c r="O14" s="8">
         <v>36.667063314099998</v>
       </c>
-      <c r="M14" s="8"/>
-      <c r="P14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="T14" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="W14" s="8"/>
-      <c r="AA14" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF14" s="7"/>
+      <c r="P14" s="17">
+        <v>1.66595265329</v>
+      </c>
+      <c r="Q14" s="8"/>
+      <c r="S14" s="8">
+        <v>25.972576892799999</v>
+      </c>
+      <c r="U14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y14" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB14" s="8"/>
+      <c r="AF14" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1910,30 +2099,41 @@
       <c r="H15" s="1">
         <v>41.9</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="J15" s="1">
+        <v>191.8</v>
+      </c>
+      <c r="L15" s="7">
         <v>8.1999999999999993</v>
       </c>
-      <c r="J15" s="7">
+      <c r="M15" s="7">
         <v>7.25616532</v>
       </c>
-      <c r="K15" s="8">
+      <c r="N15" s="8">
         <v>8.1476187211800006</v>
       </c>
-      <c r="L15" s="8">
+      <c r="O15" s="8">
         <v>42.487170725600002</v>
       </c>
-      <c r="M15" s="8"/>
-      <c r="P15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="T15" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="W15" s="8"/>
-      <c r="AA15" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF15" s="7"/>
+      <c r="P15" s="17">
+        <v>7.4857122889500003</v>
+      </c>
+      <c r="Q15" s="8"/>
+      <c r="S15" s="8">
+        <v>24.385722017999999</v>
+      </c>
+      <c r="U15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y15" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB15" s="8"/>
+      <c r="AF15" s="8" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
@@ -1961,30 +2161,41 @@
       <c r="H16" s="4">
         <v>37.9</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="J16" s="4">
+        <v>230.3</v>
+      </c>
+      <c r="L16" s="7">
         <v>8.8000000000000007</v>
       </c>
-      <c r="J16" s="7">
+      <c r="M16" s="7">
         <v>8.7522152630000001</v>
       </c>
-      <c r="K16" s="8">
+      <c r="N16" s="8">
         <v>8.8779532591700008</v>
       </c>
-      <c r="L16" s="8">
+      <c r="O16" s="8">
         <v>38.031601374300003</v>
       </c>
-      <c r="M16" s="8"/>
-      <c r="P16" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T16" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="W16" s="8"/>
-      <c r="AA16" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF16" s="7"/>
+      <c r="P16" s="17">
+        <v>3.0302681926599999</v>
+      </c>
+      <c r="Q16" s="8"/>
+      <c r="S16" s="8">
+        <v>22.313537268600001</v>
+      </c>
+      <c r="U16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y16" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB16" s="8"/>
+      <c r="AF16" s="8" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -2012,30 +2223,41 @@
       <c r="H17" s="1">
         <v>36.6</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="1">
+        <v>2</v>
+      </c>
+      <c r="J17" s="1">
+        <v>236.9</v>
+      </c>
+      <c r="L17" s="7">
         <v>9</v>
       </c>
-      <c r="J17" s="7">
+      <c r="M17" s="7">
         <v>9.0054255229999995</v>
       </c>
-      <c r="K17" s="8">
+      <c r="N17" s="8">
         <v>9.0770235013599994</v>
       </c>
-      <c r="L17" s="8">
+      <c r="O17" s="8">
         <v>36.780133411900003</v>
       </c>
-      <c r="M17" s="8"/>
-      <c r="P17" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="T17" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="W17" s="8"/>
-      <c r="AA17" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AF17" s="7"/>
+      <c r="P17" s="17">
+        <v>1.7790437461799999</v>
+      </c>
+      <c r="Q17" s="8"/>
+      <c r="S17" s="8">
+        <v>21.8413634327</v>
+      </c>
+      <c r="U17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y17" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB17" s="8"/>
+      <c r="AF17" s="8" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
@@ -2063,30 +2285,41 @@
       <c r="H18" s="4">
         <v>40.9</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="4">
+        <v>10.8</v>
+      </c>
+      <c r="J18" s="4">
+        <v>214.2</v>
+      </c>
+      <c r="L18" s="7">
         <v>9</v>
       </c>
-      <c r="J18" s="7">
+      <c r="M18" s="7">
         <v>8.1321077689999992</v>
       </c>
-      <c r="K18" s="8">
+      <c r="N18" s="8">
         <v>8.7033832451999995</v>
       </c>
-      <c r="L18" s="8">
+      <c r="O18" s="8">
         <v>43.057176394599999</v>
       </c>
-      <c r="M18" s="8"/>
-      <c r="P18" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="T18" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="W18" s="8"/>
-      <c r="AA18" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF18" s="7"/>
+      <c r="P18" s="17">
+        <v>8.0555464684399993</v>
+      </c>
+      <c r="Q18" s="8"/>
+      <c r="S18" s="8">
+        <v>21.487278510700001</v>
+      </c>
+      <c r="U18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y18" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB18" s="8"/>
+      <c r="AF18" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -2114,30 +2347,41 @@
       <c r="H19" s="1">
         <v>36.6</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="J19" s="1">
+        <v>244.2</v>
+      </c>
+      <c r="L19" s="7">
         <v>9.5</v>
       </c>
-      <c r="J19" s="7">
+      <c r="M19" s="7">
         <v>9.2810226670000002</v>
       </c>
-      <c r="K19" s="8">
+      <c r="N19" s="8">
         <v>9.2743858831299999</v>
       </c>
-      <c r="L19" s="8">
+      <c r="O19" s="8">
         <v>38.046641301599998</v>
       </c>
-      <c r="M19" s="8"/>
-      <c r="P19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="T19" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="W19" s="8"/>
-      <c r="AA19" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="AF19" s="7"/>
+      <c r="P19" s="17">
+        <v>3.0452302362500001</v>
+      </c>
+      <c r="Q19" s="8"/>
+      <c r="S19" s="8">
+        <v>19.800386083999999</v>
+      </c>
+      <c r="U19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y19" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB19" s="8"/>
+      <c r="AF19" s="8" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
@@ -2165,30 +2409,41 @@
       <c r="H20" s="4">
         <v>35.6</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="J20" s="4">
+        <v>248.2</v>
+      </c>
+      <c r="L20" s="7">
         <v>9.65</v>
       </c>
-      <c r="J20" s="7">
+      <c r="M20" s="7">
         <v>9.4350865689999992</v>
       </c>
-      <c r="K20" s="8">
+      <c r="N20" s="8">
         <v>9.4285119794799996</v>
       </c>
-      <c r="L20" s="8">
+      <c r="O20" s="8">
         <v>36.748522556099999</v>
       </c>
-      <c r="M20" s="8"/>
-      <c r="P20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="T20" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="W20" s="8"/>
-      <c r="AA20" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="AF20" s="7"/>
+      <c r="P20" s="17">
+        <v>1.74737487179</v>
+      </c>
+      <c r="Q20" s="8"/>
+      <c r="S20" s="8">
+        <v>19.438277339399999</v>
+      </c>
+      <c r="U20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y20" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AB20" s="8"/>
+      <c r="AF20" s="8" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -2216,30 +2471,41 @@
       <c r="H21" s="1">
         <v>41.1</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="1">
+        <v>11.7</v>
+      </c>
+      <c r="J21" s="1">
+        <v>111.7</v>
+      </c>
+      <c r="L21" s="7">
         <v>10</v>
       </c>
-      <c r="J21" s="7">
+      <c r="M21" s="7">
         <v>11.177502260000001</v>
       </c>
-      <c r="K21" s="8">
+      <c r="N21" s="8">
         <v>9.3406659813200008</v>
       </c>
-      <c r="L21" s="8">
+      <c r="O21" s="8">
         <v>43.658894520600001</v>
       </c>
-      <c r="M21" s="8"/>
-      <c r="P21" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="T21" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="W21" s="8"/>
-      <c r="AA21" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF21" s="7"/>
+      <c r="P21" s="17">
+        <v>14.2572725804</v>
+      </c>
+      <c r="Q21" s="8"/>
+      <c r="S21" s="8">
+        <v>92.263490076699995</v>
+      </c>
+      <c r="U21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y21" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB21" s="8"/>
+      <c r="AF21" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
@@ -2267,30 +2533,41 @@
       <c r="H22" s="4">
         <v>38.799999999999997</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="4">
+        <v>8.9</v>
+      </c>
+      <c r="J22" s="4">
+        <v>149.19999999999999</v>
+      </c>
+      <c r="L22" s="7">
         <v>11.7</v>
       </c>
-      <c r="J22" s="7">
+      <c r="M22" s="7">
         <v>13.219360229999999</v>
       </c>
-      <c r="K22" s="8">
+      <c r="N22" s="8">
         <v>12.9437558676</v>
       </c>
-      <c r="L22" s="8">
+      <c r="O22" s="8">
         <v>38.7385219214</v>
       </c>
-      <c r="M22" s="8"/>
-      <c r="P22" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="T22" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="W22" s="8"/>
-      <c r="AA22" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF22" s="7"/>
+      <c r="P22" s="17">
+        <v>9.3366670980100004</v>
+      </c>
+      <c r="Q22" s="8"/>
+      <c r="S22" s="8">
+        <v>83.743491851000002</v>
+      </c>
+      <c r="U22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y22" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB22" s="8"/>
+      <c r="AF22" s="8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -2318,30 +2595,41 @@
       <c r="H23" s="1">
         <v>37.799999999999997</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="J23" s="1">
+        <v>166.4</v>
+      </c>
+      <c r="L23" s="7">
         <v>12.5</v>
       </c>
-      <c r="J23" s="7">
+      <c r="M23" s="7">
         <v>13.59416671</v>
       </c>
-      <c r="K23" s="8">
+      <c r="N23" s="8">
         <v>14.2350662448</v>
       </c>
-      <c r="L23" s="8">
+      <c r="O23" s="8">
         <v>36.037707650800002</v>
       </c>
-      <c r="M23" s="8"/>
-      <c r="P23" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="T23" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="W23" s="8"/>
-      <c r="AA23" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF23" s="7"/>
+      <c r="P23" s="17">
+        <v>6.6353539153899996</v>
+      </c>
+      <c r="Q23" s="8"/>
+      <c r="S23" s="8">
+        <v>76.974449882800002</v>
+      </c>
+      <c r="U23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y23" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB23" s="8"/>
+      <c r="AF23" s="8" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
@@ -2369,30 +2657,41 @@
       <c r="H24" s="4">
         <v>44.9</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="4">
+        <v>16.3</v>
+      </c>
+      <c r="J24" s="4">
+        <v>133.9</v>
+      </c>
+      <c r="L24" s="7">
         <v>11.5</v>
       </c>
-      <c r="J24" s="7">
+      <c r="M24" s="7">
         <v>11.735591189999999</v>
       </c>
-      <c r="K24" s="8">
+      <c r="N24" s="8">
         <v>11.0366847651</v>
       </c>
-      <c r="L24" s="8">
+      <c r="O24" s="8">
         <v>46.979798993700001</v>
       </c>
-      <c r="M24" s="8"/>
-      <c r="P24" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="T24" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="W24" s="8"/>
-      <c r="AA24" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AF24" s="7"/>
+      <c r="P24" s="17">
+        <v>17.5781896913</v>
+      </c>
+      <c r="Q24" s="8"/>
+      <c r="S24" s="8">
+        <v>82.469053979799995</v>
+      </c>
+      <c r="U24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y24" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB24" s="8"/>
+      <c r="AF24" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -2420,30 +2719,41 @@
       <c r="H25" s="1">
         <v>40.4</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="1">
+        <v>10</v>
+      </c>
+      <c r="J25" s="1">
+        <v>183.4</v>
+      </c>
+      <c r="L25" s="7">
         <v>13.5</v>
       </c>
-      <c r="J25" s="7">
+      <c r="M25" s="7">
         <v>14.282737859999999</v>
       </c>
-      <c r="K25" s="8">
+      <c r="N25" s="8">
         <v>14.0376455414</v>
       </c>
-      <c r="L25" s="8">
+      <c r="O25" s="8">
         <v>39.6997978598</v>
       </c>
-      <c r="M25" s="8"/>
-      <c r="P25" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="T25" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="W25" s="8"/>
-      <c r="AA25" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="AF25" s="7"/>
+      <c r="P25" s="17">
+        <v>10.297383476</v>
+      </c>
+      <c r="Q25" s="8"/>
+      <c r="S25" s="8">
+        <v>70.329317754200005</v>
+      </c>
+      <c r="U25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y25" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="AB25" s="8"/>
+      <c r="AF25" s="8" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
@@ -2471,30 +2781,41 @@
       <c r="H26" s="4">
         <v>37.5</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="4">
+        <v>5.9</v>
+      </c>
+      <c r="J26" s="4">
+        <v>196.2</v>
+      </c>
+      <c r="L26" s="7">
         <v>14.2</v>
       </c>
-      <c r="J26" s="7">
+      <c r="M26" s="7">
         <v>15.104304369999999</v>
       </c>
-      <c r="K26" s="8">
+      <c r="N26" s="8">
         <v>14.8250921988</v>
       </c>
-      <c r="L26" s="8">
+      <c r="O26" s="8">
         <v>36.184008874900002</v>
       </c>
-      <c r="M26" s="8"/>
-      <c r="P26" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="T26" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="W26" s="8"/>
-      <c r="AA26" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF26" s="7"/>
+      <c r="P26" s="17">
+        <v>6.7813029292999998</v>
+      </c>
+      <c r="Q26" s="8"/>
+      <c r="S26" s="8">
+        <v>64.409442321499995</v>
+      </c>
+      <c r="U26" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y26" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB26" s="8"/>
+      <c r="AF26" s="8" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -2522,30 +2843,41 @@
       <c r="H27" s="1">
         <v>47</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="1">
+        <v>19.8</v>
+      </c>
+      <c r="J27" s="1">
+        <v>152.9</v>
+      </c>
+      <c r="L27" s="7">
         <v>13</v>
       </c>
-      <c r="J27" s="7">
+      <c r="M27" s="7">
         <v>12.34060298</v>
       </c>
-      <c r="K27" s="8">
+      <c r="N27" s="8">
         <v>12.329546318</v>
       </c>
-      <c r="L27" s="8">
+      <c r="O27" s="8">
         <v>49.323975191000002</v>
       </c>
-      <c r="M27" s="8"/>
-      <c r="P27" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="T27" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="W27" s="8"/>
-      <c r="AA27" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF27" s="7"/>
+      <c r="P27" s="17">
+        <v>19.922119521900001</v>
+      </c>
+      <c r="Q27" s="8"/>
+      <c r="S27" s="8">
+        <v>74.378326171099999</v>
+      </c>
+      <c r="U27" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y27" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="AB27" s="8"/>
+      <c r="AF27" s="8" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
@@ -2573,30 +2905,41 @@
       <c r="H28" s="4">
         <v>39.5</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="4">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J28" s="4">
+        <v>198.8</v>
+      </c>
+      <c r="L28" s="7">
         <v>14.8</v>
       </c>
-      <c r="J28" s="7">
+      <c r="M28" s="7">
         <v>15.272513630000001</v>
       </c>
-      <c r="K28" s="8">
+      <c r="N28" s="8">
         <v>14.832398797</v>
       </c>
-      <c r="L28" s="8">
+      <c r="O28" s="8">
         <v>39.876106315400001</v>
       </c>
-      <c r="M28" s="8"/>
-      <c r="P28" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="T28" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="W28" s="8"/>
-      <c r="AA28" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AF28" s="7"/>
+      <c r="P28" s="17">
+        <v>10.4732345003</v>
+      </c>
+      <c r="Q28" s="8"/>
+      <c r="S28" s="8">
+        <v>62.167764951000002</v>
+      </c>
+      <c r="U28" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y28" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="AB28" s="8"/>
+      <c r="AF28" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -2624,30 +2967,41 @@
       <c r="H29" s="1">
         <v>35.6</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="J29" s="1">
+        <v>209.4</v>
+      </c>
+      <c r="L29" s="7">
         <v>15.7</v>
       </c>
-      <c r="J29" s="7">
+      <c r="M29" s="7">
         <v>16.021434150000001</v>
       </c>
-      <c r="K29" s="8">
+      <c r="N29" s="8">
         <v>15.512902462</v>
       </c>
-      <c r="L29" s="8">
+      <c r="O29" s="8">
         <v>35.892675915399998</v>
       </c>
-      <c r="M29" s="8"/>
-      <c r="P29" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="T29" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="W29" s="8"/>
-      <c r="AA29" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF29" s="7"/>
+      <c r="P29" s="17">
+        <v>6.4896415734200001</v>
+      </c>
+      <c r="Q29" s="8"/>
+      <c r="S29" s="8">
+        <v>57.663619630100001</v>
+      </c>
+      <c r="U29" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y29" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB29" s="8"/>
+      <c r="AF29" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
@@ -2675,30 +3029,41 @@
       <c r="H30" s="4">
         <v>43.3</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J30" s="4">
+        <v>93</v>
+      </c>
+      <c r="L30" s="7">
         <v>8</v>
       </c>
-      <c r="J30" s="7">
+      <c r="M30" s="7">
         <v>9.0038824539999993</v>
       </c>
-      <c r="K30" s="8">
+      <c r="N30" s="8">
         <v>7.7752160422700003</v>
       </c>
-      <c r="L30" s="8">
+      <c r="O30" s="8">
         <v>46.516168034400003</v>
       </c>
-      <c r="M30" s="8"/>
-      <c r="P30" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="T30" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="W30" s="8"/>
-      <c r="AA30" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF30" s="7"/>
+      <c r="P30" s="17">
+        <v>11.5143277949</v>
+      </c>
+      <c r="Q30" s="8"/>
+      <c r="S30" s="8">
+        <v>94.004417167599996</v>
+      </c>
+      <c r="U30" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y30" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB30" s="8"/>
+      <c r="AF30" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -2726,30 +3091,41 @@
       <c r="H31" s="1">
         <v>40.9</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="J31" s="1">
+        <v>117.8</v>
+      </c>
+      <c r="L31" s="7">
         <v>9.5</v>
       </c>
-      <c r="J31" s="7">
+      <c r="M31" s="7">
         <v>11.48457443</v>
       </c>
-      <c r="K31" s="8">
+      <c r="N31" s="8">
         <v>10.2018576794</v>
       </c>
-      <c r="L31" s="8">
+      <c r="O31" s="8">
         <v>41.596327217000002</v>
       </c>
-      <c r="M31" s="8"/>
-      <c r="P31" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="T31" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="W31" s="8"/>
-      <c r="AA31" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF31" s="7"/>
+      <c r="P31" s="17">
+        <v>6.5945521714200002</v>
+      </c>
+      <c r="Q31" s="8"/>
+      <c r="S31" s="8">
+        <v>87.786287356000003</v>
+      </c>
+      <c r="U31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y31" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB31" s="8"/>
+      <c r="AF31" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
@@ -2777,30 +3153,41 @@
       <c r="H32" s="4">
         <v>40</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="J32" s="4">
+        <v>125.6</v>
+      </c>
+      <c r="L32" s="7">
         <v>10</v>
       </c>
-      <c r="J32" s="7">
+      <c r="M32" s="7">
         <v>12.07212595</v>
       </c>
-      <c r="K32" s="8">
+      <c r="N32" s="8">
         <v>11.6451410943</v>
       </c>
-      <c r="L32" s="8">
+      <c r="O32" s="8">
         <v>39.844373985700003</v>
       </c>
-      <c r="M32" s="8"/>
-      <c r="P32" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="T32" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="W32" s="8"/>
-      <c r="AA32" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="AF32" s="7"/>
+      <c r="P32" s="17">
+        <v>4.84253232966</v>
+      </c>
+      <c r="Q32" s="8"/>
+      <c r="S32" s="8">
+        <v>84.516840802700003</v>
+      </c>
+      <c r="U32" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y32" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="AB32" s="8"/>
+      <c r="AF32" s="8" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -2828,30 +3215,41 @@
       <c r="H33" s="1">
         <v>47.2</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="1">
+        <v>12.8</v>
+      </c>
+      <c r="J33" s="1">
+        <v>118.6</v>
+      </c>
+      <c r="L33" s="7">
         <v>10.199999999999999</v>
       </c>
-      <c r="J33" s="7">
+      <c r="M33" s="7">
         <v>10.56273097</v>
       </c>
-      <c r="K33" s="8">
+      <c r="N33" s="8">
         <v>9.6744266823499991</v>
       </c>
-      <c r="L33" s="8">
+      <c r="O33" s="8">
         <v>49.816837546800002</v>
       </c>
-      <c r="M33" s="8"/>
-      <c r="P33" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="T33" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="W33" s="8"/>
-      <c r="AA33" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF33" s="7"/>
+      <c r="P33" s="17">
+        <v>14.814999884200001</v>
+      </c>
+      <c r="Q33" s="8"/>
+      <c r="S33" s="8">
+        <v>85.446263963000007</v>
+      </c>
+      <c r="U33" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y33" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="AB33" s="8"/>
+      <c r="AF33" s="8" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
@@ -2879,30 +3277,41 @@
       <c r="H34" s="4">
         <v>43.6</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="4">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J34" s="4">
+        <v>155.9</v>
+      </c>
+      <c r="L34" s="7">
         <v>12</v>
       </c>
-      <c r="J34" s="7">
+      <c r="M34" s="7">
         <v>12.62581915</v>
       </c>
-      <c r="K34" s="8">
+      <c r="N34" s="8">
         <v>12.5151756476</v>
       </c>
-      <c r="L34" s="8">
+      <c r="O34" s="8">
         <v>43.589375310000001</v>
       </c>
-      <c r="M34" s="8"/>
-      <c r="P34" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="T34" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="W34" s="8"/>
-      <c r="AA34" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF34" s="7"/>
+      <c r="P34" s="17">
+        <v>8.5872050156699995</v>
+      </c>
+      <c r="Q34" s="8"/>
+      <c r="S34" s="8">
+        <v>76.711988744400003</v>
+      </c>
+      <c r="U34" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y34" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB34" s="8"/>
+      <c r="AF34" s="8" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="35" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -2930,30 +3339,41 @@
       <c r="H35" s="1">
         <v>42</v>
       </c>
-      <c r="I35" s="7">
+      <c r="I35" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="J35" s="1">
+        <v>168.9</v>
+      </c>
+      <c r="L35" s="7">
         <v>12.5</v>
       </c>
-      <c r="J35" s="7">
+      <c r="M35" s="7">
         <v>13.304688799999999</v>
       </c>
-      <c r="K35" s="8">
+      <c r="N35" s="8">
         <v>13.431470279299999</v>
       </c>
-      <c r="L35" s="8">
+      <c r="O35" s="8">
         <v>40.829516938200001</v>
       </c>
-      <c r="M35" s="8"/>
-      <c r="P35" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="T35" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="W35" s="8"/>
-      <c r="AA35" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF35" s="7"/>
+      <c r="P35" s="17">
+        <v>5.8271606420099999</v>
+      </c>
+      <c r="Q35" s="8"/>
+      <c r="S35" s="8">
+        <v>71.3838109231</v>
+      </c>
+      <c r="U35" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y35" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="AB35" s="8"/>
+      <c r="AF35" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
@@ -2981,30 +3401,41 @@
       <c r="H36" s="4">
         <v>49.7</v>
       </c>
-      <c r="I36" s="7">
+      <c r="I36" s="4">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J36" s="4">
+        <v>134.9</v>
+      </c>
+      <c r="L36" s="7">
         <v>11.5</v>
       </c>
-      <c r="J36" s="7">
+      <c r="M36" s="7">
         <v>11.21689995</v>
       </c>
-      <c r="K36" s="8">
+      <c r="N36" s="8">
         <v>10.8671689562</v>
       </c>
-      <c r="L36" s="8">
+      <c r="O36" s="8">
         <v>52.285627960399999</v>
       </c>
-      <c r="M36" s="8"/>
-      <c r="P36" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="T36" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="W36" s="8"/>
-      <c r="AA36" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="AF36" s="7"/>
+      <c r="P36" s="17">
+        <v>17.283810483100002</v>
+      </c>
+      <c r="Q36" s="8"/>
+      <c r="S36" s="8">
+        <v>76.587639324199998</v>
+      </c>
+      <c r="U36" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y36" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB36" s="8"/>
+      <c r="AF36" s="8" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="37" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -3032,30 +3463,41 @@
       <c r="H37" s="1">
         <v>44.3</v>
       </c>
-      <c r="I37" s="7">
+      <c r="I37" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="J37" s="1">
+        <v>177.5</v>
+      </c>
+      <c r="L37" s="7">
         <v>13.5</v>
       </c>
-      <c r="J37" s="7">
+      <c r="M37" s="7">
         <v>13.723713310000001</v>
       </c>
-      <c r="K37" s="8">
+      <c r="N37" s="8">
         <v>13.4397995098</v>
       </c>
-      <c r="L37" s="8">
+      <c r="O37" s="8">
         <v>44.352922091700002</v>
       </c>
-      <c r="M37" s="8"/>
-      <c r="P37" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T37" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="W37" s="8"/>
-      <c r="AA37" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF37" s="7"/>
+      <c r="P37" s="17">
+        <v>9.3504251887700001</v>
+      </c>
+      <c r="Q37" s="8"/>
+      <c r="S37" s="8">
+        <v>66.667788394699997</v>
+      </c>
+      <c r="U37" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y37" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB37" s="8"/>
+      <c r="AF37" s="8" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
@@ -3083,30 +3525,41 @@
       <c r="H38" s="4">
         <v>41.6</v>
       </c>
-      <c r="I38" s="7">
+      <c r="I38" s="4">
+        <v>5.2</v>
+      </c>
+      <c r="J38" s="4">
+        <v>186.6</v>
+      </c>
+      <c r="L38" s="7">
         <v>14</v>
       </c>
-      <c r="J38" s="7">
+      <c r="M38" s="7">
         <v>14.35144721</v>
       </c>
-      <c r="K38" s="8">
+      <c r="N38" s="8">
         <v>14.1935320248</v>
       </c>
-      <c r="L38" s="8">
+      <c r="O38" s="8">
         <v>40.9925610855</v>
       </c>
-      <c r="M38" s="8"/>
-      <c r="P38" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="T38" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="W38" s="8"/>
-      <c r="AA38" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF38" s="7"/>
+      <c r="P38" s="17">
+        <v>5.9899077289599996</v>
+      </c>
+      <c r="Q38" s="8"/>
+      <c r="S38" s="8">
+        <v>62.315840030499999</v>
+      </c>
+      <c r="U38" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y38" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="AB38" s="8"/>
+      <c r="AF38" s="8" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="39" spans="1:32" x14ac:dyDescent="0.2">
       <c r="J39" s="8"/>
@@ -3121,7 +3574,7 @@
       <c r="M41" s="8"/>
       <c r="O41" s="8"/>
       <c r="P41" s="8"/>
-      <c r="T41" s="8"/>
+      <c r="S41" s="8"/>
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.2">
       <c r="M42" s="8"/>
@@ -3241,7 +3694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -3279,7 +3732,7 @@
         <v>8</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -3320,7 +3773,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
update gas cooler results
</commit_message>
<xml_diff>
--- a/ComponentTests/supercritical/Table.xlsx
+++ b/ComponentTests/supercritical/Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ammarbahman/Desktop/ACHP/ComponentTests/supercritical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82452EBE-E20B-C64A-8B0D-88A1160BBF14}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63892010-0BCB-C240-AB0C-038F553D84A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -25,6 +25,7 @@
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="273">
   <si>
     <t>Test Conditions</t>
   </si>
@@ -852,6 +853,9 @@
   </si>
   <si>
     <t>14.269997918844648 37.18081807841713</t>
+  </si>
+  <si>
+    <t>Simulated Approach Temp</t>
   </si>
 </sst>
 </file>
@@ -1523,10 +1527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL76"/>
+  <dimension ref="A1:AM76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1538,22 +1542,23 @@
     <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.83203125" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="16" max="16" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.83203125" customWidth="1"/>
+    <col min="15" max="15" width="17.6640625" customWidth="1"/>
+    <col min="17" max="17" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="45.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:39">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1579,55 +1584,57 @@
         <v>143</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="16" t="s">
+      <c r="X1" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="X1" s="11"/>
       <c r="Y1" s="11"/>
       <c r="Z1" s="11"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="13"/>
       <c r="AC1" s="11"/>
       <c r="AD1" s="11"/>
       <c r="AE1" s="11"/>
@@ -1636,8 +1643,9 @@
       <c r="AH1" s="11"/>
       <c r="AI1" s="11"/>
       <c r="AJ1" s="11"/>
-    </row>
-    <row r="2" spans="1:38">
+      <c r="AK1" s="11"/>
+    </row>
+    <row r="2" spans="1:39">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1662,34 +1670,32 @@
       <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>2</v>
       </c>
       <c r="P2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="R2" s="6" t="s">
+      <c r="Q2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="16" t="s">
         <v>153</v>
       </c>
       <c r="S2" s="6" t="s">
@@ -1699,42 +1705,45 @@
         <v>153</v>
       </c>
       <c r="U2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="V2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="16" t="s">
+      <c r="X2" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="Y2" s="9" t="s">
+      <c r="Z2" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="AA2" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" t="s">
+      <c r="AB2" s="9"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" t="s">
         <v>96</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AE2" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="AG2" s="9" t="s">
+      <c r="AH2" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AH2" s="9" t="s">
+      <c r="AI2" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="AJ2" s="9" t="s">
+      <c r="AK2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AL2" s="9" t="s">
+      <c r="AM2" s="9" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:39">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1760,61 +1769,65 @@
         <v>38</v>
       </c>
       <c r="I3" s="1">
+        <f>H3-B3</f>
+        <v>8.6000000000000014</v>
+      </c>
+      <c r="J3" s="1">
         <v>10.7</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>186</v>
       </c>
-      <c r="K3" s="18">
+      <c r="L3" s="18">
         <v>29.558706730000001</v>
       </c>
-      <c r="L3" s="7">
+      <c r="M3" s="7">
         <v>8</v>
       </c>
-      <c r="M3" s="7">
+      <c r="N3" s="7">
         <v>7.1413843960000003</v>
       </c>
-      <c r="N3" s="8">
+      <c r="O3" s="8">
         <v>8.3480151618700003</v>
       </c>
-      <c r="O3" s="8">
+      <c r="P3" s="8">
         <v>37.598140358199998</v>
       </c>
-      <c r="P3" s="17">
+      <c r="Q3" s="17">
         <v>8.1967583050799995</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="R3" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="R3" s="19" t="s">
+      <c r="S3" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="T3" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="T3" s="19" t="s">
+      <c r="U3" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="U3" s="8"/>
-      <c r="W3" s="8">
+      <c r="V3" s="8"/>
+      <c r="X3" s="8">
         <v>26.362735761300002</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Z3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="8" t="s">
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AF3" s="13"/>
-      <c r="AG3" s="11"/>
+      <c r="AG3" s="13"/>
       <c r="AH3" s="11"/>
-      <c r="AJ3" s="8" t="s">
+      <c r="AI3" s="11"/>
+      <c r="AK3" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:39">
       <c r="A4" s="3">
         <f>A3+1</f>
         <v>2</v>
@@ -1841,63 +1854,67 @@
         <v>33.5</v>
       </c>
       <c r="I4" s="3">
+        <f t="shared" ref="I4:I38" si="0">H4-B4</f>
+        <v>4.1000000000000014</v>
+      </c>
+      <c r="J4" s="3">
         <v>4.3</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>233.1</v>
       </c>
-      <c r="K4" s="18">
+      <c r="L4" s="18">
         <v>101.59824159999999</v>
       </c>
-      <c r="L4" s="7">
+      <c r="M4" s="7">
         <v>9</v>
       </c>
-      <c r="M4" s="7">
+      <c r="N4" s="7">
         <v>8.8980085080000002</v>
       </c>
-      <c r="N4" s="8">
+      <c r="O4" s="8">
         <v>9.0046645190600003</v>
       </c>
-      <c r="O4" s="8">
+      <c r="P4" s="8">
         <v>32.904882553500002</v>
       </c>
-      <c r="P4" s="17">
+      <c r="Q4" s="17">
         <v>3.50355105552</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="R4" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="S4" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="S4" s="19" t="s">
+      <c r="T4" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="T4" s="19" t="s">
+      <c r="U4" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="U4" s="8"/>
-      <c r="W4" s="8">
+      <c r="V4" s="8"/>
+      <c r="X4" s="8">
         <v>23.102332791599999</v>
       </c>
-      <c r="Y4" s="8" t="s">
+      <c r="Z4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="AA4" s="11"/>
       <c r="AB4" s="11"/>
-      <c r="AC4" s="8" t="s">
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="11"/>
+      <c r="AG4" s="13"/>
       <c r="AH4" s="11"/>
-      <c r="AJ4" s="8" t="s">
+      <c r="AI4" s="11"/>
+      <c r="AK4" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:39">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A38" si="0">A4+1</f>
+        <f t="shared" ref="A5:A38" si="1">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="1">
@@ -1922,63 +1939,67 @@
         <v>31.5</v>
       </c>
       <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1000000000000014</v>
+      </c>
+      <c r="J5" s="1">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>248.6</v>
       </c>
-      <c r="K5" s="18">
+      <c r="L5" s="18">
         <v>98.714085979999993</v>
       </c>
-      <c r="L5" s="7">
+      <c r="M5" s="7">
         <v>9.5</v>
       </c>
-      <c r="M5" s="7">
+      <c r="N5" s="7">
         <v>9.4732699789999995</v>
       </c>
-      <c r="N5" s="8">
+      <c r="O5" s="8">
         <v>9.4461843300799995</v>
       </c>
-      <c r="O5" s="8">
+      <c r="P5" s="8">
         <v>31.4733065936</v>
       </c>
-      <c r="P5" s="17">
+      <c r="Q5" s="17">
         <v>2.0721776162099999</v>
       </c>
-      <c r="Q5" s="19" t="s">
+      <c r="R5" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="R5" s="19" t="s">
+      <c r="S5" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="S5" s="19" t="s">
+      <c r="T5" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="T5" s="19" t="s">
+      <c r="U5" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="U5" s="8"/>
-      <c r="W5" s="8">
+      <c r="V5" s="8"/>
+      <c r="X5" s="8">
         <v>22.896745982100001</v>
       </c>
-      <c r="Y5" s="8" t="s">
+      <c r="Z5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
-      <c r="AC5" s="8" t="s">
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="11"/>
+      <c r="AG5" s="13"/>
       <c r="AH5" s="11"/>
-      <c r="AJ5" s="8" t="s">
+      <c r="AI5" s="11"/>
+      <c r="AK5" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:39">
       <c r="A6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B6" s="4">
@@ -2002,60 +2023,64 @@
       <c r="H6" s="4">
         <v>36.9</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="J6" s="4">
         <v>12.2</v>
       </c>
-      <c r="J6" s="4">
+      <c r="K6" s="4">
         <v>214.8</v>
       </c>
-      <c r="K6" s="18">
+      <c r="L6" s="18">
         <v>65.903511750000007</v>
       </c>
-      <c r="L6" s="7">
+      <c r="M6" s="7">
         <v>9.25</v>
       </c>
-      <c r="M6" s="7">
+      <c r="N6" s="7">
         <v>8.2142050090000005</v>
       </c>
-      <c r="N6" s="8">
+      <c r="O6" s="8">
         <v>8.9216813518000002</v>
       </c>
-      <c r="O6" s="8">
+      <c r="P6" s="8">
         <v>38.183843151200001</v>
       </c>
-      <c r="P6" s="17">
+      <c r="Q6" s="17">
         <v>8.7822393613000003</v>
       </c>
-      <c r="Q6" s="19" t="s">
+      <c r="R6" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="R6" s="19" t="s">
+      <c r="S6" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="S6" s="19" t="s">
+      <c r="T6" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="T6" s="19" t="s">
+      <c r="U6" s="19" t="s">
         <v>215</v>
       </c>
-      <c r="U6" s="8"/>
-      <c r="W6" s="8">
+      <c r="V6" s="8"/>
+      <c r="X6" s="8">
         <v>22.501191319699998</v>
       </c>
-      <c r="Y6" s="8" t="s">
+      <c r="Z6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="AC6" s="8" t="s">
+      <c r="AD6" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="AF6" s="8"/>
-      <c r="AJ6" s="8" t="s">
+      <c r="AG6" s="8"/>
+      <c r="AK6" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:39">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B7" s="1">
@@ -2080,59 +2105,63 @@
         <v>31.2</v>
       </c>
       <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="J7" s="1">
         <v>2.9</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>250.2</v>
       </c>
-      <c r="K7" s="18">
+      <c r="L7" s="18">
         <v>99.688606539999995</v>
       </c>
-      <c r="L7" s="7">
+      <c r="M7" s="7">
         <v>9.75</v>
       </c>
-      <c r="M7" s="7">
+      <c r="N7" s="7">
         <v>9.5267881840000008</v>
       </c>
-      <c r="N7" s="8">
+      <c r="O7" s="8">
         <v>9.4468013662200008</v>
       </c>
-      <c r="O7" s="8">
+      <c r="P7" s="8">
         <v>32.889245552399998</v>
       </c>
-      <c r="P7" s="17">
+      <c r="Q7" s="17">
         <v>3.4877818652000001</v>
       </c>
-      <c r="Q7" s="19" t="s">
+      <c r="R7" s="19" t="s">
         <v>187</v>
       </c>
-      <c r="R7" s="19" t="s">
+      <c r="S7" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="S7" s="19" t="s">
+      <c r="T7" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="T7" s="19" t="s">
+      <c r="U7" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="U7" s="8"/>
-      <c r="W7" s="8">
+      <c r="V7" s="8"/>
+      <c r="X7" s="8">
         <v>20.177074323500001</v>
       </c>
-      <c r="Y7" s="8" t="s">
+      <c r="Z7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AD7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="AF7" s="8"/>
-      <c r="AJ7" s="8" t="s">
+      <c r="AG7" s="8"/>
+      <c r="AK7" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:39">
       <c r="A8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B8" s="4">
@@ -2156,60 +2185,64 @@
       <c r="H8" s="4">
         <v>30.3</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>0.90000000000000213</v>
+      </c>
+      <c r="J8" s="4">
         <v>1.6</v>
       </c>
-      <c r="J8" s="4">
+      <c r="K8" s="4">
         <v>253.1</v>
       </c>
-      <c r="K8" s="18">
+      <c r="L8" s="18">
         <v>113.2708459</v>
       </c>
-      <c r="L8" s="7">
+      <c r="M8" s="7">
         <v>9.9</v>
       </c>
-      <c r="M8" s="7">
+      <c r="N8" s="7">
         <v>9.6370043079999999</v>
       </c>
-      <c r="N8" s="8">
+      <c r="O8" s="8">
         <v>9.5920280747500009</v>
       </c>
-      <c r="O8" s="8">
+      <c r="P8" s="8">
         <v>31.448114325999999</v>
       </c>
-      <c r="P8" s="17">
+      <c r="Q8" s="17">
         <v>2.04684293113</v>
       </c>
-      <c r="Q8" s="19" t="s">
+      <c r="R8" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="R8" s="19" t="s">
+      <c r="S8" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="S8" s="19" t="s">
+      <c r="T8" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="T8" s="19" t="s">
+      <c r="U8" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="U8" s="8"/>
-      <c r="W8" s="8">
+      <c r="V8" s="8"/>
+      <c r="X8" s="8">
         <v>19.663378294299999</v>
       </c>
-      <c r="Y8" s="8" t="s">
+      <c r="Z8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AC8" s="8" t="s">
+      <c r="AD8" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="AF8" s="8"/>
-      <c r="AJ8" s="8" t="s">
+      <c r="AG8" s="8"/>
+      <c r="AK8" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:39">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B9" s="1">
@@ -2234,59 +2267,63 @@
         <v>34.299999999999997</v>
       </c>
       <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8999999999999986</v>
+      </c>
+      <c r="J9" s="1">
         <v>11.2</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <v>234.3</v>
       </c>
-      <c r="K9" s="18">
+      <c r="L9" s="18">
         <v>42.635408050000002</v>
       </c>
-      <c r="L9" s="7">
+      <c r="M9" s="7">
         <v>9.9</v>
       </c>
-      <c r="M9" s="7">
+      <c r="N9" s="7">
         <v>8.9167739380000004</v>
       </c>
-      <c r="N9" s="8">
+      <c r="O9" s="8">
         <v>9.2330228139399999</v>
       </c>
-      <c r="O9" s="8">
+      <c r="P9" s="8">
         <v>38.298985446800003</v>
       </c>
-      <c r="P9" s="17">
+      <c r="Q9" s="17">
         <v>8.89722508985</v>
       </c>
-      <c r="Q9" s="19" t="s">
+      <c r="R9" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="R9" s="19" t="s">
+      <c r="S9" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="S9" s="19" t="s">
+      <c r="T9" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="T9" s="19" t="s">
+      <c r="U9" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="U9" s="8"/>
-      <c r="W9" s="8">
+      <c r="V9" s="8"/>
+      <c r="X9" s="8">
         <v>19.855245389</v>
       </c>
-      <c r="Y9" s="8" t="s">
+      <c r="Z9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="AC9" s="8" t="s">
+      <c r="AD9" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="AF9" s="8"/>
-      <c r="AJ9" s="8" t="s">
+      <c r="AG9" s="8"/>
+      <c r="AK9" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:39">
       <c r="A10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B10" s="4">
@@ -2310,58 +2347,62 @@
       <c r="H10" s="4">
         <v>30.4</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="4">
         <v>2.4</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
         <v>257.8</v>
       </c>
-      <c r="K10" s="18">
+      <c r="L10" s="18">
         <v>41.286453629999997</v>
       </c>
-      <c r="L10" s="7">
+      <c r="M10" s="7">
         <v>10</v>
       </c>
-      <c r="M10" s="7">
+      <c r="N10" s="7">
         <v>9.8017882400000005</v>
       </c>
-      <c r="N10" s="8">
+      <c r="O10" s="8">
         <v>9.6931736170900002</v>
       </c>
-      <c r="O10" s="8">
+      <c r="P10" s="8">
         <v>32.618685882900003</v>
       </c>
-      <c r="P10" s="17">
+      <c r="Q10" s="17">
         <v>3.2171215737200001</v>
       </c>
-      <c r="Q10" s="19" t="s">
+      <c r="R10" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="R10" s="19" t="s">
+      <c r="S10" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="S10" s="19" t="s">
+      <c r="T10" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="T10" s="19" t="s">
+      <c r="U10" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="U10" s="8"/>
-      <c r="W10" s="8">
+      <c r="V10" s="8"/>
+      <c r="X10" s="8">
         <v>18.0854586574</v>
       </c>
-      <c r="Y10" s="8" t="s">
+      <c r="Z10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AC10" s="8" t="s">
+      <c r="AD10" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="AF10" s="8"/>
-      <c r="AJ10" s="8" t="s">
+      <c r="AG10" s="8"/>
+      <c r="AK10" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:39">
       <c r="A11" s="1">
         <f>A10+1</f>
         <v>9</v>
@@ -2388,59 +2429,63 @@
         <v>29.9</v>
       </c>
       <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="J11" s="1">
         <v>1.4</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <v>259.39999999999998</v>
       </c>
-      <c r="K11" s="18">
+      <c r="L11" s="18">
         <v>127.68255120000001</v>
       </c>
-      <c r="L11" s="7">
+      <c r="M11" s="7">
         <v>10</v>
       </c>
-      <c r="M11" s="7">
+      <c r="N11" s="7">
         <v>9.8729621600000002</v>
       </c>
-      <c r="N11" s="8">
+      <c r="O11" s="8">
         <v>9.8386747769599996</v>
       </c>
-      <c r="O11" s="8">
+      <c r="P11" s="8">
         <v>31.197889342300002</v>
       </c>
-      <c r="P11" s="17">
+      <c r="Q11" s="17">
         <v>1.79666832575</v>
       </c>
-      <c r="Q11" s="19" t="s">
+      <c r="R11" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="R11" s="19" t="s">
+      <c r="S11" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="S11" s="19" t="s">
+      <c r="T11" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="T11" s="19" t="s">
+      <c r="U11" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="U11" s="8"/>
-      <c r="W11" s="8">
+      <c r="V11" s="8"/>
+      <c r="X11" s="8">
         <v>17.754273489799999</v>
       </c>
-      <c r="Y11" s="8" t="s">
+      <c r="Z11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AC11" s="8" t="s">
+      <c r="AD11" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="AF11" s="8"/>
-      <c r="AJ11" s="8" t="s">
+      <c r="AG11" s="8"/>
+      <c r="AK11" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:39">
       <c r="A12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B12" s="4">
@@ -2464,1061 +2509,1117 @@
       <c r="H12" s="4">
         <v>40.6</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
+        <f t="shared" si="0"/>
+        <v>5.6000000000000014</v>
+      </c>
+      <c r="J12" s="4">
         <v>7.8</v>
       </c>
-      <c r="J12" s="4">
+      <c r="K12" s="4">
         <v>163.1</v>
       </c>
-      <c r="K12" s="18">
+      <c r="L12" s="18">
         <v>9.9332116609999996</v>
       </c>
-      <c r="L12" s="7">
+      <c r="M12" s="7">
         <v>7</v>
       </c>
-      <c r="M12" s="7">
+      <c r="N12" s="7">
         <v>6.2168311879999996</v>
       </c>
-      <c r="N12" s="8">
+      <c r="O12" s="8">
         <v>7.0496039637000001</v>
       </c>
-      <c r="O12" s="8">
+      <c r="P12" s="8">
         <v>40.9285437407</v>
       </c>
-      <c r="P12" s="17">
+      <c r="Q12" s="17">
         <v>5.9273643826600004</v>
       </c>
-      <c r="Q12" s="19" t="s">
+      <c r="R12" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="R12" s="19" t="s">
+      <c r="S12" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="S12" s="19" t="s">
+      <c r="T12" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="T12" s="19" t="s">
+      <c r="U12" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="U12" s="8"/>
-      <c r="W12" s="8">
+      <c r="V12" s="8"/>
+      <c r="X12" s="8">
         <v>28.177888376599999</v>
       </c>
-      <c r="Y12" s="8" t="s">
+      <c r="Z12" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AC12" s="8" t="s">
+      <c r="AD12" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="AF12" s="8"/>
-      <c r="AJ12" s="8" t="s">
+      <c r="AG12" s="8"/>
+      <c r="AK12" s="8" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:39">
       <c r="A13" s="1">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>119.4</v>
+      </c>
+      <c r="E13" s="1">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="H13" s="1">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7999999999999972</v>
+      </c>
+      <c r="J13" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="K13" s="1">
+        <v>198.2</v>
+      </c>
+      <c r="L13" s="18">
+        <v>-14.968205790000001</v>
+      </c>
+      <c r="M13" s="7">
+        <v>7.9</v>
+      </c>
+      <c r="N13" s="7">
+        <v>7.4978749960000002</v>
+      </c>
+      <c r="O13" s="8">
+        <v>8.3564408941699995</v>
+      </c>
+      <c r="P13" s="8">
+        <v>37.765944230499997</v>
+      </c>
+      <c r="Q13" s="17">
+        <v>2.7646593460500002</v>
+      </c>
+      <c r="R13" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="S13" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="T13" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="U13" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="V13" s="8"/>
+      <c r="X13" s="8">
+        <v>26.583976598300001</v>
+      </c>
+      <c r="Z13" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AD13" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG13" s="8"/>
+      <c r="AK13" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39">
+      <c r="A14" s="4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>35</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4">
+        <v>118.8</v>
+      </c>
+      <c r="E14" s="4">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G14" s="4">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="H14" s="4">
+        <v>37.9</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="0"/>
+        <v>2.8999999999999986</v>
+      </c>
+      <c r="J14" s="4">
+        <v>3.1</v>
+      </c>
+      <c r="K14" s="4">
+        <v>214.3</v>
+      </c>
+      <c r="L14" s="18">
+        <v>19.58268859</v>
+      </c>
+      <c r="M14" s="7">
+        <v>8.1</v>
+      </c>
+      <c r="N14" s="7">
+        <v>8.171220924</v>
+      </c>
+      <c r="O14" s="8">
+        <v>8.6641307019799996</v>
+      </c>
+      <c r="P14" s="8">
+        <v>36.667063314099998</v>
+      </c>
+      <c r="Q14" s="17">
+        <v>1.66595265329</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="S14" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="T14" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="U14" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="V14" s="8"/>
+      <c r="X14" s="8">
+        <v>25.972576892799999</v>
+      </c>
+      <c r="Z14" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD14" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AG14" s="8"/>
+      <c r="AK14" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39">
+      <c r="A15" s="1">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>127.7</v>
+      </c>
+      <c r="E15" s="1">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G15" s="1">
+        <v>45.5</v>
+      </c>
+      <c r="H15" s="1">
+        <v>41.9</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="0"/>
+        <v>6.8999999999999986</v>
+      </c>
+      <c r="J15" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="K15" s="1">
+        <v>191.8</v>
+      </c>
+      <c r="L15" s="18">
+        <v>-23.798967189999999</v>
+      </c>
+      <c r="M15" s="7">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="N15" s="7">
+        <v>7.25616532</v>
+      </c>
+      <c r="O15" s="8">
+        <v>8.1476187211800006</v>
+      </c>
+      <c r="P15" s="8">
+        <v>42.487170725600002</v>
+      </c>
+      <c r="Q15" s="17">
+        <v>7.4857122889500003</v>
+      </c>
+      <c r="R15" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="S15" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="T15" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="U15" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="V15" s="8"/>
+      <c r="X15" s="8">
+        <v>24.385722017999999</v>
+      </c>
+      <c r="Z15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD15" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG15" s="8"/>
+      <c r="AK15" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:39">
+      <c r="A16" s="4">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <v>35</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4">
+        <v>122.6</v>
+      </c>
+      <c r="E16" s="4">
+        <v>10</v>
+      </c>
+      <c r="F16" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G16" s="4">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="H16" s="4">
+        <v>37.9</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="0"/>
+        <v>2.8999999999999986</v>
+      </c>
+      <c r="J16" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="K16" s="4">
+        <v>230.3</v>
+      </c>
+      <c r="L16" s="18">
+        <v>1.7924288779999999</v>
+      </c>
+      <c r="M16" s="7">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="N16" s="7">
+        <v>8.7522152630000001</v>
+      </c>
+      <c r="O16" s="8">
+        <v>8.8779532591700008</v>
+      </c>
+      <c r="P16" s="8">
+        <v>38.031601374300003</v>
+      </c>
+      <c r="Q16" s="17">
+        <v>3.0302681926599999</v>
+      </c>
+      <c r="R16" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="S16" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="T16" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="U16" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="V16" s="8"/>
+      <c r="X16" s="8">
+        <v>22.313537268600001</v>
+      </c>
+      <c r="Z16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD16" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG16" s="8"/>
+      <c r="AK16" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37">
+      <c r="A17" s="1">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>122.2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G17" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H17" s="1">
+        <v>36.6</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6000000000000014</v>
+      </c>
+      <c r="J17" s="1">
+        <v>2</v>
+      </c>
+      <c r="K17" s="1">
+        <v>236.9</v>
+      </c>
+      <c r="L17" s="18">
+        <v>9.0231534589999995</v>
+      </c>
+      <c r="M17" s="7">
+        <v>9</v>
+      </c>
+      <c r="N17" s="7">
+        <v>9.0054255229999995</v>
+      </c>
+      <c r="O17" s="8">
+        <v>9.0770235013599994</v>
+      </c>
+      <c r="P17" s="8">
+        <v>36.780133411900003</v>
+      </c>
+      <c r="Q17" s="17">
+        <v>1.7790437461799999</v>
+      </c>
+      <c r="R17" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="S17" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="T17" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="U17" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="V17" s="8"/>
+      <c r="X17" s="8">
+        <v>21.8413634327</v>
+      </c>
+      <c r="Z17" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD17" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG17" s="8"/>
+      <c r="AK17" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37">
+      <c r="A18" s="4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>35</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4">
+        <v>133.30000000000001</v>
+      </c>
+      <c r="E18" s="4">
+        <v>11</v>
+      </c>
+      <c r="F18" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G18" s="4">
+        <v>46</v>
+      </c>
+      <c r="H18" s="4">
+        <v>40.9</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="0"/>
+        <v>5.8999999999999986</v>
+      </c>
+      <c r="J18" s="4">
+        <v>10.8</v>
+      </c>
+      <c r="K18" s="4">
+        <v>214.2</v>
+      </c>
+      <c r="L18" s="18">
+        <v>-12.02364169</v>
+      </c>
+      <c r="M18" s="7">
+        <v>9</v>
+      </c>
+      <c r="N18" s="7">
+        <v>8.1321077689999992</v>
+      </c>
+      <c r="O18" s="8">
+        <v>8.7033832451999995</v>
+      </c>
+      <c r="P18" s="8">
+        <v>43.057176394599999</v>
+      </c>
+      <c r="Q18" s="17">
+        <v>8.0555464684399993</v>
+      </c>
+      <c r="R18" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="S18" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="T18" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="U18" s="19" t="s">
+        <v>227</v>
+      </c>
+      <c r="V18" s="8"/>
+      <c r="X18" s="8">
+        <v>21.487278510700001</v>
+      </c>
+      <c r="Z18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AD18" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG18" s="8"/>
+      <c r="AK18" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37">
+      <c r="A19" s="1">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>35</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>128.9</v>
+      </c>
+      <c r="E19" s="1">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G19" s="1">
+        <v>38</v>
+      </c>
+      <c r="H19" s="1">
+        <v>36.6</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="0"/>
+        <v>1.6000000000000014</v>
+      </c>
+      <c r="J19" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="K19" s="1">
+        <v>244.2</v>
+      </c>
+      <c r="L19" s="18">
+        <v>6.0179755779999997</v>
+      </c>
+      <c r="M19" s="7">
+        <v>9.5</v>
+      </c>
+      <c r="N19" s="7">
+        <v>9.2810226670000002</v>
+      </c>
+      <c r="O19" s="8">
+        <v>9.2743858831299999</v>
+      </c>
+      <c r="P19" s="8">
+        <v>38.046641301599998</v>
+      </c>
+      <c r="Q19" s="17">
+        <v>3.0452302362500001</v>
+      </c>
+      <c r="R19" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="S19" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="T19" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="U19" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="V19" s="8"/>
+      <c r="X19" s="8">
+        <v>19.800386083999999</v>
+      </c>
+      <c r="Z19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD19" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG19" s="8"/>
+      <c r="AK19" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37">
+      <c r="A20" s="4">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>35</v>
+      </c>
+      <c r="C20" s="4">
+        <v>3</v>
+      </c>
+      <c r="D20" s="4">
+        <v>128.4</v>
+      </c>
+      <c r="E20" s="4">
+        <v>11</v>
+      </c>
+      <c r="F20" s="4">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="G20" s="4">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="H20" s="4">
+        <v>35.6</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="0"/>
+        <v>0.60000000000000142</v>
+      </c>
+      <c r="J20" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="K20" s="4">
+        <v>248.2</v>
+      </c>
+      <c r="L20" s="18">
+        <v>16.875317670000001</v>
+      </c>
+      <c r="M20" s="7">
+        <v>9.65</v>
+      </c>
+      <c r="N20" s="7">
+        <v>9.4350865689999992</v>
+      </c>
+      <c r="O20" s="8">
+        <v>9.4285119794799996</v>
+      </c>
+      <c r="P20" s="8">
+        <v>36.748522556099999</v>
+      </c>
+      <c r="Q20" s="17">
+        <v>1.74737487179</v>
+      </c>
+      <c r="R20" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="S20" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="T20" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="U20" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="V20" s="8"/>
+      <c r="X20" s="8">
+        <v>19.438277339399999</v>
+      </c>
+      <c r="Z20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD20" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG20" s="8"/>
+      <c r="AK20" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37">
+      <c r="A21" s="1">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>94.8</v>
+      </c>
+      <c r="E21" s="1">
+        <v>9</v>
+      </c>
+      <c r="F21" s="1">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G21" s="1">
+        <v>41.1</v>
+      </c>
+      <c r="H21" s="1">
+        <v>41.1</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="0"/>
+        <v>11.700000000000003</v>
+      </c>
+      <c r="J21" s="1">
+        <v>11.7</v>
+      </c>
+      <c r="K21" s="1">
+        <v>111.7</v>
+      </c>
+      <c r="L21" s="18">
+        <v>616.85745580000003</v>
+      </c>
+      <c r="M21" s="7">
+        <v>10</v>
+      </c>
+      <c r="N21" s="7">
+        <v>11.177502260000001</v>
+      </c>
+      <c r="O21" s="8">
+        <v>9.3406659813200008</v>
+      </c>
+      <c r="P21" s="8">
+        <v>43.658894520600001</v>
+      </c>
+      <c r="Q21" s="17">
+        <v>14.2572725804</v>
+      </c>
+      <c r="R21" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="S21" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="T21" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="U21" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="V21" s="8"/>
+      <c r="X21" s="8">
+        <v>92.263490076699995</v>
+      </c>
+      <c r="Z21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD21" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG21" s="8"/>
+      <c r="AK21" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="A22" s="4">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <v>29.4</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4">
+        <v>90.8</v>
+      </c>
+      <c r="E22" s="4">
+        <v>9</v>
+      </c>
+      <c r="F22" s="4">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G22" s="4">
+        <v>38.4</v>
+      </c>
+      <c r="H22" s="4">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="0"/>
+        <v>9.3999999999999986</v>
+      </c>
+      <c r="J22" s="4">
+        <v>8.9</v>
+      </c>
+      <c r="K22" s="4">
+        <v>149.19999999999999</v>
+      </c>
+      <c r="L22" s="18">
+        <v>389.26884050000001</v>
+      </c>
+      <c r="M22" s="7">
+        <v>11.7</v>
+      </c>
+      <c r="N22" s="7">
+        <v>13.219360229999999</v>
+      </c>
+      <c r="O22" s="8">
+        <v>12.9437558676</v>
+      </c>
+      <c r="P22" s="8">
+        <v>38.7385219214</v>
+      </c>
+      <c r="Q22" s="17">
+        <v>9.3366670980100004</v>
+      </c>
+      <c r="R22" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="S22" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="T22" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="U22" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="V22" s="8"/>
+      <c r="X22" s="8">
+        <v>83.743491851000002</v>
+      </c>
+      <c r="Z22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD22" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="AG22" s="8"/>
+      <c r="AK22" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
+      <c r="A23" s="1">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>86.9</v>
+      </c>
+      <c r="E23" s="1">
+        <v>9</v>
+      </c>
+      <c r="F23" s="1">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G23" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H23" s="1">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="0"/>
+        <v>8.3999999999999986</v>
+      </c>
+      <c r="J23" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="K23" s="1">
+        <v>166.4</v>
+      </c>
+      <c r="L23" s="18">
+        <v>333.93741590000002</v>
+      </c>
+      <c r="M23" s="7">
+        <v>12.5</v>
+      </c>
+      <c r="N23" s="7">
+        <v>13.59416671</v>
+      </c>
+      <c r="O23" s="8">
+        <v>14.2350662448</v>
+      </c>
+      <c r="P23" s="8">
+        <v>36.037707650800002</v>
+      </c>
+      <c r="Q23" s="17">
+        <v>6.6353539153899996</v>
+      </c>
+      <c r="R23" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="S23" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="T23" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="U23" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="V23" s="8"/>
+      <c r="X23" s="8">
+        <v>76.974449882800002</v>
+      </c>
+      <c r="Z23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD23" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG23" s="8"/>
+      <c r="AK23" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="A24" s="4">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="4">
+        <v>29.4</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4">
+        <v>103.3</v>
+      </c>
+      <c r="E24" s="4">
+        <v>10</v>
+      </c>
+      <c r="F24" s="4">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G24" s="4">
+        <v>45.8</v>
+      </c>
+      <c r="H24" s="4">
+        <v>44.9</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
+      <c r="J24" s="4">
+        <v>16.3</v>
+      </c>
+      <c r="K24" s="4">
+        <v>133.9</v>
+      </c>
+      <c r="L24" s="18">
+        <v>500.79838039999999</v>
+      </c>
+      <c r="M24" s="7">
+        <v>11.5</v>
+      </c>
+      <c r="N24" s="7">
+        <v>11.735591189999999</v>
+      </c>
+      <c r="O24" s="8">
+        <v>11.0366847651</v>
+      </c>
+      <c r="P24" s="8">
+        <v>46.979798993700001</v>
+      </c>
+      <c r="Q24" s="17">
+        <v>17.5781896913</v>
+      </c>
+      <c r="R24" s="19" t="s">
+        <v>202</v>
+      </c>
+      <c r="S24" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="T24" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="U24" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="V24" s="8"/>
+      <c r="X24" s="8">
+        <v>82.469053979799995</v>
+      </c>
+      <c r="Z24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD24" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="AG24" s="8"/>
+      <c r="AK24" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37">
+      <c r="A25" s="1">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>94.8</v>
+      </c>
+      <c r="E25" s="1">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G25" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>40.4</v>
+      </c>
+      <c r="I25" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="1">
-        <v>35</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1">
-        <v>119.4</v>
-      </c>
-      <c r="E13" s="1">
-        <v>9</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G13" s="1">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="H13" s="1">
-        <v>38.799999999999997</v>
-      </c>
-      <c r="I13" s="1">
-        <v>4.5</v>
-      </c>
-      <c r="J13" s="1">
-        <v>198.2</v>
-      </c>
-      <c r="K13" s="18">
-        <v>-14.968205790000001</v>
-      </c>
-      <c r="L13" s="7">
-        <v>7.9</v>
-      </c>
-      <c r="M13" s="7">
-        <v>7.4978749960000002</v>
-      </c>
-      <c r="N13" s="8">
-        <v>8.3564408941699995</v>
-      </c>
-      <c r="O13" s="8">
-        <v>37.765944230499997</v>
-      </c>
-      <c r="P13" s="17">
-        <v>2.7646593460500002</v>
-      </c>
-      <c r="Q13" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="R13" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="S13" s="19" t="s">
-        <v>252</v>
-      </c>
-      <c r="T13" s="19" t="s">
-        <v>222</v>
-      </c>
-      <c r="U13" s="8"/>
-      <c r="W13" s="8">
-        <v>26.583976598300001</v>
-      </c>
-      <c r="Y13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AC13" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="AF13" s="8"/>
-      <c r="AJ13" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:38">
-      <c r="A14" s="4">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B14" s="4">
-        <v>35</v>
-      </c>
-      <c r="C14" s="4">
-        <v>3</v>
-      </c>
-      <c r="D14" s="4">
-        <v>118.8</v>
-      </c>
-      <c r="E14" s="4">
-        <v>9</v>
-      </c>
-      <c r="F14" s="4">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G14" s="4">
-        <v>38.200000000000003</v>
-      </c>
-      <c r="H14" s="4">
-        <v>37.9</v>
-      </c>
-      <c r="I14" s="4">
-        <v>3.1</v>
-      </c>
-      <c r="J14" s="4">
-        <v>214.3</v>
-      </c>
-      <c r="K14" s="18">
-        <v>19.58268859</v>
-      </c>
-      <c r="L14" s="7">
-        <v>8.1</v>
-      </c>
-      <c r="M14" s="7">
-        <v>8.171220924</v>
-      </c>
-      <c r="N14" s="8">
-        <v>8.6641307019799996</v>
-      </c>
-      <c r="O14" s="8">
-        <v>36.667063314099998</v>
-      </c>
-      <c r="P14" s="17">
-        <v>1.66595265329</v>
-      </c>
-      <c r="Q14" s="19" t="s">
-        <v>194</v>
-      </c>
-      <c r="R14" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="S14" s="19" t="s">
-        <v>253</v>
-      </c>
-      <c r="T14" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="U14" s="8"/>
-      <c r="W14" s="8">
-        <v>25.972576892799999</v>
-      </c>
-      <c r="Y14" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC14" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF14" s="8"/>
-      <c r="AJ14" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:38">
-      <c r="A15" s="1">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B15" s="1">
-        <v>35</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>127.7</v>
-      </c>
-      <c r="E15" s="1">
+      <c r="J25" s="1">
         <v>10</v>
       </c>
-      <c r="F15" s="1">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G15" s="1">
-        <v>45.5</v>
-      </c>
-      <c r="H15" s="1">
-        <v>41.9</v>
-      </c>
-      <c r="I15" s="1">
-        <v>10.4</v>
-      </c>
-      <c r="J15" s="1">
-        <v>191.8</v>
-      </c>
-      <c r="K15" s="18">
-        <v>-23.798967189999999</v>
-      </c>
-      <c r="L15" s="7">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="M15" s="7">
-        <v>7.25616532</v>
-      </c>
-      <c r="N15" s="8">
-        <v>8.1476187211800006</v>
-      </c>
-      <c r="O15" s="8">
-        <v>42.487170725600002</v>
-      </c>
-      <c r="P15" s="17">
-        <v>7.4857122889500003</v>
-      </c>
-      <c r="Q15" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="R15" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="S15" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="T15" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="U15" s="8"/>
-      <c r="W15" s="8">
-        <v>24.385722017999999</v>
-      </c>
-      <c r="Y15" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC15" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF15" s="8"/>
-      <c r="AJ15" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:38">
-      <c r="A16" s="4">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B16" s="4">
-        <v>35</v>
-      </c>
-      <c r="C16" s="4">
-        <v>2</v>
-      </c>
-      <c r="D16" s="4">
-        <v>122.6</v>
-      </c>
-      <c r="E16" s="4">
-        <v>10</v>
-      </c>
-      <c r="F16" s="4">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G16" s="4">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="H16" s="4">
-        <v>37.9</v>
-      </c>
-      <c r="I16" s="4">
-        <v>3.6</v>
-      </c>
-      <c r="J16" s="4">
-        <v>230.3</v>
-      </c>
-      <c r="K16" s="18">
-        <v>1.7924288779999999</v>
-      </c>
-      <c r="L16" s="7">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="M16" s="7">
-        <v>8.7522152630000001</v>
-      </c>
-      <c r="N16" s="8">
-        <v>8.8779532591700008</v>
-      </c>
-      <c r="O16" s="8">
-        <v>38.031601374300003</v>
-      </c>
-      <c r="P16" s="17">
-        <v>3.0302681926599999</v>
-      </c>
-      <c r="Q16" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="R16" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="S16" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="T16" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="U16" s="8"/>
-      <c r="W16" s="8">
-        <v>22.313537268600001</v>
-      </c>
-      <c r="Y16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC16" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF16" s="8"/>
-      <c r="AJ16" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:36">
-      <c r="A17" s="1">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="1">
-        <v>35</v>
-      </c>
-      <c r="C17" s="1">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1">
-        <v>122.2</v>
-      </c>
-      <c r="E17" s="1">
-        <v>10</v>
-      </c>
-      <c r="F17" s="1">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G17" s="1">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="H17" s="1">
-        <v>36.6</v>
-      </c>
-      <c r="I17" s="1">
-        <v>2</v>
-      </c>
-      <c r="J17" s="1">
-        <v>236.9</v>
-      </c>
-      <c r="K17" s="18">
-        <v>9.0231534589999995</v>
-      </c>
-      <c r="L17" s="7">
-        <v>9</v>
-      </c>
-      <c r="M17" s="7">
-        <v>9.0054255229999995</v>
-      </c>
-      <c r="N17" s="8">
-        <v>9.0770235013599994</v>
-      </c>
-      <c r="O17" s="8">
-        <v>36.780133411900003</v>
-      </c>
-      <c r="P17" s="17">
-        <v>1.7790437461799999</v>
-      </c>
-      <c r="Q17" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="R17" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="S17" s="19" t="s">
-        <v>256</v>
-      </c>
-      <c r="T17" s="19" t="s">
-        <v>226</v>
-      </c>
-      <c r="U17" s="8"/>
-      <c r="W17" s="8">
-        <v>21.8413634327</v>
-      </c>
-      <c r="Y17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC17" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="AF17" s="8"/>
-      <c r="AJ17" s="8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:36">
-      <c r="A18" s="4">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B18" s="4">
-        <v>35</v>
-      </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="4">
-        <v>133.30000000000001</v>
-      </c>
-      <c r="E18" s="4">
-        <v>11</v>
-      </c>
-      <c r="F18" s="4">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G18" s="4">
-        <v>46</v>
-      </c>
-      <c r="H18" s="4">
-        <v>40.9</v>
-      </c>
-      <c r="I18" s="4">
-        <v>10.8</v>
-      </c>
-      <c r="J18" s="4">
-        <v>214.2</v>
-      </c>
-      <c r="K18" s="18">
-        <v>-12.02364169</v>
-      </c>
-      <c r="L18" s="7">
-        <v>9</v>
-      </c>
-      <c r="M18" s="7">
-        <v>8.1321077689999992</v>
-      </c>
-      <c r="N18" s="8">
-        <v>8.7033832451999995</v>
-      </c>
-      <c r="O18" s="8">
-        <v>43.057176394599999</v>
-      </c>
-      <c r="P18" s="17">
-        <v>8.0555464684399993</v>
-      </c>
-      <c r="Q18" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="R18" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="S18" s="19" t="s">
-        <v>257</v>
-      </c>
-      <c r="T18" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="U18" s="8"/>
-      <c r="W18" s="8">
-        <v>21.487278510700001</v>
-      </c>
-      <c r="Y18" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC18" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="AF18" s="8"/>
-      <c r="AJ18" s="8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="19" spans="1:36">
-      <c r="A19" s="1">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B19" s="1">
-        <v>35</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1">
-        <v>128.9</v>
-      </c>
-      <c r="E19" s="1">
-        <v>11</v>
-      </c>
-      <c r="F19" s="1">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G19" s="1">
-        <v>38</v>
-      </c>
-      <c r="H19" s="1">
-        <v>36.6</v>
-      </c>
-      <c r="I19" s="1">
-        <v>2.9</v>
-      </c>
-      <c r="J19" s="1">
-        <v>244.2</v>
-      </c>
-      <c r="K19" s="18">
-        <v>6.0179755779999997</v>
-      </c>
-      <c r="L19" s="7">
-        <v>9.5</v>
-      </c>
-      <c r="M19" s="7">
-        <v>9.2810226670000002</v>
-      </c>
-      <c r="N19" s="8">
-        <v>9.2743858831299999</v>
-      </c>
-      <c r="O19" s="8">
-        <v>38.046641301599998</v>
-      </c>
-      <c r="P19" s="17">
-        <v>3.0452302362500001</v>
-      </c>
-      <c r="Q19" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="R19" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="S19" s="19" t="s">
-        <v>258</v>
-      </c>
-      <c r="T19" s="19" t="s">
-        <v>228</v>
-      </c>
-      <c r="U19" s="8"/>
-      <c r="W19" s="8">
-        <v>19.800386083999999</v>
-      </c>
-      <c r="Y19" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC19" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF19" s="8"/>
-      <c r="AJ19" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:36">
-      <c r="A20" s="4">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B20" s="4">
-        <v>35</v>
-      </c>
-      <c r="C20" s="4">
-        <v>3</v>
-      </c>
-      <c r="D20" s="4">
-        <v>128.4</v>
-      </c>
-      <c r="E20" s="4">
-        <v>11</v>
-      </c>
-      <c r="F20" s="4">
-        <v>3.7999999999999999E-2</v>
-      </c>
-      <c r="G20" s="4">
-        <v>36.700000000000003</v>
-      </c>
-      <c r="H20" s="4">
-        <v>35.6</v>
-      </c>
-      <c r="I20" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="J20" s="4">
-        <v>248.2</v>
-      </c>
-      <c r="K20" s="18">
-        <v>16.875317670000001</v>
-      </c>
-      <c r="L20" s="7">
-        <v>9.65</v>
-      </c>
-      <c r="M20" s="7">
-        <v>9.4350865689999992</v>
-      </c>
-      <c r="N20" s="8">
-        <v>9.4285119794799996</v>
-      </c>
-      <c r="O20" s="8">
-        <v>36.748522556099999</v>
-      </c>
-      <c r="P20" s="17">
-        <v>1.74737487179</v>
-      </c>
-      <c r="Q20" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="R20" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="S20" s="19" t="s">
-        <v>259</v>
-      </c>
-      <c r="T20" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="U20" s="8"/>
-      <c r="W20" s="8">
-        <v>19.438277339399999</v>
-      </c>
-      <c r="Y20" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC20" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="AF20" s="8"/>
-      <c r="AJ20" s="8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:36">
-      <c r="A21" s="1">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B21" s="1">
-        <v>29.4</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
-        <v>94.8</v>
-      </c>
-      <c r="E21" s="1">
-        <v>9</v>
-      </c>
-      <c r="F21" s="1">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="G21" s="1">
-        <v>41.1</v>
-      </c>
-      <c r="H21" s="1">
-        <v>41.1</v>
-      </c>
-      <c r="I21" s="1">
-        <v>11.7</v>
-      </c>
-      <c r="J21" s="1">
-        <v>111.7</v>
-      </c>
-      <c r="K21" s="18">
-        <v>616.85745580000003</v>
-      </c>
-      <c r="L21" s="7">
-        <v>10</v>
-      </c>
-      <c r="M21" s="7">
-        <v>11.177502260000001</v>
-      </c>
-      <c r="N21" s="8">
-        <v>9.3406659813200008</v>
-      </c>
-      <c r="O21" s="8">
-        <v>43.658894520600001</v>
-      </c>
-      <c r="P21" s="17">
-        <v>14.2572725804</v>
-      </c>
-      <c r="Q21" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="R21" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="S21" s="19" t="s">
-        <v>260</v>
-      </c>
-      <c r="T21" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="U21" s="8"/>
-      <c r="W21" s="8">
-        <v>92.263490076699995</v>
-      </c>
-      <c r="Y21" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC21" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="AF21" s="8"/>
-      <c r="AJ21" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:36">
-      <c r="A22" s="4">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B22" s="4">
-        <v>29.4</v>
-      </c>
-      <c r="C22" s="4">
-        <v>2</v>
-      </c>
-      <c r="D22" s="4">
-        <v>90.8</v>
-      </c>
-      <c r="E22" s="4">
-        <v>9</v>
-      </c>
-      <c r="F22" s="4">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="G22" s="4">
-        <v>38.4</v>
-      </c>
-      <c r="H22" s="4">
-        <v>38.799999999999997</v>
-      </c>
-      <c r="I22" s="4">
-        <v>8.9</v>
-      </c>
-      <c r="J22" s="4">
-        <v>149.19999999999999</v>
-      </c>
-      <c r="K22" s="18">
-        <v>389.26884050000001</v>
-      </c>
-      <c r="L22" s="7">
-        <v>11.7</v>
-      </c>
-      <c r="M22" s="7">
-        <v>13.219360229999999</v>
-      </c>
-      <c r="N22" s="8">
-        <v>12.9437558676</v>
-      </c>
-      <c r="O22" s="8">
-        <v>38.7385219214</v>
-      </c>
-      <c r="P22" s="17">
-        <v>9.3366670980100004</v>
-      </c>
-      <c r="Q22" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="R22" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="S22" s="19" t="s">
-        <v>261</v>
-      </c>
-      <c r="T22" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="U22" s="8"/>
-      <c r="W22" s="8">
-        <v>83.743491851000002</v>
-      </c>
-      <c r="Y22" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC22" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="AF22" s="8"/>
-      <c r="AJ22" s="8" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:36">
-      <c r="A23" s="1">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B23" s="1">
-        <v>29.4</v>
-      </c>
-      <c r="C23" s="1">
-        <v>3</v>
-      </c>
-      <c r="D23" s="1">
-        <v>86.9</v>
-      </c>
-      <c r="E23" s="1">
-        <v>9</v>
-      </c>
-      <c r="F23" s="1">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="G23" s="1">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="H23" s="1">
-        <v>37.799999999999997</v>
-      </c>
-      <c r="I23" s="1">
-        <v>7.6</v>
-      </c>
-      <c r="J23" s="1">
-        <v>166.4</v>
-      </c>
-      <c r="K23" s="18">
-        <v>333.93741590000002</v>
-      </c>
-      <c r="L23" s="7">
-        <v>12.5</v>
-      </c>
-      <c r="M23" s="7">
-        <v>13.59416671</v>
-      </c>
-      <c r="N23" s="8">
-        <v>14.2350662448</v>
-      </c>
-      <c r="O23" s="8">
-        <v>36.037707650800002</v>
-      </c>
-      <c r="P23" s="17">
-        <v>6.6353539153899996</v>
-      </c>
-      <c r="Q23" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="R23" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="S23" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="T23" s="19" t="s">
-        <v>232</v>
-      </c>
-      <c r="U23" s="8"/>
-      <c r="W23" s="8">
-        <v>76.974449882800002</v>
-      </c>
-      <c r="Y23" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC23" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="AF23" s="8"/>
-      <c r="AJ23" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:36">
-      <c r="A24" s="4">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B24" s="4">
-        <v>29.4</v>
-      </c>
-      <c r="C24" s="4">
-        <v>1</v>
-      </c>
-      <c r="D24" s="4">
-        <v>103.3</v>
-      </c>
-      <c r="E24" s="4">
-        <v>10</v>
-      </c>
-      <c r="F24" s="4">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="G24" s="4">
-        <v>45.8</v>
-      </c>
-      <c r="H24" s="4">
-        <v>44.9</v>
-      </c>
-      <c r="I24" s="4">
-        <v>16.3</v>
-      </c>
-      <c r="J24" s="4">
-        <v>133.9</v>
-      </c>
-      <c r="K24" s="18">
-        <v>500.79838039999999</v>
-      </c>
-      <c r="L24" s="7">
-        <v>11.5</v>
-      </c>
-      <c r="M24" s="7">
-        <v>11.735591189999999</v>
-      </c>
-      <c r="N24" s="8">
-        <v>11.0366847651</v>
-      </c>
-      <c r="O24" s="8">
-        <v>46.979798993700001</v>
-      </c>
-      <c r="P24" s="17">
-        <v>17.5781896913</v>
-      </c>
-      <c r="Q24" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="R24" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="S24" s="19" t="s">
-        <v>263</v>
-      </c>
-      <c r="T24" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="U24" s="8"/>
-      <c r="W24" s="8">
-        <v>82.469053979799995</v>
-      </c>
-      <c r="Y24" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC24" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF24" s="8"/>
-      <c r="AJ24" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="25" spans="1:36">
-      <c r="A25" s="1">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B25" s="1">
-        <v>29.4</v>
-      </c>
-      <c r="C25" s="1">
-        <v>2</v>
-      </c>
-      <c r="D25" s="1">
-        <v>94.8</v>
-      </c>
-      <c r="E25" s="1">
-        <v>10</v>
-      </c>
-      <c r="F25" s="1">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="G25" s="1">
-        <v>39.1</v>
-      </c>
-      <c r="H25" s="1">
-        <v>40.4</v>
-      </c>
-      <c r="I25" s="1">
-        <v>10</v>
-      </c>
-      <c r="J25" s="1">
+      <c r="K25" s="1">
         <v>183.4</v>
       </c>
-      <c r="K25" s="18">
+      <c r="L25" s="18">
         <v>307.86436579999997</v>
       </c>
-      <c r="L25" s="7">
+      <c r="M25" s="7">
         <v>13.5</v>
       </c>
-      <c r="M25" s="7">
+      <c r="N25" s="7">
         <v>14.282737859999999</v>
       </c>
-      <c r="N25" s="8">
+      <c r="O25" s="8">
         <v>14.0376455414</v>
       </c>
-      <c r="O25" s="8">
+      <c r="P25" s="8">
         <v>39.6997978598</v>
       </c>
-      <c r="P25" s="17">
+      <c r="Q25" s="17">
         <v>10.297383476</v>
       </c>
-      <c r="Q25" s="19" t="s">
+      <c r="R25" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="R25" s="19" t="s">
+      <c r="S25" s="19" t="s">
         <v>175</v>
       </c>
-      <c r="S25" s="19" t="s">
+      <c r="T25" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="T25" s="19" t="s">
+      <c r="U25" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="U25" s="8"/>
-      <c r="W25" s="8">
+      <c r="V25" s="8"/>
+      <c r="X25" s="8">
         <v>70.329317754200005</v>
       </c>
-      <c r="Y25" s="8" t="s">
+      <c r="Z25" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="AC25" s="8" t="s">
+      <c r="AD25" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="AF25" s="8"/>
-      <c r="AJ25" s="8" t="s">
+      <c r="AG25" s="8"/>
+      <c r="AK25" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="26" spans="1:36">
+    <row r="26" spans="1:37">
       <c r="A26" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B26" s="4">
@@ -3542,60 +3643,64 @@
       <c r="H26" s="4">
         <v>37.5</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="3">
+        <f t="shared" si="0"/>
+        <v>8.1000000000000014</v>
+      </c>
+      <c r="J26" s="4">
         <v>5.9</v>
       </c>
-      <c r="J26" s="4">
+      <c r="K26" s="4">
         <v>196.2</v>
       </c>
-      <c r="K26" s="18">
+      <c r="L26" s="18">
         <v>325.14989100000003</v>
       </c>
-      <c r="L26" s="7">
+      <c r="M26" s="7">
         <v>14.2</v>
       </c>
-      <c r="M26" s="7">
+      <c r="N26" s="7">
         <v>15.104304369999999</v>
       </c>
-      <c r="N26" s="8">
+      <c r="O26" s="8">
         <v>14.8250921988</v>
       </c>
-      <c r="O26" s="8">
+      <c r="P26" s="8">
         <v>36.184008874900002</v>
       </c>
-      <c r="P26" s="17">
+      <c r="Q26" s="17">
         <v>6.7813029292999998</v>
       </c>
-      <c r="Q26" s="19" t="s">
+      <c r="R26" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="R26" s="19" t="s">
+      <c r="S26" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="S26" s="19" t="s">
+      <c r="T26" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="T26" s="19" t="s">
+      <c r="U26" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="U26" s="8"/>
-      <c r="W26" s="8">
+      <c r="V26" s="8"/>
+      <c r="X26" s="8">
         <v>64.409442321499995</v>
       </c>
-      <c r="Y26" s="8" t="s">
+      <c r="Z26" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="AC26" s="8" t="s">
+      <c r="AD26" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="AF26" s="8"/>
-      <c r="AJ26" s="8" t="s">
+      <c r="AG26" s="8"/>
+      <c r="AK26" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:36">
+    <row r="27" spans="1:37">
       <c r="A27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25</v>
       </c>
       <c r="B27" s="1">
@@ -3620,59 +3725,63 @@
         <v>47</v>
       </c>
       <c r="I27" s="1">
+        <f t="shared" si="0"/>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="J27" s="1">
         <v>19.8</v>
       </c>
-      <c r="J27" s="1">
+      <c r="K27" s="1">
         <v>152.9</v>
       </c>
-      <c r="K27" s="18">
+      <c r="L27" s="18">
         <v>368.6344077</v>
       </c>
-      <c r="L27" s="7">
+      <c r="M27" s="7">
         <v>13</v>
       </c>
-      <c r="M27" s="7">
+      <c r="N27" s="7">
         <v>12.34060298</v>
       </c>
-      <c r="N27" s="8">
+      <c r="O27" s="8">
         <v>12.329546318</v>
       </c>
-      <c r="O27" s="8">
+      <c r="P27" s="8">
         <v>49.323975191000002</v>
       </c>
-      <c r="P27" s="17">
+      <c r="Q27" s="17">
         <v>19.922119521900001</v>
       </c>
-      <c r="Q27" s="19" t="s">
+      <c r="R27" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="R27" s="19" t="s">
+      <c r="S27" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="S27" s="19" t="s">
+      <c r="T27" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="T27" s="19" t="s">
+      <c r="U27" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="U27" s="8"/>
-      <c r="W27" s="8">
+      <c r="V27" s="8"/>
+      <c r="X27" s="8">
         <v>74.378326171099999</v>
       </c>
-      <c r="Y27" s="8" t="s">
+      <c r="Z27" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AC27" s="8" t="s">
+      <c r="AD27" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="AF27" s="8"/>
-      <c r="AJ27" s="8" t="s">
+      <c r="AG27" s="8"/>
+      <c r="AK27" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:36">
+    <row r="28" spans="1:37">
       <c r="A28" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B28" s="4">
@@ -3696,60 +3805,64 @@
       <c r="H28" s="4">
         <v>39.5</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="3">
+        <f t="shared" si="0"/>
+        <v>10.100000000000001</v>
+      </c>
+      <c r="J28" s="4">
         <v>8.8000000000000007</v>
       </c>
-      <c r="J28" s="4">
+      <c r="K28" s="4">
         <v>198.8</v>
       </c>
-      <c r="K28" s="18">
+      <c r="L28" s="18">
         <v>309.148617</v>
       </c>
-      <c r="L28" s="7">
+      <c r="M28" s="7">
         <v>14.8</v>
       </c>
-      <c r="M28" s="7">
+      <c r="N28" s="7">
         <v>15.272513630000001</v>
       </c>
-      <c r="N28" s="8">
+      <c r="O28" s="8">
         <v>14.832398797</v>
       </c>
-      <c r="O28" s="8">
+      <c r="P28" s="8">
         <v>39.876106315400001</v>
       </c>
-      <c r="P28" s="17">
+      <c r="Q28" s="17">
         <v>10.4732345003</v>
       </c>
-      <c r="Q28" s="19" t="s">
+      <c r="R28" s="19" t="s">
         <v>207</v>
       </c>
-      <c r="R28" s="19" t="s">
+      <c r="S28" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="S28" s="19" t="s">
+      <c r="T28" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="T28" s="19" t="s">
+      <c r="U28" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="U28" s="8"/>
-      <c r="W28" s="8">
+      <c r="V28" s="8"/>
+      <c r="X28" s="8">
         <v>62.167764951000002</v>
       </c>
-      <c r="Y28" s="8" t="s">
+      <c r="Z28" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AC28" s="8" t="s">
+      <c r="AD28" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="AF28" s="8"/>
-      <c r="AJ28" s="8" t="s">
+      <c r="AG28" s="8"/>
+      <c r="AK28" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:36">
+    <row r="29" spans="1:37">
       <c r="A29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B29" s="1">
@@ -3774,59 +3887,63 @@
         <v>35.6</v>
       </c>
       <c r="I29" s="1">
+        <f t="shared" si="0"/>
+        <v>6.2000000000000028</v>
+      </c>
+      <c r="J29" s="1">
         <v>4.7</v>
       </c>
-      <c r="J29" s="1">
+      <c r="K29" s="1">
         <v>209.4</v>
       </c>
-      <c r="K29" s="18">
+      <c r="L29" s="18">
         <v>322.91958369999998</v>
       </c>
-      <c r="L29" s="7">
+      <c r="M29" s="7">
         <v>15.7</v>
       </c>
-      <c r="M29" s="7">
+      <c r="N29" s="7">
         <v>16.021434150000001</v>
       </c>
-      <c r="N29" s="8">
+      <c r="O29" s="8">
         <v>15.512902462</v>
       </c>
-      <c r="O29" s="8">
+      <c r="P29" s="8">
         <v>35.892675915399998</v>
       </c>
-      <c r="P29" s="17">
+      <c r="Q29" s="17">
         <v>6.4896415734200001</v>
       </c>
-      <c r="Q29" s="19" t="s">
+      <c r="R29" s="19" t="s">
         <v>208</v>
       </c>
-      <c r="R29" s="19" t="s">
+      <c r="S29" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="S29" s="19" t="s">
+      <c r="T29" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="T29" s="19" t="s">
+      <c r="U29" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="U29" s="8"/>
-      <c r="W29" s="8">
+      <c r="V29" s="8"/>
+      <c r="X29" s="8">
         <v>57.663619630100001</v>
       </c>
-      <c r="Y29" s="8" t="s">
+      <c r="Z29" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AC29" s="8" t="s">
+      <c r="AD29" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="AF29" s="8"/>
-      <c r="AJ29" s="8" t="s">
+      <c r="AG29" s="8"/>
+      <c r="AK29" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:36">
+    <row r="30" spans="1:37">
       <c r="A30" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="B30" s="4">
@@ -3850,60 +3967,64 @@
       <c r="H30" s="4">
         <v>43.3</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="3">
+        <f t="shared" si="0"/>
+        <v>8.2999999999999972</v>
+      </c>
+      <c r="J30" s="4">
         <v>8.6999999999999993</v>
       </c>
-      <c r="J30" s="4">
+      <c r="K30" s="4">
         <v>93</v>
       </c>
-      <c r="K30" s="18">
+      <c r="L30" s="18">
         <v>657.83283900000004</v>
       </c>
-      <c r="L30" s="7">
+      <c r="M30" s="7">
         <v>8</v>
       </c>
-      <c r="M30" s="7">
+      <c r="N30" s="7">
         <v>9.0038824539999993</v>
       </c>
-      <c r="N30" s="8">
+      <c r="O30" s="8">
         <v>7.7752160422700003</v>
       </c>
-      <c r="O30" s="8">
+      <c r="P30" s="8">
         <v>46.516168034400003</v>
       </c>
-      <c r="P30" s="17">
+      <c r="Q30" s="17">
         <v>11.5143277949</v>
       </c>
-      <c r="Q30" s="19" t="s">
+      <c r="R30" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="R30" s="19" t="s">
+      <c r="S30" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="S30" s="19" t="s">
+      <c r="T30" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="T30" s="19" t="s">
+      <c r="U30" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="U30" s="8"/>
-      <c r="W30" s="8">
+      <c r="V30" s="8"/>
+      <c r="X30" s="8">
         <v>94.004417167599996</v>
       </c>
-      <c r="Y30" s="8" t="s">
+      <c r="Z30" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="AC30" s="8" t="s">
+      <c r="AD30" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="AF30" s="8"/>
-      <c r="AJ30" s="8" t="s">
+      <c r="AG30" s="8"/>
+      <c r="AK30" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:36">
+    <row r="31" spans="1:37">
       <c r="A31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>29</v>
       </c>
       <c r="B31" s="1">
@@ -3928,59 +4049,63 @@
         <v>40.9</v>
       </c>
       <c r="I31" s="1">
+        <f t="shared" si="0"/>
+        <v>5.8999999999999986</v>
+      </c>
+      <c r="J31" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="J31" s="1">
+      <c r="K31" s="1">
         <v>117.8</v>
       </c>
-      <c r="K31" s="18">
+      <c r="L31" s="18">
         <v>488.48652629999998</v>
       </c>
-      <c r="L31" s="7">
+      <c r="M31" s="7">
         <v>9.5</v>
       </c>
-      <c r="M31" s="7">
+      <c r="N31" s="7">
         <v>11.48457443</v>
       </c>
-      <c r="N31" s="8">
+      <c r="O31" s="8">
         <v>10.2018576794</v>
       </c>
-      <c r="O31" s="8">
+      <c r="P31" s="8">
         <v>41.596327217000002</v>
       </c>
-      <c r="P31" s="17">
+      <c r="Q31" s="17">
         <v>6.5945521714200002</v>
       </c>
-      <c r="Q31" s="19" t="s">
+      <c r="R31" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="R31" s="19" t="s">
+      <c r="S31" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="S31" s="19" t="s">
+      <c r="T31" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="T31" s="19" t="s">
+      <c r="U31" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="U31" s="8"/>
-      <c r="W31" s="8">
+      <c r="V31" s="8"/>
+      <c r="X31" s="8">
         <v>87.786287356000003</v>
       </c>
-      <c r="Y31" s="8" t="s">
+      <c r="Z31" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="AC31" s="8" t="s">
+      <c r="AD31" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="AF31" s="8"/>
-      <c r="AJ31" s="8" t="s">
+      <c r="AG31" s="8"/>
+      <c r="AK31" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:36">
+    <row r="32" spans="1:37">
       <c r="A32" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="B32" s="4">
@@ -4004,60 +4129,64 @@
       <c r="H32" s="4">
         <v>40</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J32" s="4">
         <v>4.5</v>
       </c>
-      <c r="J32" s="4">
+      <c r="K32" s="4">
         <v>125.6</v>
       </c>
-      <c r="K32" s="18">
+      <c r="L32" s="18">
         <v>455.59057280000002</v>
       </c>
-      <c r="L32" s="7">
+      <c r="M32" s="7">
         <v>10</v>
       </c>
-      <c r="M32" s="7">
+      <c r="N32" s="7">
         <v>12.07212595</v>
       </c>
-      <c r="N32" s="8">
+      <c r="O32" s="8">
         <v>11.6451410943</v>
       </c>
-      <c r="O32" s="8">
+      <c r="P32" s="8">
         <v>39.844373985700003</v>
       </c>
-      <c r="P32" s="17">
+      <c r="Q32" s="17">
         <v>4.84253232966</v>
       </c>
-      <c r="Q32" s="19" t="s">
+      <c r="R32" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="R32" s="19" t="s">
+      <c r="S32" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="S32" s="19" t="s">
+      <c r="T32" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="T32" s="19" t="s">
+      <c r="U32" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="U32" s="8"/>
-      <c r="W32" s="8">
+      <c r="V32" s="8"/>
+      <c r="X32" s="8">
         <v>84.516840802700003</v>
       </c>
-      <c r="Y32" s="8" t="s">
+      <c r="Z32" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="AC32" s="8" t="s">
+      <c r="AD32" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="AF32" s="8"/>
-      <c r="AJ32" s="8" t="s">
+      <c r="AG32" s="8"/>
+      <c r="AK32" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:36">
+    <row r="33" spans="1:37">
       <c r="A33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
       <c r="B33" s="1">
@@ -4082,51 +4211,55 @@
         <v>47.2</v>
       </c>
       <c r="I33" s="1">
+        <f t="shared" si="0"/>
+        <v>12.200000000000003</v>
+      </c>
+      <c r="J33" s="1">
         <v>12.8</v>
       </c>
-      <c r="J33" s="1">
+      <c r="K33" s="1">
         <v>118.6</v>
       </c>
-      <c r="K33" s="18">
+      <c r="L33" s="18">
         <v>562.84992109999996</v>
       </c>
-      <c r="L33" s="7">
+      <c r="M33" s="7">
         <v>10.199999999999999</v>
       </c>
-      <c r="M33" s="7">
+      <c r="N33" s="7">
         <v>10.56273097</v>
       </c>
-      <c r="N33" s="8">
+      <c r="O33" s="8">
         <v>9.6744266823499991</v>
       </c>
-      <c r="O33" s="8">
+      <c r="P33" s="8">
         <v>49.816837546800002</v>
       </c>
-      <c r="P33" s="17">
+      <c r="Q33" s="17">
         <v>14.814999884200001</v>
       </c>
-      <c r="Q33" s="17"/>
       <c r="R33" s="17"/>
       <c r="S33" s="17"/>
       <c r="T33" s="17"/>
-      <c r="U33" s="8"/>
-      <c r="W33" s="8">
+      <c r="U33" s="17"/>
+      <c r="V33" s="8"/>
+      <c r="X33" s="8">
         <v>85.446263963000007</v>
       </c>
-      <c r="Y33" s="8" t="s">
+      <c r="Z33" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AC33" s="8" t="s">
+      <c r="AD33" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="AF33" s="8"/>
-      <c r="AJ33" s="8" t="s">
+      <c r="AG33" s="8"/>
+      <c r="AK33" s="8" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:36">
+    <row r="34" spans="1:37">
       <c r="A34" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="B34" s="4">
@@ -4150,52 +4283,56 @@
       <c r="H34" s="4">
         <v>43.6</v>
       </c>
-      <c r="I34" s="4">
+      <c r="I34" s="3">
+        <f t="shared" si="0"/>
+        <v>8.6000000000000014</v>
+      </c>
+      <c r="J34" s="4">
         <v>8.3000000000000007</v>
       </c>
-      <c r="J34" s="4">
+      <c r="K34" s="4">
         <v>155.9</v>
       </c>
-      <c r="K34" s="18">
+      <c r="L34" s="18">
         <v>301.93401970000002</v>
       </c>
-      <c r="L34" s="7">
+      <c r="M34" s="7">
         <v>12</v>
       </c>
-      <c r="M34" s="7">
+      <c r="N34" s="7">
         <v>12.62581915</v>
       </c>
-      <c r="N34" s="8">
+      <c r="O34" s="8">
         <v>12.5151756476</v>
       </c>
-      <c r="O34" s="8">
+      <c r="P34" s="8">
         <v>43.589375310000001</v>
       </c>
-      <c r="P34" s="17">
+      <c r="Q34" s="17">
         <v>8.5872050156699995</v>
       </c>
-      <c r="Q34" s="17"/>
       <c r="R34" s="17"/>
       <c r="S34" s="17"/>
       <c r="T34" s="17"/>
-      <c r="U34" s="8"/>
-      <c r="W34" s="8">
+      <c r="U34" s="17"/>
+      <c r="V34" s="8"/>
+      <c r="X34" s="8">
         <v>76.711988744400003</v>
       </c>
-      <c r="Y34" s="8" t="s">
+      <c r="Z34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AC34" s="8" t="s">
+      <c r="AD34" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="AF34" s="8"/>
-      <c r="AJ34" s="8" t="s">
+      <c r="AG34" s="8"/>
+      <c r="AK34" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:36">
+    <row r="35" spans="1:37">
       <c r="A35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>33</v>
       </c>
       <c r="B35" s="1">
@@ -4220,51 +4357,55 @@
         <v>42</v>
       </c>
       <c r="I35" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J35" s="1">
         <v>6.1</v>
       </c>
-      <c r="J35" s="1">
+      <c r="K35" s="1">
         <v>168.9</v>
       </c>
-      <c r="K35" s="18">
+      <c r="L35" s="18">
         <v>283.60288500000001</v>
       </c>
-      <c r="L35" s="7">
+      <c r="M35" s="7">
         <v>12.5</v>
       </c>
-      <c r="M35" s="7">
+      <c r="N35" s="7">
         <v>13.304688799999999</v>
       </c>
-      <c r="N35" s="8">
+      <c r="O35" s="8">
         <v>13.431470279299999</v>
       </c>
-      <c r="O35" s="8">
+      <c r="P35" s="8">
         <v>40.829516938200001</v>
       </c>
-      <c r="P35" s="17">
+      <c r="Q35" s="17">
         <v>5.8271606420099999</v>
       </c>
-      <c r="Q35" s="17"/>
       <c r="R35" s="17"/>
       <c r="S35" s="17"/>
       <c r="T35" s="17"/>
-      <c r="U35" s="8"/>
-      <c r="W35" s="8">
+      <c r="U35" s="17"/>
+      <c r="V35" s="8"/>
+      <c r="X35" s="8">
         <v>71.3838109231</v>
       </c>
-      <c r="Y35" s="8" t="s">
+      <c r="Z35" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AC35" s="8" t="s">
+      <c r="AD35" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="AF35" s="8"/>
-      <c r="AJ35" s="8" t="s">
+      <c r="AG35" s="8"/>
+      <c r="AK35" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:36">
+    <row r="36" spans="1:37">
       <c r="A36" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="B36" s="4">
@@ -4288,52 +4429,56 @@
       <c r="H36" s="4">
         <v>49.7</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="3">
+        <f t="shared" si="0"/>
+        <v>14.700000000000003</v>
+      </c>
+      <c r="J36" s="4">
         <v>16.399999999999999</v>
       </c>
-      <c r="J36" s="4">
+      <c r="K36" s="4">
         <v>134.9</v>
       </c>
-      <c r="K36" s="18">
+      <c r="L36" s="18">
         <v>460.27402790000002</v>
       </c>
-      <c r="L36" s="7">
+      <c r="M36" s="7">
         <v>11.5</v>
       </c>
-      <c r="M36" s="7">
+      <c r="N36" s="7">
         <v>11.21689995</v>
       </c>
-      <c r="N36" s="8">
+      <c r="O36" s="8">
         <v>10.8671689562</v>
       </c>
-      <c r="O36" s="8">
+      <c r="P36" s="8">
         <v>52.285627960399999</v>
       </c>
-      <c r="P36" s="17">
+      <c r="Q36" s="17">
         <v>17.283810483100002</v>
       </c>
-      <c r="Q36" s="17"/>
       <c r="R36" s="17"/>
       <c r="S36" s="17"/>
       <c r="T36" s="17"/>
-      <c r="U36" s="8"/>
-      <c r="W36" s="8">
+      <c r="U36" s="17"/>
+      <c r="V36" s="8"/>
+      <c r="X36" s="8">
         <v>76.587639324199998</v>
       </c>
-      <c r="Y36" s="8" t="s">
+      <c r="Z36" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AC36" s="8" t="s">
+      <c r="AD36" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="AF36" s="8"/>
-      <c r="AJ36" s="8" t="s">
+      <c r="AG36" s="8"/>
+      <c r="AK36" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:36">
+    <row r="37" spans="1:37">
       <c r="A37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="B37" s="1">
@@ -4358,51 +4503,55 @@
         <v>44.3</v>
       </c>
       <c r="I37" s="1">
+        <f t="shared" si="0"/>
+        <v>9.2999999999999972</v>
+      </c>
+      <c r="J37" s="1">
         <v>8.6</v>
       </c>
-      <c r="J37" s="1">
+      <c r="K37" s="1">
         <v>177.5</v>
       </c>
-      <c r="K37" s="18">
+      <c r="L37" s="18">
         <v>233.60337430000001</v>
       </c>
-      <c r="L37" s="7">
+      <c r="M37" s="7">
         <v>13.5</v>
       </c>
-      <c r="M37" s="7">
+      <c r="N37" s="7">
         <v>13.723713310000001</v>
       </c>
-      <c r="N37" s="8">
+      <c r="O37" s="8">
         <v>13.4397995098</v>
       </c>
-      <c r="O37" s="8">
+      <c r="P37" s="8">
         <v>44.352922091700002</v>
       </c>
-      <c r="P37" s="17">
+      <c r="Q37" s="17">
         <v>9.3504251887700001</v>
       </c>
-      <c r="Q37" s="17"/>
       <c r="R37" s="17"/>
       <c r="S37" s="17"/>
       <c r="T37" s="17"/>
-      <c r="U37" s="8"/>
-      <c r="W37" s="8">
+      <c r="U37" s="17"/>
+      <c r="V37" s="8"/>
+      <c r="X37" s="8">
         <v>66.667788394699997</v>
       </c>
-      <c r="Y37" s="8" t="s">
+      <c r="Z37" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AC37" s="8" t="s">
+      <c r="AD37" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="AF37" s="8"/>
-      <c r="AJ37" s="8" t="s">
+      <c r="AG37" s="8"/>
+      <c r="AK37" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:36">
+    <row r="38" spans="1:37">
       <c r="A38" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="B38" s="4">
@@ -4426,319 +4575,323 @@
       <c r="H38" s="4">
         <v>41.6</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="3">
+        <f t="shared" si="0"/>
+        <v>6.6000000000000014</v>
+      </c>
+      <c r="J38" s="4">
         <v>5.2</v>
       </c>
-      <c r="J38" s="4">
+      <c r="K38" s="4">
         <v>186.6</v>
       </c>
-      <c r="K38" s="18">
+      <c r="L38" s="18">
         <v>252.55478189999999</v>
       </c>
-      <c r="L38" s="7">
+      <c r="M38" s="7">
         <v>14</v>
       </c>
-      <c r="M38" s="7">
+      <c r="N38" s="7">
         <v>14.35144721</v>
       </c>
-      <c r="N38" s="8">
+      <c r="O38" s="8">
         <v>14.1935320248</v>
       </c>
-      <c r="O38" s="8">
+      <c r="P38" s="8">
         <v>40.9925610855</v>
       </c>
-      <c r="P38" s="17">
+      <c r="Q38" s="17">
         <v>5.9899077289599996</v>
       </c>
-      <c r="Q38" s="17"/>
       <c r="R38" s="17"/>
       <c r="S38" s="17"/>
       <c r="T38" s="17"/>
-      <c r="U38" s="8"/>
-      <c r="W38" s="8">
+      <c r="U38" s="17"/>
+      <c r="V38" s="8"/>
+      <c r="X38" s="8">
         <v>62.315840030499999</v>
       </c>
-      <c r="Y38" s="8" t="s">
+      <c r="Z38" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AC38" s="8" t="s">
+      <c r="AD38" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="AF38" s="8"/>
-      <c r="AJ38" s="8" t="s">
+      <c r="AG38" s="8"/>
+      <c r="AK38" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="1:36">
-      <c r="J39" s="8"/>
-      <c r="M39" s="8"/>
-    </row>
-    <row r="40" spans="1:36">
-      <c r="M40" s="8"/>
-      <c r="O40" s="8"/>
+    <row r="39" spans="1:37">
+      <c r="K39" s="8"/>
+      <c r="N39" s="8"/>
+    </row>
+    <row r="40" spans="1:37">
+      <c r="N40" s="8"/>
       <c r="P40" s="8"/>
       <c r="Q40" s="8"/>
       <c r="R40" s="8"/>
       <c r="S40" s="8"/>
       <c r="T40" s="8"/>
-    </row>
-    <row r="41" spans="1:36">
-      <c r="M41" s="8"/>
-      <c r="O41" s="8"/>
+      <c r="U40" s="8"/>
+    </row>
+    <row r="41" spans="1:37">
+      <c r="N41" s="8"/>
       <c r="P41" s="8"/>
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
       <c r="S41" s="8"/>
       <c r="T41" s="8"/>
-      <c r="W41" s="8"/>
-    </row>
-    <row r="42" spans="1:36">
-      <c r="M42" s="8"/>
-      <c r="P42" s="7"/>
+      <c r="U41" s="8"/>
+      <c r="X41" s="8"/>
+    </row>
+    <row r="42" spans="1:37">
+      <c r="N42" s="8"/>
       <c r="Q42" s="7"/>
       <c r="R42" s="7"/>
       <c r="S42" s="7"/>
       <c r="T42" s="7"/>
-    </row>
-    <row r="43" spans="1:36">
-      <c r="M43" s="8"/>
-      <c r="P43" s="7"/>
+      <c r="U42" s="7"/>
+    </row>
+    <row r="43" spans="1:37">
+      <c r="N43" s="8"/>
       <c r="Q43" s="7"/>
       <c r="R43" s="7"/>
       <c r="S43" s="7"/>
       <c r="T43" s="7"/>
-    </row>
-    <row r="44" spans="1:36">
-      <c r="M44" s="8"/>
-      <c r="P44" s="7"/>
+      <c r="U43" s="7"/>
+    </row>
+    <row r="44" spans="1:37">
+      <c r="N44" s="8"/>
       <c r="Q44" s="7"/>
       <c r="R44" s="7"/>
       <c r="S44" s="7"/>
       <c r="T44" s="7"/>
-    </row>
-    <row r="45" spans="1:36">
-      <c r="P45" s="7"/>
+      <c r="U44" s="7"/>
+    </row>
+    <row r="45" spans="1:37">
       <c r="Q45" s="7"/>
       <c r="R45" s="7"/>
       <c r="S45" s="7"/>
       <c r="T45" s="7"/>
-    </row>
-    <row r="46" spans="1:36">
-      <c r="P46" s="7"/>
+      <c r="U45" s="7"/>
+    </row>
+    <row r="46" spans="1:37">
       <c r="Q46" s="7"/>
       <c r="R46" s="7"/>
       <c r="S46" s="7"/>
       <c r="T46" s="7"/>
-    </row>
-    <row r="47" spans="1:36">
-      <c r="P47" s="7"/>
+      <c r="U46" s="7"/>
+    </row>
+    <row r="47" spans="1:37">
       <c r="Q47" s="7"/>
       <c r="R47" s="7"/>
       <c r="S47" s="7"/>
       <c r="T47" s="7"/>
-    </row>
-    <row r="48" spans="1:36">
-      <c r="P48" s="7"/>
+      <c r="U47" s="7"/>
+    </row>
+    <row r="48" spans="1:37">
       <c r="Q48" s="7"/>
       <c r="R48" s="7"/>
       <c r="S48" s="7"/>
       <c r="T48" s="7"/>
-    </row>
-    <row r="49" spans="16:20">
-      <c r="P49" s="7"/>
+      <c r="U48" s="7"/>
+    </row>
+    <row r="49" spans="17:21">
       <c r="Q49" s="7"/>
       <c r="R49" s="7"/>
       <c r="S49" s="7"/>
       <c r="T49" s="7"/>
-    </row>
-    <row r="50" spans="16:20">
-      <c r="P50" s="7"/>
+      <c r="U49" s="7"/>
+    </row>
+    <row r="50" spans="17:21">
       <c r="Q50" s="7"/>
       <c r="R50" s="7"/>
       <c r="S50" s="7"/>
       <c r="T50" s="7"/>
-    </row>
-    <row r="51" spans="16:20">
-      <c r="P51" s="7"/>
+      <c r="U50" s="7"/>
+    </row>
+    <row r="51" spans="17:21">
       <c r="Q51" s="7"/>
       <c r="R51" s="7"/>
       <c r="S51" s="7"/>
       <c r="T51" s="7"/>
-    </row>
-    <row r="52" spans="16:20">
-      <c r="P52" s="7"/>
+      <c r="U51" s="7"/>
+    </row>
+    <row r="52" spans="17:21">
       <c r="Q52" s="7"/>
       <c r="R52" s="7"/>
       <c r="S52" s="7"/>
       <c r="T52" s="7"/>
-    </row>
-    <row r="53" spans="16:20">
-      <c r="P53" s="7"/>
+      <c r="U52" s="7"/>
+    </row>
+    <row r="53" spans="17:21">
       <c r="Q53" s="7"/>
       <c r="R53" s="7"/>
       <c r="S53" s="7"/>
       <c r="T53" s="7"/>
-    </row>
-    <row r="54" spans="16:20">
-      <c r="P54" s="7"/>
+      <c r="U53" s="7"/>
+    </row>
+    <row r="54" spans="17:21">
       <c r="Q54" s="7"/>
       <c r="R54" s="7"/>
       <c r="S54" s="7"/>
       <c r="T54" s="7"/>
-    </row>
-    <row r="55" spans="16:20">
-      <c r="P55" s="7"/>
+      <c r="U54" s="7"/>
+    </row>
+    <row r="55" spans="17:21">
       <c r="Q55" s="7"/>
       <c r="R55" s="7"/>
       <c r="S55" s="7"/>
       <c r="T55" s="7"/>
-    </row>
-    <row r="56" spans="16:20">
-      <c r="P56" s="7"/>
+      <c r="U55" s="7"/>
+    </row>
+    <row r="56" spans="17:21">
       <c r="Q56" s="7"/>
       <c r="R56" s="7"/>
       <c r="S56" s="7"/>
       <c r="T56" s="7"/>
-    </row>
-    <row r="57" spans="16:20">
-      <c r="P57" s="7"/>
+      <c r="U56" s="7"/>
+    </row>
+    <row r="57" spans="17:21">
       <c r="Q57" s="7"/>
       <c r="R57" s="7"/>
       <c r="S57" s="7"/>
       <c r="T57" s="7"/>
-    </row>
-    <row r="58" spans="16:20">
-      <c r="P58" s="7"/>
+      <c r="U57" s="7"/>
+    </row>
+    <row r="58" spans="17:21">
       <c r="Q58" s="7"/>
       <c r="R58" s="7"/>
       <c r="S58" s="7"/>
       <c r="T58" s="7"/>
-    </row>
-    <row r="59" spans="16:20">
-      <c r="P59" s="8"/>
+      <c r="U58" s="7"/>
+    </row>
+    <row r="59" spans="17:21">
       <c r="Q59" s="8"/>
       <c r="R59" s="8"/>
       <c r="S59" s="8"/>
       <c r="T59" s="8"/>
-    </row>
-    <row r="60" spans="16:20">
-      <c r="P60" s="8"/>
+      <c r="U59" s="8"/>
+    </row>
+    <row r="60" spans="17:21">
       <c r="Q60" s="8"/>
       <c r="R60" s="8"/>
       <c r="S60" s="8"/>
       <c r="T60" s="8"/>
-    </row>
-    <row r="61" spans="16:20">
-      <c r="P61" s="8"/>
+      <c r="U60" s="8"/>
+    </row>
+    <row r="61" spans="17:21">
       <c r="Q61" s="8"/>
       <c r="R61" s="8"/>
       <c r="S61" s="8"/>
       <c r="T61" s="8"/>
-    </row>
-    <row r="62" spans="16:20">
-      <c r="P62" s="8"/>
+      <c r="U61" s="8"/>
+    </row>
+    <row r="62" spans="17:21">
       <c r="Q62" s="8"/>
       <c r="R62" s="8"/>
       <c r="S62" s="8"/>
       <c r="T62" s="8"/>
-    </row>
-    <row r="63" spans="16:20">
-      <c r="P63" s="8"/>
+      <c r="U62" s="8"/>
+    </row>
+    <row r="63" spans="17:21">
       <c r="Q63" s="8"/>
       <c r="R63" s="8"/>
       <c r="S63" s="8"/>
       <c r="T63" s="8"/>
-    </row>
-    <row r="64" spans="16:20">
-      <c r="P64" s="8"/>
+      <c r="U63" s="8"/>
+    </row>
+    <row r="64" spans="17:21">
       <c r="Q64" s="8"/>
       <c r="R64" s="8"/>
       <c r="S64" s="8"/>
       <c r="T64" s="8"/>
-    </row>
-    <row r="65" spans="16:20">
-      <c r="P65" s="8"/>
+      <c r="U64" s="8"/>
+    </row>
+    <row r="65" spans="17:21">
       <c r="Q65" s="8"/>
       <c r="R65" s="8"/>
       <c r="S65" s="8"/>
       <c r="T65" s="8"/>
-    </row>
-    <row r="66" spans="16:20">
-      <c r="P66" s="8"/>
+      <c r="U65" s="8"/>
+    </row>
+    <row r="66" spans="17:21">
       <c r="Q66" s="8"/>
       <c r="R66" s="8"/>
       <c r="S66" s="8"/>
       <c r="T66" s="8"/>
-    </row>
-    <row r="67" spans="16:20">
-      <c r="P67" s="8"/>
+      <c r="U66" s="8"/>
+    </row>
+    <row r="67" spans="17:21">
       <c r="Q67" s="8"/>
       <c r="R67" s="8"/>
       <c r="S67" s="8"/>
       <c r="T67" s="8"/>
-    </row>
-    <row r="68" spans="16:20">
-      <c r="P68" s="8"/>
+      <c r="U67" s="8"/>
+    </row>
+    <row r="68" spans="17:21">
       <c r="Q68" s="8"/>
       <c r="R68" s="8"/>
       <c r="S68" s="8"/>
       <c r="T68" s="8"/>
-    </row>
-    <row r="69" spans="16:20">
-      <c r="P69" s="8"/>
+      <c r="U68" s="8"/>
+    </row>
+    <row r="69" spans="17:21">
       <c r="Q69" s="8"/>
       <c r="R69" s="8"/>
       <c r="S69" s="8"/>
       <c r="T69" s="8"/>
-    </row>
-    <row r="70" spans="16:20">
-      <c r="P70" s="8"/>
+      <c r="U69" s="8"/>
+    </row>
+    <row r="70" spans="17:21">
       <c r="Q70" s="8"/>
       <c r="R70" s="8"/>
       <c r="S70" s="8"/>
       <c r="T70" s="8"/>
-    </row>
-    <row r="71" spans="16:20">
-      <c r="P71" s="8"/>
+      <c r="U70" s="8"/>
+    </row>
+    <row r="71" spans="17:21">
       <c r="Q71" s="8"/>
       <c r="R71" s="8"/>
       <c r="S71" s="8"/>
       <c r="T71" s="8"/>
-    </row>
-    <row r="72" spans="16:20">
-      <c r="P72" s="8"/>
+      <c r="U71" s="8"/>
+    </row>
+    <row r="72" spans="17:21">
       <c r="Q72" s="8"/>
       <c r="R72" s="8"/>
       <c r="S72" s="8"/>
       <c r="T72" s="8"/>
-    </row>
-    <row r="73" spans="16:20">
-      <c r="P73" s="8"/>
+      <c r="U72" s="8"/>
+    </row>
+    <row r="73" spans="17:21">
       <c r="Q73" s="8"/>
       <c r="R73" s="8"/>
       <c r="S73" s="8"/>
       <c r="T73" s="8"/>
-    </row>
-    <row r="74" spans="16:20">
-      <c r="P74" s="8"/>
+      <c r="U73" s="8"/>
+    </row>
+    <row r="74" spans="17:21">
       <c r="Q74" s="8"/>
       <c r="R74" s="8"/>
       <c r="S74" s="8"/>
       <c r="T74" s="8"/>
-    </row>
-    <row r="75" spans="16:20">
-      <c r="P75" s="8"/>
+      <c r="U74" s="8"/>
+    </row>
+    <row r="75" spans="17:21">
       <c r="Q75" s="8"/>
       <c r="R75" s="8"/>
       <c r="S75" s="8"/>
       <c r="T75" s="8"/>
-    </row>
-    <row r="76" spans="16:20">
-      <c r="P76" s="8"/>
+      <c r="U75" s="8"/>
+    </row>
+    <row r="76" spans="17:21">
       <c r="Q76" s="8"/>
       <c r="R76" s="8"/>
       <c r="S76" s="8"/>
       <c r="T76" s="8"/>
+      <c r="U76" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
update gas cooler model
</commit_message>
<xml_diff>
--- a/ComponentTests/supercritical/Table.xlsx
+++ b/ComponentTests/supercritical/Table.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ammarbahman/Desktop/ACHP/ComponentTests/supercritical/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63892010-0BCB-C240-AB0C-038F553D84A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5748FB8-7203-4543-9E30-5B9162D2A2BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="284">
   <si>
     <t>Test Conditions</t>
   </si>
@@ -856,14 +857,48 @@
   </si>
   <si>
     <t>Simulated Approach Temp</t>
+  </si>
+  <si>
+    <t>T_a,in</t>
+  </si>
+  <si>
+    <t>v_a</t>
+  </si>
+  <si>
+    <t>T_r,in</t>
+  </si>
+  <si>
+    <t>P_r,in</t>
+  </si>
+  <si>
+    <t>m_dot_r</t>
+  </si>
+  <si>
+    <t>T_r,out,exp</t>
+  </si>
+  <si>
+    <t>T_r,out,pred</t>
+  </si>
+  <si>
+    <t>T_approach_pred</t>
+  </si>
+  <si>
+    <t>T_approach_exp</t>
+  </si>
+  <si>
+    <t>Q_pred</t>
+  </si>
+  <si>
+    <t>g/s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -1087,7 +1122,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1122,6 +1157,10 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="67">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1529,8 +1568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3:Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4900,6 +4939,1513 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4180CF52-6670-F446-A913-A1A46665670D}">
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>118.1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1">
+        <v>38</v>
+      </c>
+      <c r="G3" s="1">
+        <v>40.4</v>
+      </c>
+      <c r="H3" s="22">
+        <v>37.598140358199998</v>
+      </c>
+      <c r="I3" s="1">
+        <v>10.7</v>
+      </c>
+      <c r="J3" s="22">
+        <v>8.1967583050799995</v>
+      </c>
+      <c r="K3" s="20">
+        <v>7.1413843960000003</v>
+      </c>
+      <c r="L3" s="20">
+        <v>8.3480151618700003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="3">
+        <f>A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>29.4</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>109.5</v>
+      </c>
+      <c r="E4" s="3">
+        <v>9</v>
+      </c>
+      <c r="F4" s="3">
+        <v>38</v>
+      </c>
+      <c r="G4" s="3">
+        <v>33.5</v>
+      </c>
+      <c r="H4" s="23">
+        <v>32.904882553500002</v>
+      </c>
+      <c r="I4" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="J4" s="23">
+        <v>3.50355105552</v>
+      </c>
+      <c r="K4" s="21">
+        <v>8.8980085080000002</v>
+      </c>
+      <c r="L4" s="21">
+        <v>9.0046645190600003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="1">
+        <f t="shared" ref="A5:A38" si="0">A4+1</f>
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>113.5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1">
+        <v>38</v>
+      </c>
+      <c r="G5" s="1">
+        <v>31.3</v>
+      </c>
+      <c r="H5" s="22">
+        <v>31.4733065936</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J5" s="22">
+        <v>2.0721776162099999</v>
+      </c>
+      <c r="K5" s="20">
+        <v>9.4732699789999995</v>
+      </c>
+      <c r="L5" s="20">
+        <v>9.4461843300799995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="4">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="4">
+        <v>29.4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>124</v>
+      </c>
+      <c r="E6" s="4">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4">
+        <v>38</v>
+      </c>
+      <c r="G6" s="4">
+        <v>41.5</v>
+      </c>
+      <c r="H6" s="23">
+        <v>38.183843151200001</v>
+      </c>
+      <c r="I6" s="3">
+        <v>12.2</v>
+      </c>
+      <c r="J6" s="23">
+        <v>8.7822393613000003</v>
+      </c>
+      <c r="K6" s="21">
+        <v>8.2142050090000005</v>
+      </c>
+      <c r="L6" s="21">
+        <v>8.9216813518000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>118</v>
+      </c>
+      <c r="E7" s="1">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1">
+        <v>38</v>
+      </c>
+      <c r="G7" s="1">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="H7" s="22">
+        <v>32.889245552399998</v>
+      </c>
+      <c r="I7" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="J7" s="22">
+        <v>3.4877818652000001</v>
+      </c>
+      <c r="K7" s="20">
+        <v>9.5267881840000008</v>
+      </c>
+      <c r="L7" s="20">
+        <v>9.4468013662200008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="4">
+        <v>29.4</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4">
+        <v>117.1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>10</v>
+      </c>
+      <c r="F8" s="4">
+        <v>38</v>
+      </c>
+      <c r="G8" s="4">
+        <v>31.1</v>
+      </c>
+      <c r="H8" s="23">
+        <v>31.448114325999999</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="J8" s="23">
+        <v>2.04684293113</v>
+      </c>
+      <c r="K8" s="21">
+        <v>9.6370043079999999</v>
+      </c>
+      <c r="L8" s="21">
+        <v>9.5920280747500009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1">
+        <v>128.80000000000001</v>
+      </c>
+      <c r="E9" s="1">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1">
+        <v>38</v>
+      </c>
+      <c r="G9" s="1">
+        <v>40.4</v>
+      </c>
+      <c r="H9" s="22">
+        <v>38.298985446800003</v>
+      </c>
+      <c r="I9" s="1">
+        <v>11.2</v>
+      </c>
+      <c r="J9" s="22">
+        <v>8.89722508985</v>
+      </c>
+      <c r="K9" s="20">
+        <v>8.9167739380000004</v>
+      </c>
+      <c r="L9" s="20">
+        <v>9.2330228139399999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>29.4</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>123.5</v>
+      </c>
+      <c r="E10" s="4">
+        <v>11</v>
+      </c>
+      <c r="F10" s="4">
+        <v>38</v>
+      </c>
+      <c r="G10" s="4">
+        <v>31.7</v>
+      </c>
+      <c r="H10" s="23">
+        <v>32.618685882900003</v>
+      </c>
+      <c r="I10" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="J10" s="23">
+        <v>3.2171215737200001</v>
+      </c>
+      <c r="K10" s="21">
+        <v>9.8017882400000005</v>
+      </c>
+      <c r="L10" s="21">
+        <v>9.6931736170900002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1">
+        <f>A10+1</f>
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
+        <v>123.1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1">
+        <v>30.9</v>
+      </c>
+      <c r="H11" s="22">
+        <v>31.197889342300002</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J11" s="22">
+        <v>1.79666832575</v>
+      </c>
+      <c r="K11" s="20">
+        <v>9.8729621600000002</v>
+      </c>
+      <c r="L11" s="20">
+        <v>9.8386747769599996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="4">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>121.3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>9</v>
+      </c>
+      <c r="F12" s="4">
+        <v>38</v>
+      </c>
+      <c r="G12" s="4">
+        <v>43.1</v>
+      </c>
+      <c r="H12" s="23">
+        <v>40.9285437407</v>
+      </c>
+      <c r="I12" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="J12" s="23">
+        <v>5.9273643826600004</v>
+      </c>
+      <c r="K12" s="21">
+        <v>6.2168311879999996</v>
+      </c>
+      <c r="L12" s="21">
+        <v>7.0496039637000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>35</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>119.4</v>
+      </c>
+      <c r="E13" s="1">
+        <v>9</v>
+      </c>
+      <c r="F13" s="1">
+        <v>38</v>
+      </c>
+      <c r="G13" s="1">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="H13" s="22">
+        <v>37.765944230499997</v>
+      </c>
+      <c r="I13" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="J13" s="22">
+        <v>2.7646593460500002</v>
+      </c>
+      <c r="K13" s="20">
+        <v>7.4978749960000002</v>
+      </c>
+      <c r="L13" s="20">
+        <v>8.3564408941699995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="4">
+        <v>35</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
+      </c>
+      <c r="D14" s="4">
+        <v>118.8</v>
+      </c>
+      <c r="E14" s="4">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4">
+        <v>38</v>
+      </c>
+      <c r="G14" s="4">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="H14" s="23">
+        <v>36.667063314099998</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="J14" s="23">
+        <v>1.66595265329</v>
+      </c>
+      <c r="K14" s="21">
+        <v>8.171220924</v>
+      </c>
+      <c r="L14" s="21">
+        <v>8.6641307019799996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>35</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>127.7</v>
+      </c>
+      <c r="E15" s="1">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1">
+        <v>38</v>
+      </c>
+      <c r="G15" s="1">
+        <v>45.5</v>
+      </c>
+      <c r="H15" s="22">
+        <v>42.487170725600002</v>
+      </c>
+      <c r="I15" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="J15" s="22">
+        <v>7.4857122889500003</v>
+      </c>
+      <c r="K15" s="20">
+        <v>7.25616532</v>
+      </c>
+      <c r="L15" s="20">
+        <v>8.1476187211800006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="4">
+        <v>35</v>
+      </c>
+      <c r="C16" s="4">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4">
+        <v>122.6</v>
+      </c>
+      <c r="E16" s="4">
+        <v>10</v>
+      </c>
+      <c r="F16" s="4">
+        <v>38</v>
+      </c>
+      <c r="G16" s="4">
+        <v>38.700000000000003</v>
+      </c>
+      <c r="H16" s="23">
+        <v>38.031601374300003</v>
+      </c>
+      <c r="I16" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="J16" s="23">
+        <v>3.0302681926599999</v>
+      </c>
+      <c r="K16" s="21">
+        <v>8.7522152630000001</v>
+      </c>
+      <c r="L16" s="21">
+        <v>8.8779532591700008</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1">
+        <v>3</v>
+      </c>
+      <c r="D17" s="1">
+        <v>122.2</v>
+      </c>
+      <c r="E17" s="1">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1">
+        <v>38</v>
+      </c>
+      <c r="G17" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H17" s="22">
+        <v>36.780133411900003</v>
+      </c>
+      <c r="I17" s="1">
+        <v>2</v>
+      </c>
+      <c r="J17" s="22">
+        <v>1.7790437461799999</v>
+      </c>
+      <c r="K17" s="20">
+        <v>9.0054255229999995</v>
+      </c>
+      <c r="L17" s="20">
+        <v>9.0770235013599994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>35</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="4">
+        <v>133.30000000000001</v>
+      </c>
+      <c r="E18" s="4">
+        <v>11</v>
+      </c>
+      <c r="F18" s="4">
+        <v>38</v>
+      </c>
+      <c r="G18" s="4">
+        <v>46</v>
+      </c>
+      <c r="H18" s="23">
+        <v>43.057176394599999</v>
+      </c>
+      <c r="I18" s="3">
+        <v>10.8</v>
+      </c>
+      <c r="J18" s="23">
+        <v>8.0555464684399993</v>
+      </c>
+      <c r="K18" s="21">
+        <v>8.1321077689999992</v>
+      </c>
+      <c r="L18" s="21">
+        <v>8.7033832451999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>35</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>128.9</v>
+      </c>
+      <c r="E19" s="1">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1">
+        <v>38</v>
+      </c>
+      <c r="G19" s="1">
+        <v>38</v>
+      </c>
+      <c r="H19" s="22">
+        <v>38.046641301599998</v>
+      </c>
+      <c r="I19" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="J19" s="22">
+        <v>3.0452302362500001</v>
+      </c>
+      <c r="K19" s="20">
+        <v>9.2810226670000002</v>
+      </c>
+      <c r="L19" s="20">
+        <v>9.2743858831299999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>35</v>
+      </c>
+      <c r="C20" s="4">
+        <v>3</v>
+      </c>
+      <c r="D20" s="4">
+        <v>128.4</v>
+      </c>
+      <c r="E20" s="4">
+        <v>11</v>
+      </c>
+      <c r="F20" s="4">
+        <v>38</v>
+      </c>
+      <c r="G20" s="4">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="H20" s="23">
+        <v>36.748522556099999</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="J20" s="23">
+        <v>1.74737487179</v>
+      </c>
+      <c r="K20" s="21">
+        <v>9.4350865689999992</v>
+      </c>
+      <c r="L20" s="21">
+        <v>9.4285119794799996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>94.8</v>
+      </c>
+      <c r="E21" s="1">
+        <v>9</v>
+      </c>
+      <c r="F21" s="1">
+        <v>76</v>
+      </c>
+      <c r="G21" s="1">
+        <v>41.1</v>
+      </c>
+      <c r="H21" s="22">
+        <v>43.658894520600001</v>
+      </c>
+      <c r="I21" s="1">
+        <v>11.7</v>
+      </c>
+      <c r="J21" s="22">
+        <v>14.2572725804</v>
+      </c>
+      <c r="K21" s="20">
+        <v>11.177502260000001</v>
+      </c>
+      <c r="L21" s="20">
+        <v>9.3406659813200008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <v>29.4</v>
+      </c>
+      <c r="C22" s="4">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4">
+        <v>90.8</v>
+      </c>
+      <c r="E22" s="4">
+        <v>9</v>
+      </c>
+      <c r="F22" s="4">
+        <v>76</v>
+      </c>
+      <c r="G22" s="4">
+        <v>38.4</v>
+      </c>
+      <c r="H22" s="23">
+        <v>38.7385219214</v>
+      </c>
+      <c r="I22" s="3">
+        <v>8.9</v>
+      </c>
+      <c r="J22" s="23">
+        <v>9.3366670980100004</v>
+      </c>
+      <c r="K22" s="21">
+        <v>13.219360229999999</v>
+      </c>
+      <c r="L22" s="21">
+        <v>12.9437558676</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="1">
+        <v>86.9</v>
+      </c>
+      <c r="E23" s="1">
+        <v>9</v>
+      </c>
+      <c r="F23" s="1">
+        <v>76</v>
+      </c>
+      <c r="G23" s="1">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H23" s="22">
+        <v>36.037707650800002</v>
+      </c>
+      <c r="I23" s="1">
+        <v>7.6</v>
+      </c>
+      <c r="J23" s="22">
+        <v>6.6353539153899996</v>
+      </c>
+      <c r="K23" s="20">
+        <v>13.59416671</v>
+      </c>
+      <c r="L23" s="20">
+        <v>14.2350662448</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="4">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="4">
+        <v>29.4</v>
+      </c>
+      <c r="C24" s="4">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4">
+        <v>103.3</v>
+      </c>
+      <c r="E24" s="4">
+        <v>10</v>
+      </c>
+      <c r="F24" s="4">
+        <v>76</v>
+      </c>
+      <c r="G24" s="4">
+        <v>45.8</v>
+      </c>
+      <c r="H24" s="23">
+        <v>46.979798993700001</v>
+      </c>
+      <c r="I24" s="3">
+        <v>16.3</v>
+      </c>
+      <c r="J24" s="23">
+        <v>17.5781896913</v>
+      </c>
+      <c r="K24" s="21">
+        <v>11.735591189999999</v>
+      </c>
+      <c r="L24" s="21">
+        <v>11.0366847651</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>94.8</v>
+      </c>
+      <c r="E25" s="1">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <v>76</v>
+      </c>
+      <c r="G25" s="1">
+        <v>39.1</v>
+      </c>
+      <c r="H25" s="22">
+        <v>39.6997978598</v>
+      </c>
+      <c r="I25" s="1">
+        <v>10</v>
+      </c>
+      <c r="J25" s="22">
+        <v>10.297383476</v>
+      </c>
+      <c r="K25" s="20">
+        <v>14.282737859999999</v>
+      </c>
+      <c r="L25" s="20">
+        <v>14.0376455414</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="4">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="4">
+        <v>29.4</v>
+      </c>
+      <c r="C26" s="4">
+        <v>3</v>
+      </c>
+      <c r="D26" s="4">
+        <v>90.7</v>
+      </c>
+      <c r="E26" s="4">
+        <v>10</v>
+      </c>
+      <c r="F26" s="4">
+        <v>76</v>
+      </c>
+      <c r="G26" s="4">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="H26" s="23">
+        <v>36.184008874900002</v>
+      </c>
+      <c r="I26" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="J26" s="23">
+        <v>6.7813029292999998</v>
+      </c>
+      <c r="K26" s="21">
+        <v>15.104304369999999</v>
+      </c>
+      <c r="L26" s="21">
+        <v>14.8250921988</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>110.6</v>
+      </c>
+      <c r="E27" s="1">
+        <v>11</v>
+      </c>
+      <c r="F27" s="1">
+        <v>76</v>
+      </c>
+      <c r="G27" s="1">
+        <v>49.3</v>
+      </c>
+      <c r="H27" s="22">
+        <v>49.323975191000002</v>
+      </c>
+      <c r="I27" s="1">
+        <v>19.8</v>
+      </c>
+      <c r="J27" s="22">
+        <v>19.922119521900001</v>
+      </c>
+      <c r="K27" s="20">
+        <v>12.34060298</v>
+      </c>
+      <c r="L27" s="20">
+        <v>12.329546318</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="4">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="4">
+        <v>29.4</v>
+      </c>
+      <c r="C28" s="4">
+        <v>2</v>
+      </c>
+      <c r="D28" s="4">
+        <v>100.7</v>
+      </c>
+      <c r="E28" s="4">
+        <v>11</v>
+      </c>
+      <c r="F28" s="4">
+        <v>76</v>
+      </c>
+      <c r="G28" s="4">
+        <v>38.4</v>
+      </c>
+      <c r="H28" s="23">
+        <v>39.876106315400001</v>
+      </c>
+      <c r="I28" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J28" s="23">
+        <v>10.4732345003</v>
+      </c>
+      <c r="K28" s="21">
+        <v>15.272513630000001</v>
+      </c>
+      <c r="L28" s="21">
+        <v>14.832398797</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="1">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="1">
+        <v>29.4</v>
+      </c>
+      <c r="C29" s="1">
+        <v>3</v>
+      </c>
+      <c r="D29" s="1">
+        <v>97.1</v>
+      </c>
+      <c r="E29" s="1">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1">
+        <v>76</v>
+      </c>
+      <c r="G29" s="1">
+        <v>33.9</v>
+      </c>
+      <c r="H29" s="22">
+        <v>35.892675915399998</v>
+      </c>
+      <c r="I29" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="J29" s="22">
+        <v>6.4896415734200001</v>
+      </c>
+      <c r="K29" s="20">
+        <v>16.021434150000001</v>
+      </c>
+      <c r="L29" s="20">
+        <v>15.512902462</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="4">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="4">
+        <v>35</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1</v>
+      </c>
+      <c r="D30" s="4">
+        <v>92.5</v>
+      </c>
+      <c r="E30" s="4">
+        <v>9</v>
+      </c>
+      <c r="F30" s="4">
+        <v>76</v>
+      </c>
+      <c r="G30" s="4">
+        <v>43.8</v>
+      </c>
+      <c r="H30" s="23">
+        <v>46.516168034400003</v>
+      </c>
+      <c r="I30" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J30" s="23">
+        <v>11.5143277949</v>
+      </c>
+      <c r="K30" s="21">
+        <v>9.0038824539999993</v>
+      </c>
+      <c r="L30" s="21">
+        <v>7.7752160422700003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="1">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="1">
+        <v>35</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>90</v>
+      </c>
+      <c r="E31" s="1">
+        <v>9</v>
+      </c>
+      <c r="F31" s="1">
+        <v>76</v>
+      </c>
+      <c r="G31" s="1">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="H31" s="22">
+        <v>41.596327217000002</v>
+      </c>
+      <c r="I31" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="J31" s="22">
+        <v>6.5945521714200002</v>
+      </c>
+      <c r="K31" s="20">
+        <v>11.48457443</v>
+      </c>
+      <c r="L31" s="20">
+        <v>10.2018576794</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="4">
+        <v>35</v>
+      </c>
+      <c r="C32" s="4">
+        <v>3</v>
+      </c>
+      <c r="D32" s="4">
+        <v>88.4</v>
+      </c>
+      <c r="E32" s="4">
+        <v>9</v>
+      </c>
+      <c r="F32" s="4">
+        <v>76</v>
+      </c>
+      <c r="G32" s="4">
+        <v>39.4</v>
+      </c>
+      <c r="H32" s="23">
+        <v>39.844373985700003</v>
+      </c>
+      <c r="I32" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="J32" s="23">
+        <v>4.84253232966</v>
+      </c>
+      <c r="K32" s="21">
+        <v>12.07212595</v>
+      </c>
+      <c r="L32" s="21">
+        <v>11.6451410943</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="1">
+        <v>35</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>104.1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1">
+        <v>76</v>
+      </c>
+      <c r="G33" s="1">
+        <v>48</v>
+      </c>
+      <c r="H33" s="22">
+        <v>49.816837546800002</v>
+      </c>
+      <c r="I33" s="1">
+        <v>12.8</v>
+      </c>
+      <c r="J33" s="22">
+        <v>14.814999884200001</v>
+      </c>
+      <c r="K33" s="20">
+        <v>10.56273097</v>
+      </c>
+      <c r="L33" s="20">
+        <v>9.6744266823499991</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="4">
+        <v>35</v>
+      </c>
+      <c r="C34" s="4">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4">
+        <v>98.4</v>
+      </c>
+      <c r="E34" s="4">
+        <v>10</v>
+      </c>
+      <c r="F34" s="4">
+        <v>76</v>
+      </c>
+      <c r="G34" s="4">
+        <v>43.4</v>
+      </c>
+      <c r="H34" s="23">
+        <v>43.589375310000001</v>
+      </c>
+      <c r="I34" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J34" s="23">
+        <v>8.5872050156699995</v>
+      </c>
+      <c r="K34" s="21">
+        <v>12.62581915</v>
+      </c>
+      <c r="L34" s="21">
+        <v>12.5151756476</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="1">
+        <v>35</v>
+      </c>
+      <c r="C35" s="1">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1">
+        <v>93.9</v>
+      </c>
+      <c r="E35" s="1">
+        <v>10</v>
+      </c>
+      <c r="F35" s="1">
+        <v>76</v>
+      </c>
+      <c r="G35" s="1">
+        <v>41.1</v>
+      </c>
+      <c r="H35" s="22">
+        <v>40.829516938200001</v>
+      </c>
+      <c r="I35" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="J35" s="22">
+        <v>5.8271606420099999</v>
+      </c>
+      <c r="K35" s="20">
+        <v>13.304688799999999</v>
+      </c>
+      <c r="L35" s="20">
+        <v>13.431470279299999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="4">
+        <v>35</v>
+      </c>
+      <c r="C36" s="4">
+        <v>1</v>
+      </c>
+      <c r="D36" s="4">
+        <v>109.6</v>
+      </c>
+      <c r="E36" s="4">
+        <v>11</v>
+      </c>
+      <c r="F36" s="4">
+        <v>76</v>
+      </c>
+      <c r="G36" s="4">
+        <v>51.5</v>
+      </c>
+      <c r="H36" s="23">
+        <v>52.285627960399999</v>
+      </c>
+      <c r="I36" s="3">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J36" s="23">
+        <v>17.283810483100002</v>
+      </c>
+      <c r="K36" s="21">
+        <v>11.21689995</v>
+      </c>
+      <c r="L36" s="21">
+        <v>10.8671689562</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="1">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="1">
+        <v>35</v>
+      </c>
+      <c r="C37" s="1">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>101.9</v>
+      </c>
+      <c r="E37" s="1">
+        <v>11</v>
+      </c>
+      <c r="F37" s="1">
+        <v>76</v>
+      </c>
+      <c r="G37" s="1">
+        <v>43.6</v>
+      </c>
+      <c r="H37" s="22">
+        <v>44.352922091700002</v>
+      </c>
+      <c r="I37" s="1">
+        <v>8.6</v>
+      </c>
+      <c r="J37" s="22">
+        <v>9.3504251887700001</v>
+      </c>
+      <c r="K37" s="20">
+        <v>13.723713310000001</v>
+      </c>
+      <c r="L37" s="20">
+        <v>13.4397995098</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="4">
+        <v>35</v>
+      </c>
+      <c r="C38" s="4">
+        <v>3</v>
+      </c>
+      <c r="D38" s="4">
+        <v>98.4</v>
+      </c>
+      <c r="E38" s="4">
+        <v>11</v>
+      </c>
+      <c r="F38" s="4">
+        <v>76</v>
+      </c>
+      <c r="G38" s="4">
+        <v>40.5</v>
+      </c>
+      <c r="H38" s="23">
+        <v>40.9925610855</v>
+      </c>
+      <c r="I38" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="J38" s="23">
+        <v>5.9899077289599996</v>
+      </c>
+      <c r="K38" s="21">
+        <v>14.35144721</v>
+      </c>
+      <c r="L38" s="21">
+        <v>14.1935320248</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="K39" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH76"/>
   <sheetViews>

</xml_diff>